<commit_message>
added calculator for upstream LCI CO2 emissions to factory
</commit_message>
<xml_diff>
--- a/data/shared/upstream.xlsx
+++ b/data/shared/upstream.xlsx
@@ -1,35 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\setanzer\GitHub\BlackBlox\data\shared\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/shared/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53ED757F-1AF3-454E-A90F-5DBF221517A3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18645" windowHeight="11175"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25440" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="upstream" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="B6" authorId="0" shapeId="0">
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -63,7 +70,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0" shapeId="0">
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -97,7 +104,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="0" shapeId="0">
+    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -130,7 +137,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B21" authorId="0" shapeId="0">
+    <comment ref="B21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -239,15 +246,9 @@
     <t>substance</t>
   </si>
   <si>
-    <t>upstream CO2</t>
-  </si>
-  <si>
     <t>biomass-to-fuel ratio</t>
   </si>
   <si>
-    <t>CO2 removal</t>
-  </si>
-  <si>
     <t>is fossil</t>
   </si>
   <si>
@@ -272,23 +273,28 @@
     <t>CaCO3</t>
   </si>
   <si>
-    <t>upstream
-CH4</t>
-  </si>
-  <si>
     <t>t CO2eq/t fuel</t>
   </si>
   <si>
-    <t>iron ore - 65% Fe</t>
-  </si>
-  <si>
     <t>charcoal - 2050</t>
+  </si>
+  <si>
+    <t>CO2</t>
+  </si>
+  <si>
+    <t>CH4</t>
+  </si>
+  <si>
+    <t>CO2 removed</t>
+  </si>
+  <si>
+    <t>iron ore</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -639,50 +645,50 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="7" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="7" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -695,26 +701,26 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -739,12 +745,12 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B5">
         <f>0.5</f>
@@ -762,7 +768,7 @@
       <c r="F5" s="4"/>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -786,10 +792,10 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -813,10 +819,10 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -840,10 +846,10 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -855,10 +861,10 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -870,10 +876,10 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -885,10 +891,10 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -900,10 +906,10 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -915,10 +921,10 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -930,10 +936,10 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -945,10 +951,10 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -960,10 +966,10 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -975,10 +981,10 @@
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -990,10 +996,10 @@
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -1007,7 +1013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -1025,7 +1031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -1046,17 +1052,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B22">
         <v>2E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B23">
         <v>1.6500000000000001E-2</v>

</xml_diff>

<commit_message>
added ecoinvent 3.5 data to  upstream.xlsx
</commit_message>
<xml_diff>
--- a/data/shared/upstream.xlsx
+++ b/data/shared/upstream.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/shared/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53ED757F-1AF3-454E-A90F-5DBF221517A3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C53941-B825-0C44-B0C7-3E342AC2AD44}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25440" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16140" yWindow="2120" windowWidth="25440" windowHeight="14540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="upstream" sheetId="1" r:id="rId1"/>
+    <sheet name="upstream inflows" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,107 +37,6 @@
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">ecoinvent 2.2
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">ecoinvent 2.2
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>ecoinvent 2.2</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="B21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
@@ -166,7 +66,31 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">from </t>
+          <t>from https://www.forestresearch.gov.uk/tools-and-resources/biomass-energy-resources/reference-biomass/facts-figures/carbon-emissions-of-different-fuels/</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Microsoft Office User</author>
+  </authors>
+  <commentList>
+    <comment ref="B21" authorId="0" shapeId="0" xr:uid="{723C515B-93A0-D346-B5CE-BF01BA40B0E4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
         </r>
         <r>
           <rPr>
@@ -175,7 +99,17 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>https://www.forestresearch.gov.uk/tools-and-resources/biomass-energy-resources/reference-biomass/facts-figures/carbon-emissions-of-different-fuels/</t>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>from https://www.forestresearch.gov.uk/tools-and-resources/biomass-energy-resources/reference-biomass/facts-figures/carbon-emissions-of-different-fuels/</t>
         </r>
       </text>
     </comment>
@@ -184,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="38">
   <si>
     <t>meta-notes</t>
   </si>
@@ -279,16 +213,25 @@
     <t>charcoal - 2050</t>
   </si>
   <si>
-    <t>CO2</t>
-  </si>
-  <si>
-    <t>CH4</t>
-  </si>
-  <si>
     <t>CO2 removed</t>
   </si>
   <si>
     <t>iron ore</t>
+  </si>
+  <si>
+    <t>CO2, biogenic</t>
+  </si>
+  <si>
+    <t>CO2 fossil</t>
+  </si>
+  <si>
+    <t>CH4, fossil</t>
+  </si>
+  <si>
+    <t>CH4, biogenic</t>
+  </si>
+  <si>
+    <t>CO2 from atmosphere</t>
   </si>
 </sst>
 </file>
@@ -646,49 +589,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="4" width="12.6640625" customWidth="1"/>
-    <col min="5" max="7" width="15.5" customWidth="1"/>
+    <col min="2" max="6" width="12.6640625" customWidth="1"/>
+    <col min="7" max="9" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -700,55 +649,66 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>2.95</v>
+        <f>0.292</f>
+        <v>0.29199999999999998</v>
       </c>
       <c r="C4">
-        <v>1.01</v>
-      </c>
-      <c r="D4" s="6">
-        <f>6.2/E4</f>
-        <v>5.166666666666667</v>
-      </c>
-      <c r="E4" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="F4" s="4">
-        <v>0</v>
-      </c>
-      <c r="G4" s="5">
-        <f>1-F4</f>
-        <v>1</v>
-      </c>
-      <c r="I4" t="s">
+        <v>2.7</v>
+      </c>
+      <c r="D4">
+        <v>3.3699999999999999E-6</v>
+      </c>
+      <c r="E4">
+        <v>1120</v>
+      </c>
+      <c r="F4" s="6">
+        <f>6.2/G4</f>
+        <v>1.3656387665198237</v>
+      </c>
+      <c r="G4" s="3">
+        <v>4.54</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0</v>
+      </c>
+      <c r="I4" s="5">
+        <f>1-H4</f>
+        <v>1</v>
+      </c>
+      <c r="K4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -756,316 +716,510 @@
         <f>0.5</f>
         <v>0.5</v>
       </c>
-      <c r="C5">
-        <v>0.2</v>
-      </c>
-      <c r="D5" s="6">
+      <c r="F5" s="6">
         <v>4</v>
       </c>
-      <c r="E5" s="3">
+      <c r="G5" s="3">
         <v>1.2</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H5" s="4"/>
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6">
-        <v>6.4000000000000001E-2</v>
+        <f>0.238</f>
+        <v>0.23799999999999999</v>
       </c>
       <c r="C6">
-        <v>0.191</v>
+        <v>3.3800000000000002E-3</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>6.3999999999999997E-6</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>6.2600000000000003E-2</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <f t="shared" ref="G6:G7" si="0">1-F6</f>
-        <v>0</v>
-      </c>
-      <c r="I6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <f t="shared" ref="I6:I7" si="0">1-H6</f>
+        <v>0</v>
+      </c>
+      <c r="K6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7">
-        <v>6.4000000000000001E-2</v>
+        <f>0.238</f>
+        <v>0.23799999999999999</v>
       </c>
       <c r="C7">
-        <v>0.191</v>
+        <v>3.3800000000000002E-3</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>6.3999999999999997E-6</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>6.2600000000000003E-2</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I7" t="s">
+      <c r="K7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8">
         <v>0.35599999999999998</v>
       </c>
-      <c r="C8">
-        <v>0.188</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
       <c r="F8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <f>1-F8</f>
-        <v>0</v>
-      </c>
-      <c r="I8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <f>1-H8</f>
+        <v>0</v>
+      </c>
+      <c r="K8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9">
-        <f t="shared" ref="G9:G18" si="1">1-F9</f>
-        <v>0</v>
-      </c>
-      <c r="I9" t="s">
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <f t="shared" ref="I9:I18" si="1">1-H9</f>
+        <v>0</v>
+      </c>
+      <c r="K9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10">
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I10" t="s">
+      <c r="K10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11">
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I11" t="s">
+      <c r="K11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12">
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I12" t="s">
+      <c r="K12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>10</v>
       </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13">
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I13" t="s">
+      <c r="K13" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>11</v>
       </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14">
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I14" t="s">
+      <c r="K14" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>12</v>
       </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15">
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I15" t="s">
+      <c r="K15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>13</v>
       </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16">
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I16" t="s">
+      <c r="K16" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>14</v>
       </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17">
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I17" t="s">
+      <c r="K17" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>15</v>
       </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="G18">
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I18" t="s">
+      <c r="K18" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>16</v>
       </c>
       <c r="B19">
         <v>0</v>
       </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="6">
+      <c r="F20" s="6">
         <v>1.8</v>
       </c>
-      <c r="E20" s="7">
+      <c r="G20" s="7">
         <v>1.2</v>
       </c>
-      <c r="F20" s="4">
-        <v>0</v>
-      </c>
-      <c r="G20" s="5">
-        <f t="shared" ref="G20:G21" si="2">1-F20</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="H20" s="4">
+        <v>0</v>
+      </c>
+      <c r="I20" s="5">
+        <f t="shared" ref="I20:I21" si="2">1-H20</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>18</v>
       </c>
       <c r="B21">
         <v>0.36520000000000002</v>
       </c>
-      <c r="D21" s="6">
+      <c r="F21" s="6">
         <v>1.5</v>
       </c>
-      <c r="E21" s="7">
+      <c r="G21" s="7">
         <v>1.2</v>
       </c>
-      <c r="F21" s="4">
-        <v>0</v>
-      </c>
-      <c r="G21" s="5">
+      <c r="H21" s="4">
+        <v>0</v>
+      </c>
+      <c r="I21" s="5">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>28</v>
       </c>
       <c r="B22">
-        <v>2E-3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+        <v>4.7499999999999999E-3</v>
+      </c>
+      <c r="C22">
+        <v>8.6399999999999999E-5</v>
+      </c>
+      <c r="D22">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="E22">
+        <v>2.5999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B23">
-        <v>1.6500000000000001E-2</v>
+        <f>(0.116+0.00782)/2</f>
+        <v>6.1910000000000007E-2</v>
+      </c>
+      <c r="C23">
+        <f>(0.000685+0.000984)/2</f>
+        <v>8.3449999999999996E-4</v>
+      </c>
+      <c r="D23">
+        <f>(0.000000244+0.00000131)/2</f>
+        <v>7.7699999999999993E-7</v>
+      </c>
+      <c r="E23">
+        <f>(0.00585+0.059)/2</f>
+        <v>3.2424999999999995E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{431692A7-AA4F-6C4F-BC6A-7C3261165D7B}">
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>4.54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5">
+        <v>4.54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>2.06E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>2.06E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22">
+        <v>8.8700000000000001E-5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23">
+        <f>(0.0114+0.123)/2</f>
+        <v>6.7199999999999996E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added more upstream data from ecoinvent
only change to var file was a comment in co2 capture
</commit_message>
<xml_diff>
--- a/data/shared/upstream.xlsx
+++ b/data/shared/upstream.xlsx
@@ -1,23 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/shared/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\setanzer\GitHub\BlackBlox\data\shared\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A359E6E7-B923-9B46-B880-08D1599F3066}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1460" yWindow="460" windowWidth="22680" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1455" yWindow="465" windowWidth="22680" windowHeight="17535"/>
   </bookViews>
   <sheets>
     <sheet name="emissions" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
-    <sheet name="removals" sheetId="2" r:id="rId3"/>
+    <sheet name="removals" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,12 +31,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="C9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="C9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -76,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="61">
   <si>
     <t>meta-notes</t>
   </si>
@@ -150,28 +148,124 @@
     <t>ecoinvent 3.5</t>
   </si>
   <si>
-    <t>wood (wet)</t>
-  </si>
-  <si>
     <t>solvent (MEA)</t>
   </si>
   <si>
-    <t>ecoinvent 3.2</t>
-  </si>
-  <si>
     <t>WEO</t>
   </si>
   <si>
-    <t>–</t>
-  </si>
-  <si>
     <t>wood (20% moisture)</t>
+  </si>
+  <si>
+    <t>CO2 land transformation</t>
+  </si>
+  <si>
+    <t>biomethane</t>
+  </si>
+  <si>
+    <t>ecoinvent 3.4</t>
+  </si>
+  <si>
+    <t>meta-source notes</t>
+  </si>
+  <si>
+    <t>charcola (GLO)</t>
+  </si>
+  <si>
+    <t>hard coal (RoW)</t>
+  </si>
+  <si>
+    <t>hard coal (West Europe)</t>
+  </si>
+  <si>
+    <t>average of 45% and 65% FE</t>
+  </si>
+  <si>
+    <t>Limestone (CH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ecoinvent 3.4 </t>
+  </si>
+  <si>
+    <t>CaCO3 - ROW</t>
+  </si>
+  <si>
+    <t>Limestone (ROW)</t>
+  </si>
+  <si>
+    <t>natural gas - mix EU</t>
+  </si>
+  <si>
+    <t>Natural Gas</t>
+  </si>
+  <si>
+    <t>Oxygen -EU27 Mix</t>
+  </si>
+  <si>
+    <t>pipeline transport (1 tkm)</t>
+  </si>
+  <si>
+    <t>solvent (generic)</t>
+  </si>
+  <si>
+    <t>Solvent (GLO)</t>
+  </si>
+  <si>
+    <t>solvent (DEA)</t>
+  </si>
+  <si>
+    <t>solvent (TEA)</t>
+  </si>
+  <si>
+    <t>wood (44% moisture)</t>
+  </si>
+  <si>
+    <t>Steel, HRC (GLO)</t>
+  </si>
+  <si>
+    <t>Steel, HRC (EU)</t>
+  </si>
+  <si>
+    <t>Steel, HRC (Asia)</t>
+  </si>
+  <si>
+    <t>Steel, HRC (BF route)</t>
+  </si>
+  <si>
+    <t>Steel, unalloyed</t>
+  </si>
+  <si>
+    <t>wood syngas, fixed bed</t>
+  </si>
+  <si>
+    <t>wood syngas, fluidized bed</t>
+  </si>
+  <si>
+    <t>CH4 land transformation</t>
+  </si>
+  <si>
+    <t>wood chips (EU no swiss, dry)</t>
+  </si>
+  <si>
+    <t>wood chips, RER (dry)</t>
+  </si>
+  <si>
+    <t>RER</t>
+  </si>
+  <si>
+    <t>EU, excluding switzerland</t>
+  </si>
+  <si>
+    <t>CH</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -244,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -256,6 +350,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -535,21 +632,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="15.1640625" customWidth="1"/>
-    <col min="3" max="6" width="12.6640625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="4" width="12.7109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" style="5" customWidth="1"/>
+    <col min="6" max="7" width="12.7109375" style="5" customWidth="1"/>
+    <col min="8" max="8" width="11" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -563,16 +664,25 @@
         <v>19</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="J1" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -581,9 +691,10 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="G2" s="4"/>
+      <c r="I2" s="4"/>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -592,13 +703,14 @@
         <v>13</v>
       </c>
       <c r="D3" s="4"/>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="4"/>
+      <c r="F3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G3" s="4"/>
+      <c r="I3" s="4"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -614,16 +726,25 @@
         <v>2.7</v>
       </c>
       <c r="E4" s="5">
-        <v>3.3700000000000001E-9</v>
+        <v>2.4599999999999999E-3</v>
       </c>
       <c r="F4" s="5">
+        <v>2.5700000000000001E-2</v>
+      </c>
+      <c r="G4" s="5">
         <v>1.1200000000000001</v>
       </c>
-      <c r="G4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" s="5">
+        <v>3.9199999999999997E-5</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -639,16 +760,25 @@
         <v>3.3800000000000002E-3</v>
       </c>
       <c r="E5" s="5">
-        <v>6.4000000000000002E-9</v>
+        <v>2.34E-4</v>
       </c>
       <c r="F5" s="5">
+        <v>0.31</v>
+      </c>
+      <c r="G5" s="5">
         <v>6.2600000000000004E-5</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" s="5">
+        <v>9.3999999999999998E-6</v>
+      </c>
+      <c r="I5" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -663,17 +793,20 @@
       <c r="D6" s="5">
         <v>3.3800000000000002E-3</v>
       </c>
-      <c r="E6" s="5">
-        <v>6.4000000000000002E-9</v>
-      </c>
       <c r="F6" s="5">
+        <v>0.31</v>
+      </c>
+      <c r="G6" s="5">
         <v>6.2600000000000004E-5</v>
       </c>
-      <c r="G6" t="s">
+      <c r="I6" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -684,11 +817,11 @@
       <c r="C7" s="5">
         <v>0.35599999999999998</v>
       </c>
-      <c r="G7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I7" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -696,7 +829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -708,7 +841,7 @@
         <v>0.36520000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -722,388 +855,994 @@
       <c r="D10" s="5">
         <v>8.6399999999999999E-5</v>
       </c>
-      <c r="E10" s="5">
-        <v>5.8999999999999998E-5</v>
-      </c>
       <c r="F10" s="5">
+        <v>1.3899999999999999E-4</v>
+      </c>
+      <c r="G10" s="5">
         <v>2.6000000000000001E-6</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H10" s="7">
+        <v>5.2999999999999998E-8</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="J10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="B11">
         <f>SUM(C11:D11)</f>
+        <v>5.3365000000000001E-3</v>
+      </c>
+      <c r="C11" s="5">
+        <v>5.2500000000000003E-3</v>
+      </c>
+      <c r="D11" s="5">
+        <v>8.6500000000000002E-5</v>
+      </c>
+      <c r="E11" s="5">
+        <v>3.3299999999999999E-6</v>
+      </c>
+      <c r="F11" s="5">
+        <v>1.94E-4</v>
+      </c>
+      <c r="G11" s="5">
+        <v>2.6800000000000001E-5</v>
+      </c>
+      <c r="H11" s="7">
+        <v>5.4E-8</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="J11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <f>SUM(C12:D12)</f>
         <v>6.2744500000000009E-2</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C12" s="5">
         <f>(0.116+0.00782)/2</f>
         <v>6.1910000000000007E-2</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D12" s="5">
         <f>(0.000685+0.000984)/2</f>
         <v>8.3449999999999996E-4</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E12" s="5">
+        <f>(0.0000114+0.000123)/2</f>
+        <v>6.7200000000000007E-5</v>
+      </c>
+      <c r="F12" s="5">
         <f>(0.000000000244+0.00000000131)/2</f>
         <v>7.7700000000000001E-10</v>
       </c>
-      <c r="F11" s="5">
+      <c r="G12" s="5">
         <f>(0.00000585+0.000059)/2</f>
         <v>3.2425000000000002E-5</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="H12" s="5">
+        <v>5.0000000000000003E-10</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>8</v>
       </c>
-      <c r="B12">
+      <c r="B13">
+        <f t="shared" ref="B13:B35" si="0">SUM(C13:D13)</f>
         <v>0</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C13" s="5">
         <v>0</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D13" s="5">
         <v>0</v>
       </c>
-      <c r="E12" s="5">
+      <c r="F13" s="5">
         <v>0</v>
       </c>
-      <c r="F12" s="5">
+      <c r="G13" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>7</v>
       </c>
-      <c r="B13">
+      <c r="B14">
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="G13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="I14" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>6</v>
       </c>
-      <c r="B14">
+      <c r="B15">
         <v>0.19400000000000001</v>
       </c>
-      <c r="G14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15">
+      <c r="I15" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16">
         <v>0.6</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16">
-        <f>C16</f>
-        <v>1.8638999999999999</v>
-      </c>
-      <c r="C16" s="5">
-        <f>1.71+0.125+0.0289</f>
-        <v>1.8638999999999999</v>
-      </c>
-      <c r="E16" s="5">
-        <f>0.295+0.0267</f>
-        <v>0.32169999999999999</v>
-      </c>
-      <c r="G16" t="s">
-        <v>26</v>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>0.76119999999999999</v>
+      </c>
+      <c r="C17" s="5">
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="D17" s="5">
+        <v>2.52E-2</v>
+      </c>
+      <c r="E17" s="5">
+        <v>4.1899999999999999E-4</v>
+      </c>
+      <c r="F17" s="5">
+        <v>7.9100000000000004E-2</v>
+      </c>
+      <c r="G17" s="5">
+        <v>4.1599999999999997E-4</v>
+      </c>
+      <c r="H17" s="5">
+        <v>2.5900000000000002E-6</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>3.61</v>
+      </c>
+      <c r="C18" s="5">
+        <v>1.21</v>
+      </c>
+      <c r="D18" s="5">
+        <v>2.4</v>
+      </c>
+      <c r="E18" s="5">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="G18" s="5">
+        <v>1.02</v>
+      </c>
+      <c r="H18" s="5">
+        <v>1.5900000000000001E-3</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>2.648E-2</v>
+      </c>
+      <c r="C19" s="5">
+        <v>2.3099999999999999E-2</v>
+      </c>
+      <c r="D19" s="5">
+        <v>3.3800000000000002E-3</v>
+      </c>
+      <c r="E19" s="5">
+        <v>1.25E-4</v>
+      </c>
+      <c r="F19" s="5">
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="G19" s="5">
+        <v>6.4400000000000002E-6</v>
+      </c>
+      <c r="H19" s="5">
+        <v>1.95E-6</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>0.32052000000000003</v>
+      </c>
+      <c r="C20" s="5">
+        <v>0.313</v>
+      </c>
+      <c r="D20" s="5">
+        <v>7.5199999999999998E-3</v>
+      </c>
+      <c r="J20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="C21" s="5">
+        <v>0.13900000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>7.0666099999999998E-5</v>
+      </c>
+      <c r="C22" s="7">
+        <v>7.0599999999999995E-5</v>
+      </c>
+      <c r="D22" s="5">
+        <v>6.6100000000000003E-8</v>
+      </c>
+      <c r="E22" s="7">
+        <v>1.5300000000000001E-8</v>
+      </c>
+      <c r="F22" s="5">
+        <v>5.4400000000000001E-5</v>
+      </c>
+      <c r="G22" s="5">
+        <f>0.00000011</f>
+        <v>1.1000000000000001E-7</v>
+      </c>
+      <c r="H22" s="7">
+        <v>1.8199999999999999E-10</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>2.6067999999999998</v>
+      </c>
+      <c r="C23" s="5">
+        <v>2.57</v>
+      </c>
+      <c r="D23" s="5">
+        <v>3.6799999999999999E-2</v>
+      </c>
+      <c r="E23" s="5">
+        <v>1.9599999999999999E-3</v>
+      </c>
+      <c r="F23" s="5">
+        <v>0.379</v>
+      </c>
+      <c r="G23" s="5">
+        <v>2.64E-3</v>
+      </c>
+      <c r="H23" s="5">
+        <v>5.1499999999999998E-5</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>2.6046</v>
+      </c>
+      <c r="C24" s="5">
+        <v>2.57</v>
+      </c>
+      <c r="D24" s="5">
+        <v>3.4599999999999999E-2</v>
+      </c>
+      <c r="E24" s="5">
+        <v>1.8400000000000001E-3</v>
+      </c>
+      <c r="F24" s="5">
+        <v>0.35099999999999998</v>
+      </c>
+      <c r="G24" s="5">
+        <v>2.64E-3</v>
+      </c>
+      <c r="H24" s="5">
+        <v>5.0099999999999998E-5</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>1.9873000000000001</v>
+      </c>
+      <c r="C25" s="5">
+        <v>1.97</v>
+      </c>
+      <c r="D25" s="5">
+        <v>1.7299999999999999E-2</v>
+      </c>
+      <c r="E25" s="5">
+        <v>1.0300000000000001E-3</v>
+      </c>
+      <c r="F25" s="5">
+        <v>0.40500000000000003</v>
+      </c>
+      <c r="G25" s="5">
+        <v>9.990000000000001E-4</v>
+      </c>
+      <c r="H25" s="5">
+        <v>3.8E-6</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>6.8199999999999997E-3</v>
+      </c>
+      <c r="C26" s="5">
+        <v>6.8199999999999997E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>2.0971000000000002</v>
+      </c>
+      <c r="C27" s="5">
+        <v>2.08</v>
+      </c>
+      <c r="D27" s="5">
+        <v>1.7100000000000001E-2</v>
+      </c>
+      <c r="G27" s="5">
+        <v>1.2400000000000001E-4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>1.952</v>
+      </c>
+      <c r="C28" s="5">
+        <v>1.94</v>
+      </c>
+      <c r="D28" s="5">
+        <v>1.2E-2</v>
+      </c>
+      <c r="G28" s="5">
+        <v>1.0900000000000001E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>2.1913999999999998</v>
+      </c>
+      <c r="C29" s="5">
+        <v>2.17</v>
+      </c>
+      <c r="D29" s="5">
+        <v>2.1399999999999999E-2</v>
+      </c>
+      <c r="G29" s="5">
+        <v>1.37E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>0.89800000000000002</v>
+      </c>
+      <c r="C30" s="5">
+        <v>0.89800000000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>2.05918</v>
+      </c>
+      <c r="C31" s="5">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="D31" s="5">
+        <v>9.1800000000000007E-3</v>
+      </c>
+      <c r="F31" s="5">
+        <v>0.184</v>
+      </c>
+      <c r="G31" s="5">
+        <v>1.3699999999999999E-5</v>
+      </c>
+      <c r="H31" s="5">
+        <v>2.5000000000000002E-6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>0.3342</v>
+      </c>
+      <c r="C32" s="5">
+        <v>3.4200000000000001E-2</v>
+      </c>
+      <c r="D32" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="F32" s="5">
+        <v>2.0899999999999998E-3</v>
+      </c>
+      <c r="G32" s="5">
+        <v>1.37E-4</v>
+      </c>
+      <c r="H32" s="5">
+        <v>8.1899999999999995E-6</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J32" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="0"/>
+        <v>0.37089999999999995</v>
+      </c>
+      <c r="C33" s="5">
+        <v>2.5899999999999999E-2</v>
+      </c>
+      <c r="D33" s="5">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="F33" s="5">
+        <v>2.8500000000000001E-3</v>
+      </c>
+      <c r="G33" s="5">
+        <v>1.4200000000000001E-4</v>
+      </c>
+      <c r="H33" s="5">
+        <v>7.9699999999999999E-6</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J33" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" s="9">
+        <f t="shared" si="0"/>
+        <v>4.1459999999999997E-2</v>
+      </c>
+      <c r="C34" s="5">
+        <v>3.6499999999999998E-2</v>
+      </c>
+      <c r="D34" s="5">
+        <v>4.96E-3</v>
+      </c>
+      <c r="E34" s="5">
+        <v>8.4199999999999998E-4</v>
+      </c>
+      <c r="F34" s="5">
+        <v>1.47E-3</v>
+      </c>
+      <c r="G34" s="5">
+        <v>1.3699999999999999E-5</v>
+      </c>
+      <c r="H34" s="5">
+        <v>1.3999999999999999E-4</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J34" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>57</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="0"/>
+        <v>0.34699999999999998</v>
+      </c>
+      <c r="C35" s="5">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="D35" s="5">
+        <v>0.216</v>
+      </c>
+      <c r="E35" s="5">
+        <v>7.0200000000000004E-4</v>
+      </c>
+      <c r="F35" s="5">
+        <v>1.26E-2</v>
+      </c>
+      <c r="G35" s="5">
+        <v>9.7499999999999996E-4</v>
+      </c>
+      <c r="H35" s="5">
+        <v>9.7699999999999996E-6</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J35" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06AF85B5-DFA1-8340-9803-CB44123E00DF}">
-  <dimension ref="A1:C14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="5"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>2.992</v>
-      </c>
-      <c r="C2">
+      <c r="B4">
         <v>4.54</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="C4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
-        <v>0.24137999999999998</v>
-      </c>
-      <c r="C3">
+      <c r="B5">
         <v>2.06E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="C5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
-        <v>0.24137999999999998</v>
-      </c>
-      <c r="C4">
+      <c r="B6">
         <v>2.06E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="C6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
-        <v>0.35599999999999998</v>
-      </c>
-      <c r="C5">
+      <c r="B7">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="C7" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B6">
+      <c r="B8">
         <v>0</v>
       </c>
-      <c r="C6">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7">
-        <v>0.36520000000000002</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="B8">
-        <v>4.8364000000000002E-3</v>
-      </c>
-      <c r="C8">
+      <c r="B10">
         <v>8.8700000000000001E-5</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="C10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="8">
+        <v>5.63E-5</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>17</v>
       </c>
-      <c r="B9">
-        <v>6.2744500000000009E-2</v>
-      </c>
-      <c r="C9">
+      <c r="B12">
         <f>(0.0114+0.123)/2</f>
         <v>6.7199999999999996E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="C12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>8</v>
       </c>
-      <c r="B10">
+      <c r="B13">
+        <f t="shared" ref="B13" si="0">SUM(C13:D13)</f>
         <v>0</v>
       </c>
-      <c r="C10" t="s">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16">
+        <v>3.54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17">
+        <v>2.63E-2</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11">
-        <v>7.2999999999999995E-2</v>
-      </c>
-      <c r="C11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12">
-        <v>0.19400000000000001</v>
-      </c>
-      <c r="C12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="B18">
+        <v>1.64</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19">
+        <v>2.4299999999999999E-2</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20">
+        <v>8.0700000000000008E-3</v>
+      </c>
+      <c r="D20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21">
+        <v>2.66E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="8">
+        <v>7.5499999999999994E-8</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23">
+        <v>4.0399999999999998E-2</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>24</v>
       </c>
-      <c r="C13">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14">
-        <v>1.8638999999999999</v>
-      </c>
-      <c r="C14" t="s">
-        <v>28</v>
+      <c r="B24">
+        <v>3.8699999999999998E-2</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25">
+        <v>2.1499999999999998E-2</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27">
+        <v>1.5299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28">
+        <v>1.03E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29">
+        <v>1.9699999999999999E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31">
+        <v>1.7000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32">
+        <v>0.58499999999999996</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33">
+        <v>0.58599999999999997</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34">
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>57</v>
+      </c>
+      <c r="B35">
+        <v>0.81399999999999995</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2"/>
-    </row>
-    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>4.54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>2.06E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>2.06E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10">
-        <v>8.8700000000000001E-5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11">
-        <f>(0.0114+0.123)/2</f>
-        <v>6.7199999999999996E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12">
-        <v>3.54</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
connected heat use to DRI
</commit_message>
<xml_diff>
--- a/data/shared/upstream.xlsx
+++ b/data/shared/upstream.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\setanzer\GitHub\BlackBlox\data\shared\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/shared/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5B5BB8E-43EA-BD47-A946-CDD7BE7DC11C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1455" yWindow="465" windowWidth="22680" windowHeight="17535"/>
+    <workbookView xWindow="1460" yWindow="460" windowWidth="22680" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="emissions" sheetId="1" r:id="rId1"/>
     <sheet name="removals" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,12 +32,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="C9" authorId="0" shapeId="0">
+    <comment ref="C9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -74,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="76">
   <si>
     <t>meta-notes</t>
   </si>
@@ -296,12 +297,18 @@
   </si>
   <si>
     <t>wood chips, medium emissions</t>
+  </si>
+  <si>
+    <t>including disposal</t>
+  </si>
+  <si>
+    <t>charcoal (GLO)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0E+00"/>
@@ -675,28 +682,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A43" sqref="A43"/>
+      <selection pane="bottomRight" activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="3" max="4" width="12.7109375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" style="5" customWidth="1"/>
-    <col min="6" max="7" width="12.7109375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" customWidth="1"/>
+    <col min="3" max="4" width="12.6640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="16.5" style="5" customWidth="1"/>
+    <col min="6" max="7" width="12.6640625" style="5" customWidth="1"/>
     <col min="8" max="8" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.85546875" style="5"/>
+    <col min="9" max="9" width="8.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -728,7 +735,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -740,7 +747,7 @@
       <c r="G2" s="4"/>
       <c r="I2" s="4"/>
     </row>
-    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -756,7 +763,7 @@
       <c r="G3" s="4"/>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -790,7 +797,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -824,7 +831,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -852,7 +859,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -867,7 +874,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -875,7 +882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -887,7 +894,7 @@
         <v>0.36520000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -917,7 +924,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -950,7 +957,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -988,12 +995,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>8</v>
       </c>
       <c r="B13">
-        <f t="shared" ref="B13:B41" si="0">SUM(C13:D13)</f>
+        <f t="shared" ref="B13:B39" si="0">SUM(C13:D13)</f>
         <v>0</v>
       </c>
       <c r="C13" s="5">
@@ -1009,7 +1016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -1020,7 +1027,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -1031,7 +1038,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>26</v>
       </c>
@@ -1039,7 +1046,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -1072,7 +1079,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -1099,7 +1106,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -1129,7 +1136,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -1147,7 +1154,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -1159,7 +1166,7 @@
         <v>0.13900000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>70</v>
       </c>
@@ -1190,7 +1197,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -1220,7 +1227,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1229,23 +1236,23 @@
         <v>4.5786999999999995</v>
       </c>
       <c r="C24" s="5">
-        <f>C25+C39</f>
+        <f>C25+C38</f>
         <v>4.5299999999999994</v>
       </c>
       <c r="D24" s="5">
-        <f>D25+D39</f>
+        <f>D25+D38</f>
         <v>4.87E-2</v>
       </c>
       <c r="E24" s="5">
-        <f>E25+E39</f>
+        <f>E25+E38</f>
         <v>2.055E-3</v>
       </c>
       <c r="F24" s="5">
-        <f>F25+F39</f>
+        <f>F25+F38</f>
         <v>0.37600001169999997</v>
       </c>
       <c r="G24" s="5">
-        <f>G25+G39</f>
+        <f>G25+G38</f>
         <v>3.1939999999999998E-3</v>
       </c>
       <c r="H24" s="5">
@@ -1254,8 +1261,11 @@
       <c r="I24" s="5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>69</v>
       </c>
@@ -1285,7 +1295,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>45</v>
       </c>
@@ -1315,7 +1325,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>46</v>
       </c>
@@ -1327,7 +1337,7 @@
         <v>6.8199999999999997E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>47</v>
       </c>
@@ -1345,7 +1355,7 @@
         <v>1.2400000000000001E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>48</v>
       </c>
@@ -1363,7 +1373,7 @@
         <v>1.0900000000000001E-4</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>49</v>
       </c>
@@ -1381,82 +1391,100 @@
         <v>1.37E-4</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>50</v>
-      </c>
-      <c r="B31">
+        <v>51</v>
+      </c>
+      <c r="B31" s="9">
         <f t="shared" si="0"/>
-        <v>0.89800000000000002</v>
+        <v>2.05918</v>
       </c>
       <c r="C31" s="5">
-        <v>0.89800000000000002</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="D31" s="5">
+        <v>9.1800000000000007E-3</v>
+      </c>
+      <c r="F31" s="5">
+        <v>0.184</v>
+      </c>
+      <c r="G31" s="5">
+        <v>1.3699999999999999E-5</v>
+      </c>
+      <c r="H31" s="5">
+        <v>2.5000000000000002E-6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="B32" s="9">
         <f t="shared" si="0"/>
-        <v>2.05918</v>
+        <v>1.51</v>
       </c>
       <c r="C32" s="5">
-        <v>2.0499999999999998</v>
-      </c>
-      <c r="D32" s="5">
-        <v>9.1800000000000007E-3</v>
+        <v>1.51</v>
+      </c>
+      <c r="E32" s="5">
+        <v>2.8900000000000001E-5</v>
       </c>
       <c r="F32" s="5">
-        <v>0.184</v>
-      </c>
-      <c r="G32" s="5">
-        <v>1.3699999999999999E-5</v>
-      </c>
-      <c r="H32" s="5">
-        <v>2.5000000000000002E-6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.115</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>63</v>
-      </c>
-      <c r="B33" s="9">
+        <v>52</v>
+      </c>
+      <c r="B33">
         <f t="shared" si="0"/>
-        <v>1.51</v>
+        <v>0.3342</v>
       </c>
       <c r="C33" s="5">
-        <v>1.51</v>
-      </c>
-      <c r="E33" s="5">
-        <v>2.8900000000000001E-5</v>
+        <v>3.4200000000000001E-2</v>
+      </c>
+      <c r="D33" s="5">
+        <v>0.3</v>
       </c>
       <c r="F33" s="5">
-        <v>0.115</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2.0899999999999998E-3</v>
+      </c>
+      <c r="G33" s="5">
+        <v>1.37E-4</v>
+      </c>
+      <c r="H33" s="5">
+        <v>8.1899999999999995E-6</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J33" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B34">
         <f t="shared" si="0"/>
-        <v>0.3342</v>
+        <v>0.37089999999999995</v>
       </c>
       <c r="C34" s="5">
-        <v>3.4200000000000001E-2</v>
+        <v>2.5899999999999999E-2</v>
       </c>
       <c r="D34" s="5">
-        <v>0.3</v>
+        <v>0.34499999999999997</v>
       </c>
       <c r="F34" s="5">
-        <v>2.0899999999999998E-3</v>
+        <v>2.8500000000000001E-3</v>
       </c>
       <c r="G34" s="5">
-        <v>1.37E-4</v>
+        <v>1.4200000000000001E-4</v>
       </c>
       <c r="H34" s="5">
-        <v>8.1899999999999995E-6</v>
+        <v>7.9699999999999999E-6</v>
       </c>
       <c r="I34" s="5" t="s">
         <v>29</v>
@@ -1465,253 +1493,223 @@
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>53</v>
-      </c>
-      <c r="B35">
-        <f t="shared" si="0"/>
-        <v>0.37089999999999995</v>
-      </c>
-      <c r="C35" s="5">
-        <v>2.5899999999999999E-2</v>
-      </c>
-      <c r="D35" s="5">
-        <v>0.34499999999999997</v>
-      </c>
-      <c r="F35" s="5">
-        <v>2.8500000000000001E-3</v>
-      </c>
-      <c r="G35" s="5">
-        <v>1.4200000000000001E-4</v>
-      </c>
-      <c r="H35" s="5">
-        <v>7.9699999999999999E-6</v>
-      </c>
-      <c r="I35" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="J35" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
         <v>55</v>
       </c>
-      <c r="B36" s="9">
+      <c r="B35" s="9">
         <f t="shared" si="0"/>
         <v>3.6996000000000001E-2</v>
       </c>
+      <c r="C35" s="5">
+        <v>3.6499999999999998E-2</v>
+      </c>
+      <c r="D35" s="5">
+        <v>4.9600000000000002E-4</v>
+      </c>
+      <c r="E35" s="5">
+        <v>8.4199999999999998E-4</v>
+      </c>
+      <c r="F35" s="5">
+        <v>1.47E-3</v>
+      </c>
+      <c r="G35" s="5">
+        <v>1.3699999999999999E-5</v>
+      </c>
+      <c r="H35" s="5">
+        <v>1.3999999999999999E-4</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J35" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="0"/>
+        <v>0.34699999999999998</v>
+      </c>
       <c r="C36" s="5">
-        <v>3.6499999999999998E-2</v>
+        <v>0.13100000000000001</v>
       </c>
       <c r="D36" s="5">
-        <v>4.9600000000000002E-4</v>
+        <v>0.216</v>
       </c>
       <c r="E36" s="5">
-        <v>8.4199999999999998E-4</v>
+        <v>7.0200000000000004E-4</v>
       </c>
       <c r="F36" s="5">
-        <v>1.47E-3</v>
+        <v>1.26E-2</v>
       </c>
       <c r="G36" s="5">
-        <v>1.3699999999999999E-5</v>
+        <v>9.7499999999999996E-4</v>
       </c>
       <c r="H36" s="5">
-        <v>1.3999999999999999E-4</v>
+        <v>9.7699999999999996E-6</v>
       </c>
       <c r="I36" s="5" t="s">
         <v>29</v>
       </c>
       <c r="J36" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B37">
         <f t="shared" si="0"/>
-        <v>0.34699999999999998</v>
+        <v>4.5212000000000003</v>
       </c>
       <c r="C37" s="5">
-        <v>0.13100000000000001</v>
+        <v>4.4400000000000004</v>
       </c>
       <c r="D37" s="5">
-        <v>0.216</v>
+        <v>8.1199999999999994E-2</v>
       </c>
       <c r="E37" s="5">
-        <v>7.0200000000000004E-4</v>
+        <v>4.2500000000000003E-3</v>
       </c>
       <c r="F37" s="5">
-        <v>1.26E-2</v>
+        <v>0.41099999999999998</v>
       </c>
       <c r="G37" s="5">
-        <v>9.7499999999999996E-4</v>
+        <v>3.7000000000000002E-3</v>
       </c>
       <c r="H37" s="5">
-        <v>9.7699999999999996E-6</v>
+        <v>1.24E-5</v>
       </c>
       <c r="I37" s="5" t="s">
         <v>29</v>
       </c>
       <c r="J37" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B38">
         <f t="shared" si="0"/>
-        <v>4.5212000000000003</v>
+        <v>1.9741</v>
       </c>
       <c r="C38" s="5">
-        <v>4.4400000000000004</v>
+        <v>1.96</v>
       </c>
       <c r="D38" s="5">
-        <v>8.1199999999999994E-2</v>
+        <v>1.41E-2</v>
       </c>
       <c r="E38" s="5">
-        <v>4.2500000000000003E-3</v>
+        <v>2.1499999999999999E-4</v>
       </c>
       <c r="F38" s="5">
-        <v>0.41099999999999998</v>
+        <f>0.0000000117+0.025</f>
+        <v>2.5000011700000001E-2</v>
       </c>
       <c r="G38" s="5">
-        <v>3.7000000000000002E-3</v>
+        <f>0.000554</f>
+        <v>5.5400000000000002E-4</v>
       </c>
       <c r="H38" s="5">
-        <v>1.24E-5</v>
+        <f>0.00000336</f>
+        <v>3.36E-6</v>
       </c>
       <c r="I38" s="5" t="s">
         <v>29</v>
       </c>
       <c r="J38" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B39">
         <f t="shared" si="0"/>
-        <v>1.9741</v>
+        <v>8.7720000000000003E-3</v>
       </c>
       <c r="C39" s="5">
-        <v>1.96</v>
+        <v>8.3999999999999995E-3</v>
       </c>
       <c r="D39" s="5">
-        <v>1.41E-2</v>
+        <v>3.7199999999999999E-4</v>
       </c>
       <c r="E39" s="5">
-        <v>2.1499999999999999E-4</v>
+        <v>6.1099999999999999E-6</v>
       </c>
       <c r="F39" s="5">
-        <f>0.0000000117+0.025</f>
-        <v>2.5000011700000001E-2</v>
-      </c>
-      <c r="G39" s="5">
-        <f>0.000554</f>
-        <v>5.5400000000000002E-4</v>
-      </c>
-      <c r="H39" s="5">
-        <f>0.00000336</f>
-        <v>3.36E-6</v>
-      </c>
-      <c r="I39" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="J39" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>68</v>
-      </c>
-      <c r="B40">
-        <f t="shared" si="0"/>
-        <v>8.7720000000000003E-3</v>
-      </c>
-      <c r="C40" s="5">
-        <v>8.3999999999999995E-3</v>
-      </c>
-      <c r="D40" s="5">
-        <v>3.7199999999999999E-4</v>
-      </c>
-      <c r="E40" s="5">
-        <v>6.1099999999999999E-6</v>
-      </c>
-      <c r="F40" s="5">
         <f>0.000000000197+0.000391</f>
         <v>3.9100019700000004E-4</v>
       </c>
-      <c r="G40" s="5">
+      <c r="G39" s="5">
         <f>0.00000663</f>
         <v>6.63E-6</v>
       </c>
-      <c r="H40" s="5">
+      <c r="H39" s="5">
         <f>0.0000000773</f>
         <v>7.7299999999999997E-8</v>
       </c>
-      <c r="I40" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="J40" t="s">
+      <c r="I39" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J39" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>71</v>
       </c>
-      <c r="B41">
-        <f>B37</f>
+      <c r="B40">
+        <f>B36</f>
         <v>0.34699999999999998</v>
       </c>
-      <c r="C41">
-        <f t="shared" ref="C41:H41" si="2">C37</f>
+      <c r="C40">
+        <f t="shared" ref="C40:H40" si="2">C36</f>
         <v>0.13100000000000001</v>
       </c>
-      <c r="D41">
+      <c r="D40">
         <f t="shared" si="2"/>
         <v>0.216</v>
       </c>
-      <c r="E41">
+      <c r="E40">
         <f t="shared" si="2"/>
         <v>7.0200000000000004E-4</v>
       </c>
-      <c r="F41">
+      <c r="F40">
         <f t="shared" si="2"/>
         <v>1.26E-2</v>
       </c>
-      <c r="G41">
+      <c r="G40">
         <f t="shared" si="2"/>
         <v>9.7499999999999996E-4</v>
       </c>
-      <c r="H41">
+      <c r="H40">
         <f t="shared" si="2"/>
         <v>9.7699999999999996E-6</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>72</v>
+      </c>
+      <c r="B41">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B42">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>73</v>
-      </c>
-      <c r="B43">
         <v>0.1</v>
       </c>
     </row>
@@ -1723,21 +1721,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40:XFD40"/>
+    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="5"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1751,14 +1749,14 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1767,7 +1765,7 @@
       </c>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1778,10 +1776,10 @@
         <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1795,7 +1793,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1809,7 +1807,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1820,7 +1818,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1828,7 +1826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1836,7 +1834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1850,7 +1848,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -1864,7 +1862,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1879,7 +1877,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1888,7 +1886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -1899,7 +1897,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -1910,7 +1908,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -1921,7 +1919,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -1935,7 +1933,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -1946,7 +1944,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -1957,7 +1955,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -1968,7 +1966,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -1976,7 +1974,7 @@
         <v>2.66E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>70</v>
       </c>
@@ -1987,7 +1985,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -1998,7 +1996,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -2009,7 +2007,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>45</v>
       </c>
@@ -2020,7 +2018,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>46</v>
       </c>
@@ -2028,7 +2026,7 @@
         <v>1.03</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>47</v>
       </c>
@@ -2036,7 +2034,7 @@
         <v>1.5299999999999999E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>48</v>
       </c>
@@ -2044,7 +2042,7 @@
         <v>1.03E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>49</v>
       </c>
@@ -2052,12 +2050,12 @@
         <v>1.9699999999999999E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>51</v>
       </c>
@@ -2065,7 +2063,7 @@
         <v>1.7000000000000001E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>52</v>
       </c>
@@ -2073,7 +2071,7 @@
         <v>0.58499999999999996</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>53</v>
       </c>
@@ -2081,7 +2079,7 @@
         <v>0.58599999999999997</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>55</v>
       </c>
@@ -2089,7 +2087,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>56</v>
       </c>
@@ -2097,7 +2095,7 @@
         <v>0.81399999999999995</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>63</v>
       </c>
@@ -2105,7 +2103,7 @@
         <v>2.3300000000000001E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>66</v>
       </c>
@@ -2116,7 +2114,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>65</v>
       </c>
@@ -2124,7 +2122,7 @@
         <v>4.57E-4</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>71</v>
       </c>
@@ -2133,7 +2131,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>72</v>
       </c>
@@ -2141,7 +2139,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>73</v>
       </c>

</xml_diff>

<commit_message>
added remaining factory use values
</commit_message>
<xml_diff>
--- a/data/shared/upstream.xlsx
+++ b/data/shared/upstream.xlsx
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="103">
   <si>
     <t>meta-notes</t>
   </si>
@@ -346,9 +346,6 @@
     <t>BF factory use</t>
   </si>
   <si>
-    <t>o2 factory use</t>
-  </si>
-  <si>
     <t>pellet factory use</t>
   </si>
   <si>
@@ -374,6 +371,18 @@
   </si>
   <si>
     <t>lime kiln use</t>
+  </si>
+  <si>
+    <t>O2 factory use</t>
+  </si>
+  <si>
+    <t>electricity turbine use</t>
+  </si>
+  <si>
+    <t>heat turbine use</t>
+  </si>
+  <si>
+    <t>includes methane emissions from nat gas use</t>
   </si>
 </sst>
 </file>
@@ -777,13 +786,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O58"/>
+  <dimension ref="A1:O60"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B63" sqref="B63"/>
+      <selection pane="bottomRight" activeCell="A59" sqref="A59:A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -817,7 +826,7 @@
         <v>77</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G1" s="15" t="s">
         <v>83</v>
@@ -835,7 +844,7 @@
         <v>74</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>75</v>
@@ -1055,7 +1064,7 @@
         <v>9</v>
       </c>
       <c r="G8" s="14">
-        <f t="shared" ref="G8:G58" si="1">SUM(H8:J8)</f>
+        <f t="shared" ref="G8:G47" si="1">SUM(H8:J8)</f>
         <v>0</v>
       </c>
       <c r="M8" s="9"/>
@@ -1323,11 +1332,11 @@
         <v>2.5900000000000002E-6</v>
       </c>
       <c r="K17" s="5">
-        <f>SUM(C17:J17)</f>
+        <f t="shared" ref="K17:K26" si="5">SUM(C17:J17)</f>
         <v>0.92065617999999994</v>
       </c>
       <c r="M17" s="9">
-        <f>K17/B17</f>
+        <f t="shared" ref="M17:M43" si="6">K17/B17</f>
         <v>1.2088146172823946</v>
       </c>
       <c r="N17" s="5" t="s">
@@ -1365,11 +1374,11 @@
         <v>1.5900000000000001E-3</v>
       </c>
       <c r="K18" s="5">
-        <f>SUM(C18:J18)</f>
+        <f t="shared" si="5"/>
         <v>5.7041800000000009</v>
       </c>
       <c r="M18" s="10">
-        <f>K18/B18</f>
+        <f t="shared" si="6"/>
         <v>1.5580934170991534</v>
       </c>
       <c r="N18" s="5" t="s">
@@ -1407,11 +1416,11 @@
         <v>1.95E-6</v>
       </c>
       <c r="K19" s="5">
-        <f>SUM(C19:J19)</f>
+        <f t="shared" si="5"/>
         <v>0.86062178</v>
       </c>
       <c r="M19" s="10">
-        <f>K19/B19</f>
+        <f t="shared" si="6"/>
         <v>32.348121781619994</v>
       </c>
       <c r="N19" s="5" t="s">
@@ -1437,11 +1446,11 @@
         <v>0</v>
       </c>
       <c r="K20" s="5">
-        <f>SUM(C20:J20)</f>
+        <f t="shared" si="5"/>
         <v>0.32052000000000003</v>
       </c>
       <c r="M20" s="9">
-        <f>K20/B20</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="O20" t="s">
@@ -1464,11 +1473,11 @@
         <v>0</v>
       </c>
       <c r="K21" s="5">
-        <f>SUM(C21:J21)</f>
+        <f t="shared" si="5"/>
         <v>0.13900000000000001</v>
       </c>
       <c r="M21" s="9">
-        <f>K21/B21</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -1505,11 +1514,11 @@
         <v>1.8199999999999999E-10</v>
       </c>
       <c r="K22" s="5">
-        <f>SUM(C22:J22)</f>
+        <f t="shared" si="5"/>
         <v>1.7970176399999998E-4</v>
       </c>
       <c r="M22" s="10">
-        <f>K22/B22</f>
+        <f t="shared" si="6"/>
         <v>2.5424194201020351</v>
       </c>
       <c r="N22" s="5" t="s">
@@ -1547,11 +1556,11 @@
         <v>5.1499999999999998E-5</v>
       </c>
       <c r="K23" s="5">
-        <f>SUM(C23:J23)</f>
+        <f t="shared" si="5"/>
         <v>3.3721429999999999</v>
       </c>
       <c r="M23" s="9">
-        <f>K23/B23</f>
+        <f t="shared" si="6"/>
         <v>1.2926229319676783</v>
       </c>
       <c r="N23" s="5" t="s">
@@ -1594,11 +1603,11 @@
         <v>5.0099999999999998E-5</v>
       </c>
       <c r="K24" s="5">
-        <f>SUM(C24:J24)</f>
+        <f t="shared" si="5"/>
         <v>5.3392432234000005</v>
       </c>
       <c r="M24" s="9">
-        <f>K24/B24</f>
+        <f t="shared" si="6"/>
         <v>1.1655814867636449</v>
       </c>
       <c r="N24" s="5" t="s">
@@ -1639,11 +1648,11 @@
         <v>5.0099999999999998E-5</v>
       </c>
       <c r="K25" s="5">
-        <f>SUM(C25:J25)</f>
+        <f t="shared" si="5"/>
         <v>3.3138202000000003</v>
       </c>
       <c r="M25" s="9">
-        <f>K25/B25</f>
+        <f t="shared" si="6"/>
         <v>1.2713970780067834</v>
       </c>
       <c r="N25" s="5" t="s">
@@ -1681,11 +1690,11 @@
         <v>3.8E-6</v>
       </c>
       <c r="K26" s="5">
-        <f>SUM(C26:J26)</f>
+        <f t="shared" si="5"/>
         <v>2.8003356000000004</v>
       </c>
       <c r="M26" s="10">
-        <f>K26/B26</f>
+        <f t="shared" si="6"/>
         <v>1.4083857307388614</v>
       </c>
       <c r="N26" s="5" t="s">
@@ -1708,7 +1717,7 @@
         <v>0</v>
       </c>
       <c r="M27" s="9">
-        <f>K27/B27</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -1734,11 +1743,11 @@
         <v>1.2400000000000001E-4</v>
       </c>
       <c r="K28" s="5">
-        <f>SUM(C28:J28)</f>
+        <f t="shared" ref="K28:K43" si="7">SUM(C28:J28)</f>
         <v>2.0973480000000002</v>
       </c>
       <c r="M28" s="9">
-        <f>K28/B28</f>
+        <f t="shared" si="6"/>
         <v>1.0001182585475181</v>
       </c>
     </row>
@@ -1764,11 +1773,11 @@
         <v>1.0900000000000001E-4</v>
       </c>
       <c r="K29" s="5">
-        <f>SUM(C29:J29)</f>
+        <f t="shared" si="7"/>
         <v>1.9522179999999998</v>
       </c>
       <c r="M29" s="9">
-        <f>K29/B29</f>
+        <f t="shared" si="6"/>
         <v>1.0001116803278687</v>
       </c>
     </row>
@@ -1794,11 +1803,11 @@
         <v>1.37E-4</v>
       </c>
       <c r="K30" s="5">
-        <f>SUM(C30:J30)</f>
+        <f t="shared" si="7"/>
         <v>2.1916739999999999</v>
       </c>
       <c r="M30" s="9">
-        <f>K30/B30</f>
+        <f t="shared" si="6"/>
         <v>1.0001250342246966</v>
       </c>
     </row>
@@ -1830,11 +1839,11 @@
         <v>2.5000000000000002E-6</v>
       </c>
       <c r="K31" s="5">
-        <f>SUM(C31:J31)</f>
+        <f t="shared" si="7"/>
         <v>2.4272123999999997</v>
       </c>
       <c r="M31" s="9">
-        <f>K31/B31</f>
+        <f t="shared" si="6"/>
         <v>1.1787276488699383</v>
       </c>
     </row>
@@ -1860,11 +1869,11 @@
         <v>0.115</v>
       </c>
       <c r="K32" s="5">
-        <f>SUM(C32:J32)</f>
+        <f t="shared" si="7"/>
         <v>1.7400289</v>
       </c>
       <c r="M32" s="9">
-        <f>K32/B32</f>
+        <f t="shared" si="6"/>
         <v>1.1523149656274791</v>
       </c>
     </row>
@@ -1896,11 +1905,11 @@
         <v>8.1899999999999995E-6</v>
       </c>
       <c r="K33" s="5">
-        <f>SUM(C33:J33)</f>
+        <f t="shared" si="7"/>
         <v>0.33867037999999999</v>
       </c>
       <c r="M33" s="9">
-        <f>K33/B33</f>
+        <f t="shared" si="6"/>
         <v>1.0133763614602034</v>
       </c>
       <c r="N33" s="5" t="s">
@@ -1938,11 +1947,11 @@
         <v>7.9699999999999999E-6</v>
       </c>
       <c r="K34" s="5">
-        <f>SUM(C34:J34)</f>
+        <f t="shared" si="7"/>
         <v>0.37689993999999999</v>
       </c>
       <c r="M34" s="9">
-        <f>K34/B34</f>
+        <f t="shared" si="6"/>
         <v>1.0161767053114048</v>
       </c>
       <c r="N34" s="5" t="s">
@@ -1983,11 +1992,11 @@
         <v>1.3999999999999999E-4</v>
       </c>
       <c r="K35" s="5">
-        <f>SUM(C35:J35)</f>
+        <f t="shared" si="7"/>
         <v>4.1085400000000001E-2</v>
       </c>
       <c r="M35" s="9">
-        <f>K35/B35</f>
+        <f t="shared" si="6"/>
         <v>1.0858237750409641</v>
       </c>
       <c r="N35" s="5" t="s">
@@ -2028,11 +2037,11 @@
         <v>9.7699999999999996E-6</v>
       </c>
       <c r="K36" s="5">
-        <f>SUM(C36:J36)</f>
+        <f t="shared" si="7"/>
         <v>0.37487154</v>
       </c>
       <c r="M36" s="9">
-        <f>K36/B36</f>
+        <f t="shared" si="6"/>
         <v>1.0781403040534712</v>
       </c>
       <c r="N36" s="5" t="s">
@@ -2073,11 +2082,11 @@
         <v>1.24E-5</v>
       </c>
       <c r="K37" s="5">
-        <f>SUM(C37:J37)</f>
+        <f t="shared" si="7"/>
         <v>5.3548748000000002</v>
       </c>
       <c r="M37" s="9">
-        <f>K37/B37</f>
+        <f t="shared" si="6"/>
         <v>1.18328007159509</v>
       </c>
       <c r="N37" s="5" t="s">
@@ -2121,11 +2130,11 @@
         <v>3.36E-6</v>
       </c>
       <c r="K38" s="5">
-        <f>SUM(C38:J38)</f>
+        <f t="shared" si="7"/>
         <v>2.0254297434000001</v>
       </c>
       <c r="M38" s="9">
-        <f>K38/B38</f>
+        <f t="shared" si="6"/>
         <v>1.0258898622560231</v>
       </c>
       <c r="N38" s="5" t="s">
@@ -2169,11 +2178,11 @@
         <v>7.7299999999999997E-8</v>
       </c>
       <c r="K39" s="5">
-        <f>SUM(C39:J39)</f>
+        <f t="shared" si="7"/>
         <v>9.573524994000002E-3</v>
       </c>
       <c r="M39" s="9">
-        <f>K39/B39</f>
+        <f t="shared" si="6"/>
         <v>1.0906134685029012</v>
       </c>
       <c r="N39" s="5" t="s">
@@ -2192,15 +2201,15 @@
         <v>0.34770199999999996</v>
       </c>
       <c r="C40">
-        <f t="shared" ref="C40:J40" si="5">C36</f>
+        <f t="shared" ref="C40:J40" si="8">C36</f>
         <v>0.13100000000000001</v>
       </c>
       <c r="D40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.216</v>
       </c>
       <c r="E40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>7.0200000000000004E-4</v>
       </c>
       <c r="F40"/>
@@ -2209,23 +2218,23 @@
         <v>1.3584769999999999E-2</v>
       </c>
       <c r="H40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.26E-2</v>
       </c>
       <c r="I40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>9.7499999999999996E-4</v>
       </c>
       <c r="J40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>9.7699999999999996E-6</v>
       </c>
       <c r="K40" s="5">
-        <f>SUM(C40:J40)</f>
+        <f t="shared" si="7"/>
         <v>0.37487154</v>
       </c>
       <c r="M40" s="9">
-        <f>K40/B40</f>
+        <f t="shared" si="6"/>
         <v>1.0781403040534712</v>
       </c>
     </row>
@@ -2241,11 +2250,11 @@
         <v>0</v>
       </c>
       <c r="K41" s="5">
-        <f>SUM(C41:J41)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M41" s="9">
-        <f>K41/B41</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -2261,11 +2270,11 @@
         <v>0</v>
       </c>
       <c r="K42" s="5">
-        <f>SUM(C42:J42)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M42" s="9">
-        <f>K42/B42</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -2282,11 +2291,11 @@
         <v>0</v>
       </c>
       <c r="K43" s="5">
-        <f>SUM(C43:J43)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M43" s="9">
-        <f>K43/B43</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -2378,7 +2387,7 @@
         <v>82</v>
       </c>
       <c r="B47" s="11">
-        <f t="shared" ref="B47:B58" si="6">SUM(C47:E47)</f>
+        <f t="shared" ref="B47" si="9">SUM(C47:E47)</f>
         <v>0.12100999999999999</v>
       </c>
       <c r="C47" s="5">
@@ -2421,7 +2430,7 @@
         <v>1.13E-5</v>
       </c>
       <c r="F48" s="11">
-        <f>SUM(C48:E48)</f>
+        <f t="shared" ref="F48:F58" si="10">SUM(C48:E48)</f>
         <v>1.1072300000000002E-2</v>
       </c>
       <c r="H48" s="5">
@@ -2435,11 +2444,11 @@
       </c>
       <c r="K48" s="7"/>
       <c r="L48" s="14">
-        <f>SUM(H48:J48)</f>
+        <f t="shared" ref="L48:L60" si="11">SUM(H48:J48)</f>
         <v>1.0599427000000002E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>86</v>
       </c>
@@ -2453,7 +2462,7 @@
         <v>1.7399999999999999E-5</v>
       </c>
       <c r="F49" s="11">
-        <f>SUM(C49:E49)</f>
+        <f t="shared" si="10"/>
         <v>3.3737400000000001E-2</v>
       </c>
       <c r="H49" s="5">
@@ -2466,11 +2475,11 @@
         <v>9.3999999999999995E-8</v>
       </c>
       <c r="L49" s="14">
-        <f>SUM(H49:J49)</f>
+        <f t="shared" si="11"/>
         <v>1.8145939999999999E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>87</v>
       </c>
@@ -2484,7 +2493,7 @@
         <v>4.5800000000000002E-4</v>
       </c>
       <c r="F50" s="11">
-        <f>SUM(C50:E50)</f>
+        <f t="shared" si="10"/>
         <v>0.53225800000000001</v>
       </c>
       <c r="H50" s="5">
@@ -2497,11 +2506,11 @@
         <v>1.9E-6</v>
       </c>
       <c r="L50" s="14">
-        <f>SUM(H50:J50)</f>
+        <f t="shared" si="11"/>
         <v>5.4999899999999997E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>88</v>
       </c>
@@ -2515,7 +2524,7 @@
         <v>5.1200000000000002E-8</v>
       </c>
       <c r="F51" s="11">
-        <f>SUM(C51:E51)</f>
+        <f t="shared" si="10"/>
         <v>7.8016200000000007E-5</v>
       </c>
       <c r="H51" s="7">
@@ -2528,11 +2537,11 @@
         <v>3.5099999999999998E-10</v>
       </c>
       <c r="L51" s="14">
-        <f>SUM(H51:J51)</f>
+        <f t="shared" si="11"/>
         <v>6.6999509999999995E-6</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>89</v>
       </c>
@@ -2546,7 +2555,7 @@
         <v>1.0499999999999999E-5</v>
       </c>
       <c r="F52" s="11">
-        <f>SUM(C52:E52)</f>
+        <f t="shared" si="10"/>
         <v>1.9099500000000002E-2</v>
       </c>
       <c r="H52" s="5">
@@ -2559,13 +2568,13 @@
         <v>4.6499999999999999E-8</v>
       </c>
       <c r="L52" s="14">
-        <f>SUM(H52:J52)</f>
+        <f t="shared" si="11"/>
         <v>8.1044649999999999E-4</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="C53" s="5">
         <v>9.8900000000000008E-4</v>
@@ -2577,7 +2586,7 @@
         <v>2.1100000000000001E-6</v>
       </c>
       <c r="F53" s="11">
-        <f>SUM(C53:E53)</f>
+        <f t="shared" si="10"/>
         <v>1.0214100000000002E-3</v>
       </c>
       <c r="H53" s="5">
@@ -2590,13 +2599,13 @@
         <v>6.1900000000000003E-9</v>
       </c>
       <c r="L53" s="14">
-        <f>SUM(H53:J53)</f>
+        <f t="shared" si="11"/>
         <v>1.1458618999999999E-4</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C54" s="5">
         <v>2.1299999999999999E-2</v>
@@ -2608,7 +2617,7 @@
         <v>2.4899999999999999E-5</v>
       </c>
       <c r="F54" s="11">
-        <f>SUM(C54:E54)</f>
+        <f t="shared" si="10"/>
         <v>2.17819E-2</v>
       </c>
       <c r="H54" s="5">
@@ -2621,13 +2630,13 @@
         <v>7.17E-8</v>
       </c>
       <c r="L54" s="14">
-        <f>SUM(H54:J54)</f>
+        <f t="shared" si="11"/>
         <v>3.3639717000000001E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C55" s="5">
         <v>1.21E-2</v>
@@ -2639,7 +2648,7 @@
         <v>6.9700000000000002E-6</v>
       </c>
       <c r="F55" s="11">
-        <f>SUM(C55:E55)</f>
+        <f t="shared" si="10"/>
         <v>1.2324969999999999E-2</v>
       </c>
       <c r="H55" s="5">
@@ -2652,13 +2661,13 @@
         <v>2.85E-8</v>
       </c>
       <c r="L55" s="14">
-        <f>SUM(H55:J55)</f>
+        <f t="shared" si="11"/>
         <v>8.7928850000000005E-4</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C56" s="5">
         <v>4.9800000000000001E-3</v>
@@ -2670,7 +2679,7 @@
         <v>2.3E-6</v>
       </c>
       <c r="F56" s="11">
-        <f>SUM(C56:E56)</f>
+        <f t="shared" si="10"/>
         <v>5.0114000000000001E-3</v>
       </c>
       <c r="H56" s="5">
@@ -2683,13 +2692,13 @@
         <v>4.4599999999999999E-9</v>
       </c>
       <c r="L56" s="14">
-        <f>SUM(H56:J56)</f>
+        <f t="shared" si="11"/>
         <v>5.8874445999999988E-4</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C57" s="5">
         <v>1.43E-2</v>
@@ -2701,7 +2710,7 @@
         <v>7.5800000000000003E-6</v>
       </c>
       <c r="F57" s="11">
-        <f>SUM(C57:E57)</f>
+        <f t="shared" si="10"/>
         <v>1.4915580000000001E-2</v>
       </c>
       <c r="H57" s="7">
@@ -2714,13 +2723,13 @@
         <v>4.3999999999999997E-8</v>
       </c>
       <c r="L57" s="14">
-        <f>SUM(H57:J57)</f>
+        <f t="shared" si="11"/>
         <v>5.9562840000000009E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C58" s="5">
         <v>5.4299999999999999E-3</v>
@@ -2732,7 +2741,7 @@
         <v>4.8099999999999997E-5</v>
       </c>
       <c r="F58" s="11">
-        <f>SUM(C58:E58)</f>
+        <f t="shared" si="10"/>
         <v>2.5078099999999999E-2</v>
       </c>
       <c r="H58" s="5">
@@ -2745,8 +2754,76 @@
         <v>6.1600000000000001E-7</v>
       </c>
       <c r="L58" s="14">
-        <f>SUM(H58:J58)</f>
+        <f t="shared" si="11"/>
         <v>5.3051600000000008E-4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>100</v>
+      </c>
+      <c r="C59" s="5">
+        <v>1.2400000000000001E-4</v>
+      </c>
+      <c r="D59" s="5">
+        <v>5.5600000000000001E-6</v>
+      </c>
+      <c r="E59" s="5">
+        <v>1.2200000000000001E-7</v>
+      </c>
+      <c r="F59" s="5">
+        <f>SUM(C59:E59)</f>
+        <v>1.29682E-4</v>
+      </c>
+      <c r="H59" s="5">
+        <v>4.26E-4</v>
+      </c>
+      <c r="I59" s="5">
+        <v>1.67E-7</v>
+      </c>
+      <c r="J59" s="7">
+        <v>1.6999999999999999E-9</v>
+      </c>
+      <c r="L59" s="5">
+        <f t="shared" si="11"/>
+        <v>4.2616869999999996E-4</v>
+      </c>
+      <c r="O59" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>101</v>
+      </c>
+      <c r="C60" s="5">
+        <v>2.12E-4</v>
+      </c>
+      <c r="D60" s="5">
+        <v>1.04E-5</v>
+      </c>
+      <c r="E60" s="5">
+        <v>1.8900000000000001E-7</v>
+      </c>
+      <c r="F60" s="5">
+        <f>SUM(C60:E60)</f>
+        <v>2.2258900000000001E-4</v>
+      </c>
+      <c r="H60" s="5">
+        <v>9.6599999999999995E-4</v>
+      </c>
+      <c r="I60" s="5">
+        <v>1.02E-8</v>
+      </c>
+      <c r="J60" s="7">
+        <v>1.25E-9</v>
+      </c>
+      <c r="L60" s="5">
+        <f t="shared" si="11"/>
+        <v>9.6601144999999995E-4</v>
+      </c>
+      <c r="O60" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -2758,10 +2835,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E57"/>
+  <dimension ref="A1:E59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" zoomScale="101" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2779,7 +2856,7 @@
         <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>12</v>
@@ -3274,7 +3351,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="C52" s="8">
         <v>3.2499999999999997E-5</v>
@@ -3282,7 +3359,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C53">
         <v>6.2E-4</v>
@@ -3290,7 +3367,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C54" s="8">
         <v>1.7699999999999999E-4</v>
@@ -3298,7 +3375,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C55" s="8">
         <v>4.88E-5</v>
@@ -3306,7 +3383,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C56" s="8">
         <v>5.71E-4</v>
@@ -3314,10 +3391,26 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C57" s="8">
         <v>1.7899999999999999E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>100</v>
+      </c>
+      <c r="C58" s="8">
+        <v>5.5799999999999999E-6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>101</v>
+      </c>
+      <c r="C59" s="8">
+        <v>9.7100000000000002E-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
upstream emissions cleft timber and alloy use
</commit_message>
<xml_diff>
--- a/data/shared/upstream.xlsx
+++ b/data/shared/upstream.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/shared/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\setanzer\GitHub\BlackBlox\data\shared\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FA351AA-F161-C94B-9090-7563B36FEA17}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
   </bookViews>
   <sheets>
     <sheet name="emissions" sheetId="1" r:id="rId1"/>
     <sheet name="removals" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,12 +31,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="C9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="C9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -392,7 +391,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
@@ -797,31 +796,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K61" sqref="K61"/>
+      <selection pane="bottomRight" activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="15.1640625" style="11" customWidth="1"/>
-    <col min="3" max="4" width="12.6640625" style="5" customWidth="1"/>
-    <col min="5" max="6" width="10.83203125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="14" customWidth="1"/>
-    <col min="8" max="9" width="12.6640625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="8.6640625" style="5" customWidth="1"/>
-    <col min="11" max="12" width="9.83203125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" style="11" customWidth="1"/>
+    <col min="3" max="4" width="12.7109375" style="5" customWidth="1"/>
+    <col min="5" max="6" width="10.85546875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" style="14" customWidth="1"/>
+    <col min="8" max="9" width="12.7109375" style="5" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" style="5" customWidth="1"/>
+    <col min="11" max="12" width="9.85546875" style="5" customWidth="1"/>
     <col min="13" max="13" width="11" style="5" customWidth="1"/>
-    <col min="14" max="14" width="8.83203125" style="5"/>
+    <col min="14" max="14" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -868,7 +867,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -882,7 +881,7 @@
       <c r="I2" s="4"/>
       <c r="N2" s="4"/>
     </row>
-    <row r="3" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -917,7 +916,7 @@
       <c r="L3" s="4"/>
       <c r="N3" s="4"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -963,7 +962,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1009,7 +1008,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1049,7 +1048,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1071,7 +1070,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1081,7 +1080,7 @@
       </c>
       <c r="M8" s="9"/>
     </row>
-    <row r="9" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1101,7 +1100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1143,7 +1142,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -1188,7 +1187,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1238,7 +1237,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1268,7 +1267,7 @@
       </c>
       <c r="M13" s="9"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -1284,7 +1283,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -1300,7 +1299,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>26</v>
       </c>
@@ -1313,7 +1312,7 @@
       </c>
       <c r="M16" s="9"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -1358,7 +1357,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -1397,7 +1396,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -1439,7 +1438,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -1469,7 +1468,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -1493,7 +1492,7 @@
         <v>1.0010190863309352</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>67</v>
       </c>
@@ -1537,7 +1536,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -1579,7 +1578,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1629,7 +1628,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>66</v>
       </c>
@@ -1671,7 +1670,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>44</v>
       </c>
@@ -1713,7 +1712,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>45</v>
       </c>
@@ -1733,7 +1732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>46</v>
       </c>
@@ -1763,7 +1762,7 @@
         <v>1.0001182585475181</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>47</v>
       </c>
@@ -1793,7 +1792,7 @@
         <v>1.0001116803278687</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>48</v>
       </c>
@@ -1823,7 +1822,7 @@
         <v>1.0001250342246966</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>50</v>
       </c>
@@ -1859,7 +1858,7 @@
         <v>1.1787276488699383</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>61</v>
       </c>
@@ -1889,7 +1888,7 @@
         <v>1.1523149656274791</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>51</v>
       </c>
@@ -1931,7 +1930,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>52</v>
       </c>
@@ -1973,7 +1972,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>53</v>
       </c>
@@ -2018,7 +2017,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>54</v>
       </c>
@@ -2063,7 +2062,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>59</v>
       </c>
@@ -2108,7 +2107,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>62</v>
       </c>
@@ -2156,7 +2155,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>73</v>
       </c>
@@ -2204,7 +2203,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>68</v>
       </c>
@@ -2250,7 +2249,7 @@
         <v>1.0781403040534712</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>69</v>
       </c>
@@ -2270,7 +2269,7 @@
         <v>2.7169539999999999E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>70</v>
       </c>
@@ -2290,7 +2289,7 @@
         <v>0.13584769999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>78</v>
       </c>
@@ -2311,7 +2310,7 @@
         <v>0.7652392751948599</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>79</v>
       </c>
@@ -2324,7 +2323,7 @@
         <v>1.1457392000000002</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>80</v>
       </c>
@@ -2359,7 +2358,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>81</v>
       </c>
@@ -2394,12 +2393,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>82</v>
       </c>
       <c r="B47" s="11">
-        <f t="shared" ref="B47" si="9">SUM(C47:E47)</f>
+        <f t="shared" ref="B47:B60" si="9">SUM(C47:E47)</f>
         <v>0.12100999999999999</v>
       </c>
       <c r="C47" s="5">
@@ -2428,7 +2427,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>85</v>
       </c>
@@ -2460,7 +2459,7 @@
         <v>1.0599427000000002E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>86</v>
       </c>
@@ -2491,7 +2490,7 @@
         <v>1.8145939999999999E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>87</v>
       </c>
@@ -2522,7 +2521,7 @@
         <v>5.4999899999999997E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>88</v>
       </c>
@@ -2553,7 +2552,7 @@
         <v>6.6999509999999995E-6</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>89</v>
       </c>
@@ -2584,7 +2583,7 @@
         <v>8.1044649999999999E-4</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>99</v>
       </c>
@@ -2615,7 +2614,7 @@
         <v>1.1458618999999999E-4</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>90</v>
       </c>
@@ -2646,7 +2645,7 @@
         <v>3.3639717000000001E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>91</v>
       </c>
@@ -2677,7 +2676,7 @@
         <v>8.7928850000000005E-4</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>92</v>
       </c>
@@ -2708,7 +2707,7 @@
         <v>5.8874445999999988E-4</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>94</v>
       </c>
@@ -2739,7 +2738,7 @@
         <v>5.9562840000000009E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>98</v>
       </c>
@@ -2770,7 +2769,7 @@
         <v>5.3051600000000008E-4</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>100</v>
       </c>
@@ -2804,7 +2803,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>101</v>
       </c>
@@ -2838,17 +2837,39 @@
         <v>102</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="16" t="s">
         <v>103</v>
       </c>
       <c r="B61" s="11">
-        <f>B40</f>
-        <v>0.34770199999999996</v>
-      </c>
-      <c r="G61" s="11">
-        <f>G40</f>
-        <v>1.3584769999999999E-2</v>
+        <f t="shared" ref="B61" si="12">SUM(C61:E61)</f>
+        <v>3.2772999999999997E-2</v>
+      </c>
+      <c r="C61" s="5">
+        <v>3.0800000000000001E-2</v>
+      </c>
+      <c r="D61" s="5">
+        <v>6.4300000000000002E-4</v>
+      </c>
+      <c r="E61" s="5">
+        <v>1.33E-3</v>
+      </c>
+      <c r="F61" s="5">
+        <f>SUM(C61:E61)</f>
+        <v>3.2772999999999997E-2</v>
+      </c>
+      <c r="G61" s="14">
+        <f t="shared" ref="G61" si="13">SUM(H61:J61)</f>
+        <v>1.7989E-3</v>
+      </c>
+      <c r="H61" s="5">
+        <v>1.7600000000000001E-3</v>
+      </c>
+      <c r="I61" s="5">
+        <v>1.6699999999999999E-5</v>
+      </c>
+      <c r="J61" s="5">
+        <v>2.2200000000000001E-5</v>
       </c>
       <c r="L61" s="11">
         <f>L40</f>
@@ -2863,21 +2884,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView topLeftCell="A26" zoomScale="101" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60"/>
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="3" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -2894,7 +2915,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2902,7 +2923,7 @@
       <c r="C2" s="2"/>
       <c r="D2" s="4"/>
     </row>
-    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -2912,7 +2933,7 @@
       <c r="C3" s="2"/>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2926,7 +2947,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2940,7 +2961,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -2954,7 +2975,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -2965,7 +2986,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -2973,7 +2994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -2981,7 +3002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -2995,7 +3016,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -3010,7 +3031,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -3025,7 +3046,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -3034,7 +3055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -3045,7 +3066,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -3056,7 +3077,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -3067,7 +3088,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -3081,7 +3102,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -3092,7 +3113,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -3103,7 +3124,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -3114,7 +3135,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -3122,7 +3143,7 @@
         <v>2.66E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>67</v>
       </c>
@@ -3134,7 +3155,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -3145,7 +3166,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -3156,7 +3177,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>44</v>
       </c>
@@ -3167,7 +3188,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>45</v>
       </c>
@@ -3175,7 +3196,7 @@
         <v>1.03</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>46</v>
       </c>
@@ -3183,7 +3204,7 @@
         <v>1.5299999999999999E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>47</v>
       </c>
@@ -3191,7 +3212,7 @@
         <v>1.03E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>48</v>
       </c>
@@ -3199,12 +3220,12 @@
         <v>1.9699999999999999E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>50</v>
       </c>
@@ -3212,7 +3233,7 @@
         <v>1.7000000000000001E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>51</v>
       </c>
@@ -3220,7 +3241,7 @@
         <v>0.58499999999999996</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>52</v>
       </c>
@@ -3228,7 +3249,7 @@
         <v>0.58599999999999997</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>53</v>
       </c>
@@ -3236,7 +3257,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>54</v>
       </c>
@@ -3244,7 +3265,7 @@
         <v>0.81399999999999995</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>61</v>
       </c>
@@ -3252,7 +3273,7 @@
         <v>2.3300000000000001E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>64</v>
       </c>
@@ -3263,7 +3284,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>63</v>
       </c>
@@ -3271,7 +3292,7 @@
         <v>4.57E-4</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>68</v>
       </c>
@@ -3280,7 +3301,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>69</v>
       </c>
@@ -3288,7 +3309,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>70</v>
       </c>
@@ -3296,7 +3317,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>78</v>
       </c>
@@ -3305,7 +3326,7 @@
         <v>4.54</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>79</v>
       </c>
@@ -3314,7 +3335,7 @@
         <v>4.54</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>80</v>
       </c>
@@ -3322,7 +3343,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>81</v>
       </c>
@@ -3330,7 +3351,7 @@
         <v>2.7799999999999999E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>82</v>
       </c>
@@ -3338,7 +3359,7 @@
         <v>4.8700000000000002E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>85</v>
       </c>
@@ -3346,7 +3367,7 @@
         <v>3.0299999999999999E-4</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>86</v>
       </c>
@@ -3354,7 +3375,7 @@
         <v>1.2199999999999999E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>87</v>
       </c>
@@ -3362,7 +3383,7 @@
         <v>2.4199999999999999E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>88</v>
       </c>
@@ -3370,7 +3391,7 @@
         <v>1.0300000000000001E-6</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>89</v>
       </c>
@@ -3378,7 +3399,7 @@
         <v>2.2499999999999999E-4</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>99</v>
       </c>
@@ -3386,7 +3407,7 @@
         <v>3.2499999999999997E-5</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>90</v>
       </c>
@@ -3394,7 +3415,7 @@
         <v>6.2E-4</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>91</v>
       </c>
@@ -3402,7 +3423,7 @@
         <v>1.7699999999999999E-4</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>92</v>
       </c>
@@ -3410,7 +3431,7 @@
         <v>4.88E-5</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>94</v>
       </c>
@@ -3418,7 +3439,7 @@
         <v>5.71E-4</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>93</v>
       </c>
@@ -3426,7 +3447,7 @@
         <v>1.7899999999999999E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>100</v>
       </c>
@@ -3434,7 +3455,7 @@
         <v>5.5799999999999999E-6</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>101</v>
       </c>
@@ -3442,13 +3463,12 @@
         <v>9.7100000000000002E-5</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="16" t="s">
         <v>103</v>
       </c>
       <c r="B60">
-        <f>B39</f>
-        <v>1.81</v>
+        <v>1.65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added upstream for alloy
</commit_message>
<xml_diff>
--- a/data/shared/upstream.xlsx
+++ b/data/shared/upstream.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\setanzer\GitHub\BlackBlox\data\shared\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/shared/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB3F3CF5-F935-C145-83E3-3E42D1DEE9A3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
+    <workbookView xWindow="10040" yWindow="460" windowWidth="15920" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="emissions" sheetId="1" r:id="rId1"/>
     <sheet name="removals" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,12 +32,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="C9" authorId="0" shapeId="0">
+    <comment ref="C9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -74,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="109">
   <si>
     <t>meta-notes</t>
   </si>
@@ -358,9 +359,6 @@
     <t>lime factory use</t>
   </si>
   <si>
-    <t>BOF use - no alloy</t>
-  </si>
-  <si>
     <t>factory CO2</t>
   </si>
   <si>
@@ -386,12 +384,30 @@
   </si>
   <si>
     <t>dry cleft timber</t>
+  </si>
+  <si>
+    <t>BOF use + low alloy</t>
+  </si>
+  <si>
+    <t>charcoal kiln use</t>
+  </si>
+  <si>
+    <t>low alloy</t>
+  </si>
+  <si>
+    <t>no alloy</t>
+  </si>
+  <si>
+    <t>chromium alloy</t>
+  </si>
+  <si>
+    <t>BOF use - low alloy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
@@ -796,31 +812,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O61"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H43" sqref="H43"/>
+      <selection pane="bottomRight" activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" style="11" customWidth="1"/>
-    <col min="3" max="4" width="12.7109375" style="5" customWidth="1"/>
-    <col min="5" max="6" width="10.85546875" style="5" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" style="14" customWidth="1"/>
-    <col min="8" max="9" width="12.7109375" style="5" customWidth="1"/>
-    <col min="10" max="10" width="8.7109375" style="5" customWidth="1"/>
-    <col min="11" max="12" width="9.85546875" style="5" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" style="11" customWidth="1"/>
+    <col min="3" max="4" width="12.6640625" style="5" customWidth="1"/>
+    <col min="5" max="6" width="10.83203125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="14" customWidth="1"/>
+    <col min="8" max="9" width="12.6640625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="8.6640625" style="5" customWidth="1"/>
+    <col min="11" max="12" width="9.83203125" style="5" customWidth="1"/>
     <col min="13" max="13" width="11" style="5" customWidth="1"/>
-    <col min="14" max="14" width="8.85546875" style="5"/>
+    <col min="14" max="14" width="8.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -837,7 +853,7 @@
         <v>77</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G1" s="15" t="s">
         <v>83</v>
@@ -855,7 +871,7 @@
         <v>74</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>75</v>
@@ -867,7 +883,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -881,7 +897,7 @@
       <c r="I2" s="4"/>
       <c r="N2" s="4"/>
     </row>
-    <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -916,7 +932,7 @@
       <c r="L3" s="4"/>
       <c r="N3" s="4"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -962,7 +978,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1008,7 +1024,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1048,7 +1064,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1070,7 +1086,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1080,7 +1096,7 @@
       </c>
       <c r="M8" s="9"/>
     </row>
-    <row r="9" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1100,7 +1116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1142,7 +1158,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -1187,7 +1203,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1237,7 +1253,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1267,7 +1283,7 @@
       </c>
       <c r="M13" s="9"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -1283,7 +1299,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -1299,7 +1315,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>26</v>
       </c>
@@ -1312,7 +1328,7 @@
       </c>
       <c r="M16" s="9"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -1357,7 +1373,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -1396,7 +1412,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -1438,7 +1454,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -1468,7 +1484,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -1492,7 +1508,7 @@
         <v>1.0010190863309352</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>67</v>
       </c>
@@ -1536,7 +1552,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -1578,7 +1594,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1628,7 +1644,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>66</v>
       </c>
@@ -1670,7 +1686,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>44</v>
       </c>
@@ -1712,7 +1728,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>45</v>
       </c>
@@ -1732,7 +1748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>46</v>
       </c>
@@ -1762,7 +1778,7 @@
         <v>1.0001182585475181</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>47</v>
       </c>
@@ -1792,7 +1808,7 @@
         <v>1.0001116803278687</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>48</v>
       </c>
@@ -1822,7 +1838,7 @@
         <v>1.0001250342246966</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>50</v>
       </c>
@@ -1858,7 +1874,7 @@
         <v>1.1787276488699383</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>61</v>
       </c>
@@ -1888,7 +1904,7 @@
         <v>1.1523149656274791</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>51</v>
       </c>
@@ -1930,7 +1946,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>52</v>
       </c>
@@ -1972,7 +1988,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>53</v>
       </c>
@@ -2017,7 +2033,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>54</v>
       </c>
@@ -2062,7 +2078,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>59</v>
       </c>
@@ -2107,7 +2123,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>62</v>
       </c>
@@ -2155,7 +2171,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>73</v>
       </c>
@@ -2203,7 +2219,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>68</v>
       </c>
@@ -2249,7 +2265,7 @@
         <v>1.0781403040534712</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>69</v>
       </c>
@@ -2269,7 +2285,7 @@
         <v>2.7169539999999999E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>70</v>
       </c>
@@ -2289,7 +2305,7 @@
         <v>0.13584769999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>78</v>
       </c>
@@ -2310,7 +2326,7 @@
         <v>0.7652392751948599</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>79</v>
       </c>
@@ -2323,7 +2339,7 @@
         <v>1.1457392000000002</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>80</v>
       </c>
@@ -2358,7 +2374,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>81</v>
       </c>
@@ -2393,12 +2409,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>82</v>
       </c>
       <c r="B47" s="11">
-        <f t="shared" ref="B47:B60" si="9">SUM(C47:E47)</f>
+        <f t="shared" ref="B47" si="9">SUM(C47:E47)</f>
         <v>0.12100999999999999</v>
       </c>
       <c r="C47" s="5">
@@ -2427,7 +2443,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>85</v>
       </c>
@@ -2459,7 +2475,7 @@
         <v>1.0599427000000002E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>86</v>
       </c>
@@ -2490,9 +2506,9 @@
         <v>1.8145939999999999E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="C50" s="5">
         <v>0.505</v>
@@ -2521,7 +2537,7 @@
         <v>5.4999899999999997E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>88</v>
       </c>
@@ -2552,7 +2568,7 @@
         <v>6.6999509999999995E-6</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>89</v>
       </c>
@@ -2583,9 +2599,9 @@
         <v>8.1044649999999999E-4</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C53" s="5">
         <v>9.8900000000000008E-4</v>
@@ -2614,7 +2630,7 @@
         <v>1.1458618999999999E-4</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>90</v>
       </c>
@@ -2645,7 +2661,7 @@
         <v>3.3639717000000001E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>91</v>
       </c>
@@ -2676,7 +2692,7 @@
         <v>8.7928850000000005E-4</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>92</v>
       </c>
@@ -2707,9 +2723,9 @@
         <v>5.8874445999999988E-4</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C57" s="5">
         <v>1.43E-2</v>
@@ -2738,9 +2754,9 @@
         <v>5.9562840000000009E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C58" s="5">
         <v>5.4299999999999999E-3</v>
@@ -2769,9 +2785,9 @@
         <v>5.3051600000000008E-4</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C59" s="5">
         <v>1.2400000000000001E-4</v>
@@ -2800,12 +2816,12 @@
         <v>4.2616869999999996E-4</v>
       </c>
       <c r="O59" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C60" s="5">
         <v>2.12E-4</v>
@@ -2834,15 +2850,15 @@
         <v>9.6601144999999995E-4</v>
       </c>
       <c r="O60" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A61" s="16" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A61" s="16" t="s">
-        <v>103</v>
-      </c>
       <c r="B61" s="11">
-        <f t="shared" ref="B61" si="12">SUM(C61:E61)</f>
+        <f t="shared" ref="B61:B65" si="12">SUM(C61:E61)</f>
         <v>3.2772999999999997E-2</v>
       </c>
       <c r="C61" s="5">
@@ -2859,7 +2875,7 @@
         <v>3.2772999999999997E-2</v>
       </c>
       <c r="G61" s="14">
-        <f t="shared" ref="G61" si="13">SUM(H61:J61)</f>
+        <f t="shared" ref="G61:G65" si="13">SUM(H61:J61)</f>
         <v>1.7989E-3</v>
       </c>
       <c r="H61" s="5">
@@ -2874,6 +2890,106 @@
       <c r="L61" s="11">
         <f>L40</f>
         <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>106</v>
+      </c>
+      <c r="B63" s="11">
+        <f>SUM(C63:E63)</f>
+        <v>5.4908799999999994E-2</v>
+      </c>
+      <c r="C63" s="5">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="D63" s="5">
+        <v>2.8700000000000002E-3</v>
+      </c>
+      <c r="E63" s="7">
+        <v>3.8800000000000001E-5</v>
+      </c>
+      <c r="G63" s="14">
+        <f t="shared" si="13"/>
+        <v>5.7666219999999999E-3</v>
+      </c>
+      <c r="H63" s="5">
+        <f>0.00572</f>
+        <v>5.7200000000000003E-3</v>
+      </c>
+      <c r="I63" s="5">
+        <f>0.0000465</f>
+        <v>4.6499999999999999E-5</v>
+      </c>
+      <c r="J63" s="7">
+        <v>1.2200000000000001E-7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>107</v>
+      </c>
+      <c r="B64" s="11">
+        <f t="shared" si="12"/>
+        <v>3.51464</v>
+      </c>
+      <c r="C64" s="5">
+        <v>3.33</v>
+      </c>
+      <c r="D64" s="5">
+        <v>0.182</v>
+      </c>
+      <c r="E64" s="5">
+        <v>2.64E-3</v>
+      </c>
+      <c r="G64" s="14">
+        <f t="shared" si="13"/>
+        <v>0.36993814999999997</v>
+      </c>
+      <c r="H64" s="5">
+        <v>0.36699999999999999</v>
+      </c>
+      <c r="I64" s="5">
+        <v>2.9299999999999999E-3</v>
+      </c>
+      <c r="J64" s="7">
+        <v>8.1499999999999999E-6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>105</v>
+      </c>
+      <c r="B65" s="11">
+        <f t="shared" si="12"/>
+        <v>0.51764999999999994</v>
+      </c>
+      <c r="C65" s="5">
+        <v>0.49099999999999999</v>
+      </c>
+      <c r="D65" s="5">
+        <v>2.6200000000000001E-2</v>
+      </c>
+      <c r="E65" s="5">
+        <v>4.4999999999999999E-4</v>
+      </c>
+      <c r="G65" s="14">
+        <f t="shared" si="13"/>
+        <v>5.4393850000000001E-2</v>
+      </c>
+      <c r="H65" s="5">
+        <v>5.3900000000000003E-2</v>
+      </c>
+      <c r="I65" s="5">
+        <v>4.9200000000000003E-4</v>
+      </c>
+      <c r="J65" s="7">
+        <v>1.8500000000000001E-6</v>
       </c>
     </row>
   </sheetData>
@@ -2884,21 +3000,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E60"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScale="101" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView topLeftCell="A25" zoomScale="101" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="3" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -2906,7 +3022,7 @@
         <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>12</v>
@@ -2915,7 +3031,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2923,7 +3039,7 @@
       <c r="C2" s="2"/>
       <c r="D2" s="4"/>
     </row>
-    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -2933,7 +3049,7 @@
       <c r="C3" s="2"/>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2947,7 +3063,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2961,7 +3077,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -2975,7 +3091,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -2986,7 +3102,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -2994,7 +3110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -3002,7 +3118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -3016,7 +3132,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -3031,7 +3147,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -3046,7 +3162,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -3055,7 +3171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -3066,7 +3182,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -3077,7 +3193,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -3088,7 +3204,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -3102,7 +3218,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -3113,7 +3229,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -3124,7 +3240,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -3135,7 +3251,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -3143,7 +3259,7 @@
         <v>2.66E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>67</v>
       </c>
@@ -3155,7 +3271,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -3166,7 +3282,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -3177,7 +3293,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>44</v>
       </c>
@@ -3188,7 +3304,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>45</v>
       </c>
@@ -3196,7 +3312,7 @@
         <v>1.03</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>46</v>
       </c>
@@ -3204,7 +3320,7 @@
         <v>1.5299999999999999E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>47</v>
       </c>
@@ -3212,7 +3328,7 @@
         <v>1.03E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>48</v>
       </c>
@@ -3220,12 +3336,12 @@
         <v>1.9699999999999999E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>50</v>
       </c>
@@ -3233,7 +3349,7 @@
         <v>1.7000000000000001E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>51</v>
       </c>
@@ -3241,7 +3357,7 @@
         <v>0.58499999999999996</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>52</v>
       </c>
@@ -3249,7 +3365,7 @@
         <v>0.58599999999999997</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>53</v>
       </c>
@@ -3257,7 +3373,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>54</v>
       </c>
@@ -3265,7 +3381,7 @@
         <v>0.81399999999999995</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>61</v>
       </c>
@@ -3273,7 +3389,7 @@
         <v>2.3300000000000001E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>64</v>
       </c>
@@ -3284,7 +3400,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>63</v>
       </c>
@@ -3292,7 +3408,7 @@
         <v>4.57E-4</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>68</v>
       </c>
@@ -3301,7 +3417,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>69</v>
       </c>
@@ -3309,7 +3425,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>70</v>
       </c>
@@ -3317,7 +3433,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>78</v>
       </c>
@@ -3326,7 +3442,7 @@
         <v>4.54</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>79</v>
       </c>
@@ -3335,7 +3451,7 @@
         <v>4.54</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>80</v>
       </c>
@@ -3343,7 +3459,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>81</v>
       </c>
@@ -3351,7 +3467,7 @@
         <v>2.7799999999999999E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>82</v>
       </c>
@@ -3359,7 +3475,7 @@
         <v>4.8700000000000002E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>85</v>
       </c>
@@ -3367,7 +3483,7 @@
         <v>3.0299999999999999E-4</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>86</v>
       </c>
@@ -3375,15 +3491,15 @@
         <v>1.2199999999999999E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
       <c r="C49">
         <v>2.4199999999999999E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>88</v>
       </c>
@@ -3391,7 +3507,7 @@
         <v>1.0300000000000001E-6</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>89</v>
       </c>
@@ -3399,15 +3515,15 @@
         <v>2.2499999999999999E-4</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C52" s="8">
         <v>3.2499999999999997E-5</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>90</v>
       </c>
@@ -3415,7 +3531,7 @@
         <v>6.2E-4</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>91</v>
       </c>
@@ -3423,7 +3539,7 @@
         <v>1.7699999999999999E-4</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>92</v>
       </c>
@@ -3431,15 +3547,15 @@
         <v>4.88E-5</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C56" s="8">
         <v>5.71E-4</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>93</v>
       </c>
@@ -3447,28 +3563,52 @@
         <v>1.7899999999999999E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C58" s="8">
         <v>5.5799999999999999E-6</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C59" s="8">
         <v>9.7100000000000002E-5</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B60">
         <v>1.65</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>106</v>
+      </c>
+      <c r="B61">
+        <v>2.5500000000000002E-3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>107</v>
+      </c>
+      <c r="B62">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>105</v>
+      </c>
+      <c r="B63">
+        <v>2.3699999999999999E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
blank sheets for ecoinvent 3.5
</commit_message>
<xml_diff>
--- a/data/shared/upstream.xlsx
+++ b/data/shared/upstream.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/shared/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\BlackBlox\data\shared\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A9C349-4BFC-444A-A676-4705FA3182D9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
   </bookViews>
   <sheets>
     <sheet name="emissions" sheetId="3" r:id="rId1"/>
     <sheet name="removals" sheetId="2" r:id="rId2"/>
+    <sheet name="emissions3.5" sheetId="4" r:id="rId3"/>
+    <sheet name="removals3.5" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -394,7 +395,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
@@ -789,16 +790,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E004197-C2FA-1848-902A-BAAA9C3812C9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="44.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -848,7 +852,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -866,7 +870,7 @@
       <c r="M2" s="5"/>
       <c r="N2" s="4"/>
     </row>
-    <row r="3" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -902,7 +906,7 @@
       <c r="M3" s="5"/>
       <c r="N3" s="4"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>102</v>
       </c>
@@ -941,7 +945,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>26</v>
       </c>
@@ -967,7 +971,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -991,7 +995,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
       <c r="M6" s="9">
-        <f>K6/B6</f>
+        <f t="shared" ref="M6:M16" si="0">K6/B6</f>
         <v>0</v>
       </c>
       <c r="N6" s="5"/>
@@ -999,7 +1003,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>53</v>
       </c>
@@ -1031,12 +1035,12 @@
         <v>1.3999999999999999E-4</v>
       </c>
       <c r="K7" s="5">
-        <f>SUM(C7:J7)</f>
+        <f t="shared" ref="K7:K16" si="1">SUM(C7:J7)</f>
         <v>4.1085400000000001E-2</v>
       </c>
       <c r="L7" s="5"/>
       <c r="M7" s="9">
-        <f>K7/B7</f>
+        <f t="shared" si="0"/>
         <v>1.0858237750409641</v>
       </c>
       <c r="N7" s="5" t="s">
@@ -1049,7 +1053,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>69</v>
       </c>
@@ -1068,12 +1072,12 @@
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
       <c r="K8" s="5">
-        <f>SUM(C8:J8)</f>
+        <f t="shared" si="1"/>
         <v>1.6236999999999998E-3</v>
       </c>
       <c r="L8" s="5"/>
       <c r="M8" s="9">
-        <f>K8/B8</f>
+        <f t="shared" si="0"/>
         <v>3.2473999999999997E-3</v>
       </c>
       <c r="N8" s="5"/>
@@ -1081,7 +1085,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>70</v>
       </c>
@@ -1100,12 +1104,12 @@
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5">
-        <f>SUM(C9:J9)</f>
+        <f t="shared" si="1"/>
         <v>1.6236999999999998E-3</v>
       </c>
       <c r="L9" s="5"/>
       <c r="M9" s="9">
-        <f>K9/B9</f>
+        <f t="shared" si="0"/>
         <v>1.6236999999999998E-2</v>
       </c>
       <c r="N9" s="5"/>
@@ -1113,12 +1117,12 @@
         <v>113</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>68</v>
       </c>
       <c r="B10" s="11">
-        <f>SUM(C10:E10)</f>
+        <f t="shared" ref="B10:B16" si="2">SUM(C10:E10)</f>
         <v>0.34770199999999996</v>
       </c>
       <c r="C10" s="5">
@@ -1145,12 +1149,12 @@
         <v>9.7699999999999996E-6</v>
       </c>
       <c r="K10" s="5">
-        <f>SUM(C10:J10)</f>
+        <f t="shared" si="1"/>
         <v>0.37487154</v>
       </c>
       <c r="L10" s="5"/>
       <c r="M10" s="9">
-        <f>K10/B10</f>
+        <f t="shared" si="0"/>
         <v>1.0781403040534712</v>
       </c>
       <c r="N10" s="5" t="s">
@@ -1163,12 +1167,12 @@
         <v>113</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>40</v>
       </c>
       <c r="B11" s="11">
-        <f>SUM(C11:E11)</f>
+        <f t="shared" si="2"/>
         <v>0.13900000000000001</v>
       </c>
       <c r="C11" s="5">
@@ -1185,12 +1189,12 @@
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
       <c r="K11" s="5">
-        <f>SUM(C11:J11)</f>
+        <f t="shared" si="1"/>
         <v>0.1407989</v>
       </c>
       <c r="L11" s="5"/>
       <c r="M11" s="9">
-        <f>K11/B11</f>
+        <f t="shared" si="0"/>
         <v>1.0129417266187051</v>
       </c>
       <c r="N11" s="5"/>
@@ -1198,12 +1202,12 @@
         <v>114</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>43</v>
       </c>
       <c r="B12" s="11">
-        <f>SUM(C12:E12)</f>
+        <f t="shared" si="2"/>
         <v>2.6087599999999997</v>
       </c>
       <c r="C12" s="5">
@@ -1217,7 +1221,7 @@
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="14">
-        <f>SUM(H12:J12)</f>
+        <f t="shared" ref="G12:G23" si="3">SUM(H12:J12)</f>
         <v>0.38169149999999996</v>
       </c>
       <c r="H12" s="5">
@@ -1230,12 +1234,12 @@
         <v>5.1499999999999998E-5</v>
       </c>
       <c r="K12" s="5">
-        <f>SUM(C12:J12)</f>
+        <f t="shared" si="1"/>
         <v>3.3721429999999999</v>
       </c>
       <c r="L12" s="5"/>
       <c r="M12" s="9">
-        <f>K12/B12</f>
+        <f t="shared" si="0"/>
         <v>1.2926229319676783</v>
       </c>
       <c r="N12" s="5" t="s">
@@ -1245,12 +1249,12 @@
         <v>114</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>41</v>
       </c>
       <c r="B13" s="11">
-        <f>SUM(C13:E13)</f>
+        <f t="shared" si="2"/>
         <v>0.76161899999999993</v>
       </c>
       <c r="C13" s="5">
@@ -1264,7 +1268,7 @@
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="14">
-        <f>SUM(H13:J13)</f>
+        <f t="shared" si="3"/>
         <v>7.951859E-2</v>
       </c>
       <c r="H13" s="5">
@@ -1277,12 +1281,12 @@
         <v>2.5900000000000002E-6</v>
       </c>
       <c r="K13" s="5">
-        <f>SUM(C13:J13)</f>
+        <f t="shared" si="1"/>
         <v>0.92065617999999994</v>
       </c>
       <c r="L13" s="5"/>
       <c r="M13" s="9">
-        <f>K13/B13</f>
+        <f t="shared" si="0"/>
         <v>1.2088146172823946</v>
       </c>
       <c r="N13" s="5" t="s">
@@ -1295,12 +1299,12 @@
         <v>114</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
       <c r="B14" s="11">
-        <f>SUM(C14:E14)</f>
+        <f t="shared" si="2"/>
         <v>2.6330450000000001</v>
       </c>
       <c r="C14" s="5">
@@ -1317,7 +1321,7 @@
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="14">
-        <f>SUM(H14:J14)</f>
+        <f t="shared" si="3"/>
         <v>0.7706965400000001</v>
       </c>
       <c r="H14" s="5">
@@ -1332,12 +1336,12 @@
         <v>5.0099999999999998E-5</v>
       </c>
       <c r="K14" s="5">
-        <f>SUM(C14:J14)</f>
+        <f t="shared" si="1"/>
         <v>4.1744380800000007</v>
       </c>
       <c r="L14" s="5"/>
       <c r="M14" s="9">
-        <f>K14/B14</f>
+        <f t="shared" si="0"/>
         <v>1.5854032422537407</v>
       </c>
       <c r="N14" s="5" t="s">
@@ -1350,12 +1354,12 @@
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>66</v>
       </c>
       <c r="B15" s="11">
-        <f>SUM(C15:E15)</f>
+        <f t="shared" si="2"/>
         <v>2.6064400000000001</v>
       </c>
       <c r="C15" s="5">
@@ -1369,7 +1373,7 @@
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="14">
-        <f>SUM(H15:J15)</f>
+        <f t="shared" si="3"/>
         <v>0.35369009999999995</v>
       </c>
       <c r="H15" s="5">
@@ -1382,12 +1386,12 @@
         <v>5.0099999999999998E-5</v>
       </c>
       <c r="K15" s="5">
-        <f>SUM(C15:J15)</f>
+        <f t="shared" si="1"/>
         <v>3.3138202000000003</v>
       </c>
       <c r="L15" s="5"/>
       <c r="M15" s="9">
-        <f>K15/B15</f>
+        <f t="shared" si="0"/>
         <v>1.2713970780067834</v>
       </c>
       <c r="N15" s="5" t="s">
@@ -1397,12 +1401,12 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>44</v>
       </c>
       <c r="B16" s="11">
-        <f>SUM(C16:E16)</f>
+        <f t="shared" si="2"/>
         <v>1.9883300000000002</v>
       </c>
       <c r="C16" s="5">
@@ -1416,7 +1420,7 @@
       </c>
       <c r="F16" s="5"/>
       <c r="G16" s="14">
-        <f>SUM(H16:J16)</f>
+        <f t="shared" si="3"/>
         <v>0.40600280000000005</v>
       </c>
       <c r="H16" s="5">
@@ -1429,12 +1433,12 @@
         <v>3.8E-6</v>
       </c>
       <c r="K16" s="5">
-        <f>SUM(C16:J16)</f>
+        <f t="shared" si="1"/>
         <v>2.8003356000000004</v>
       </c>
       <c r="L16" s="5"/>
       <c r="M16" s="10">
-        <f>K16/B16</f>
+        <f t="shared" si="0"/>
         <v>1.4083857307388614</v>
       </c>
       <c r="N16" s="5" t="s">
@@ -1444,7 +1448,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -1456,7 +1460,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="14">
-        <f>SUM(H17:J17)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H17" s="5"/>
@@ -1472,7 +1476,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -1489,7 +1493,7 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="14">
-        <f>SUM(H18:J18)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H18" s="5">
@@ -1510,7 +1514,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -1522,7 +1526,7 @@
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="14">
-        <f>SUM(H19:J19)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H19" s="5"/>
@@ -1538,7 +1542,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>81</v>
       </c>
@@ -1557,7 +1561,7 @@
       </c>
       <c r="F20" s="5"/>
       <c r="G20" s="14">
-        <f>SUM(H20:J20)</f>
+        <f t="shared" si="3"/>
         <v>5.5818774028000007E-2</v>
       </c>
       <c r="H20" s="7">
@@ -1580,7 +1584,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>80</v>
       </c>
@@ -1599,7 +1603,7 @@
       </c>
       <c r="F21" s="5"/>
       <c r="G21" s="14">
-        <f>SUM(H21:J21)</f>
+        <f t="shared" si="3"/>
         <v>9.0642799999999992E-3</v>
       </c>
       <c r="H21" s="5">
@@ -1622,7 +1626,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -1641,7 +1645,7 @@
       </c>
       <c r="F22" s="5"/>
       <c r="G22" s="14">
-        <f>SUM(H22:J22)</f>
+        <f t="shared" si="3"/>
         <v>1.02159</v>
       </c>
       <c r="H22" s="5"/>
@@ -1667,7 +1671,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>2</v>
       </c>
@@ -1687,7 +1691,7 @@
       </c>
       <c r="F23" s="5"/>
       <c r="G23" s="14">
-        <f>SUM(H23:J23)</f>
+        <f t="shared" si="3"/>
         <v>1.1457392000000002</v>
       </c>
       <c r="H23" s="5">
@@ -1718,7 +1722,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>79</v>
       </c>
@@ -1745,7 +1749,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>78</v>
       </c>
@@ -1770,7 +1774,7 @@
       </c>
       <c r="L25" s="5"/>
       <c r="M25" s="9">
-        <f>K25/B25</f>
+        <f t="shared" ref="M25:M32" si="4">K25/B25</f>
         <v>2</v>
       </c>
       <c r="N25" s="5"/>
@@ -1778,12 +1782,12 @@
         <v>111</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>3</v>
       </c>
       <c r="B26" s="11">
-        <f>SUM(C26:E26)</f>
+        <f t="shared" ref="B26:B32" si="5">SUM(C26:E26)</f>
         <v>0.241614</v>
       </c>
       <c r="C26" s="5">
@@ -1816,7 +1820,7 @@
       </c>
       <c r="L26" s="5"/>
       <c r="M26" s="10">
-        <f>K26/B26</f>
+        <f t="shared" si="4"/>
         <v>3.5666724610328875</v>
       </c>
       <c r="N26" s="5" t="s">
@@ -1829,12 +1833,12 @@
         <v>111</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>4</v>
       </c>
       <c r="B27" s="11">
-        <f>SUM(C27:E27)</f>
+        <f t="shared" si="5"/>
         <v>0.24137999999999998</v>
       </c>
       <c r="C27" s="5">
@@ -1863,7 +1867,7 @@
       </c>
       <c r="L27" s="5"/>
       <c r="M27" s="10">
-        <f>K27/B27</f>
+        <f t="shared" si="4"/>
         <v>3.569082774049217</v>
       </c>
       <c r="N27" s="5" t="s">
@@ -1876,12 +1880,12 @@
         <v>111</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>32</v>
       </c>
       <c r="B28" s="11">
-        <f>SUM(C28:E28)</f>
+        <f t="shared" si="5"/>
         <v>2.6605E-2</v>
       </c>
       <c r="C28" s="5">
@@ -1913,7 +1917,7 @@
       </c>
       <c r="L28" s="5"/>
       <c r="M28" s="10">
-        <f>K28/B28</f>
+        <f t="shared" si="4"/>
         <v>32.348121781619994</v>
       </c>
       <c r="N28" s="5" t="s">
@@ -1923,12 +1927,12 @@
         <v>111</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>5</v>
       </c>
       <c r="B29" s="11">
-        <f>SUM(C29:E29)</f>
+        <f t="shared" si="5"/>
         <v>0.35599999999999998</v>
       </c>
       <c r="C29" s="5">
@@ -1946,7 +1950,7 @@
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
       <c r="M29" s="9">
-        <f>K29/B29</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N29" s="5" t="s">
@@ -1956,12 +1960,12 @@
         <v>111</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>38</v>
       </c>
       <c r="B30" s="11">
-        <f>SUM(C30:E30)</f>
+        <f t="shared" si="5"/>
         <v>0.32052000000000003</v>
       </c>
       <c r="C30" s="5">
@@ -1985,7 +1989,7 @@
       </c>
       <c r="L30" s="5"/>
       <c r="M30" s="9">
-        <f>K30/B30</f>
+        <f t="shared" si="4"/>
         <v>2.1034883938599775</v>
       </c>
       <c r="N30" s="5"/>
@@ -1996,12 +2000,12 @@
         <v>111</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>51</v>
       </c>
       <c r="B31" s="11">
-        <f>SUM(C31:E31)</f>
+        <f t="shared" si="5"/>
         <v>0.3342</v>
       </c>
       <c r="C31" s="5">
@@ -2031,7 +2035,7 @@
       </c>
       <c r="L31" s="5"/>
       <c r="M31" s="9">
-        <f>K31/B31</f>
+        <f t="shared" si="4"/>
         <v>1.0133763614602034</v>
       </c>
       <c r="N31" s="5" t="s">
@@ -2044,12 +2048,12 @@
         <v>111</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>52</v>
       </c>
       <c r="B32" s="11">
-        <f>SUM(C32:E32)</f>
+        <f t="shared" si="5"/>
         <v>0.37089999999999995</v>
       </c>
       <c r="C32" s="5">
@@ -2079,7 +2083,7 @@
       </c>
       <c r="L32" s="5"/>
       <c r="M32" s="9">
-        <f>K32/B32</f>
+        <f t="shared" si="4"/>
         <v>1.0161767053114048</v>
       </c>
       <c r="N32" s="5" t="s">
@@ -2092,7 +2096,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>89</v>
       </c>
@@ -2107,7 +2111,7 @@
         <v>1.0499999999999999E-5</v>
       </c>
       <c r="F33" s="11">
-        <f>SUM(C33:E33)</f>
+        <f t="shared" ref="F33:F46" si="6">SUM(C33:E33)</f>
         <v>1.9099500000000002E-2</v>
       </c>
       <c r="G33" s="14"/>
@@ -2131,7 +2135,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>87</v>
       </c>
@@ -2146,7 +2150,7 @@
         <v>7.5800000000000003E-6</v>
       </c>
       <c r="F34" s="11">
-        <f>SUM(C34:E34)</f>
+        <f t="shared" si="6"/>
         <v>1.4915580000000001E-2</v>
       </c>
       <c r="G34" s="14"/>
@@ -2170,7 +2174,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>103</v>
       </c>
@@ -2185,7 +2189,7 @@
         <v>4.5800000000000002E-4</v>
       </c>
       <c r="F35" s="11">
-        <f>SUM(C35:E35)</f>
+        <f t="shared" si="6"/>
         <v>0.53225800000000001</v>
       </c>
       <c r="G35" s="14"/>
@@ -2209,7 +2213,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>104</v>
       </c>
@@ -2224,7 +2228,7 @@
         <v>2.0999999999999998E-6</v>
       </c>
       <c r="F36" s="18">
-        <f>SUM(C36:E36)</f>
+        <f t="shared" si="6"/>
         <v>5.0540999999999997E-3</v>
       </c>
       <c r="G36" s="17"/>
@@ -2239,7 +2243,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>92</v>
       </c>
@@ -2254,7 +2258,7 @@
         <v>2.3E-6</v>
       </c>
       <c r="F37" s="11">
-        <f>SUM(C37:E37)</f>
+        <f t="shared" si="6"/>
         <v>5.0114000000000001E-3</v>
       </c>
       <c r="G37" s="14"/>
@@ -2269,7 +2273,7 @@
       </c>
       <c r="K37" s="5"/>
       <c r="L37" s="14">
-        <f>SUM(H37:J37)</f>
+        <f t="shared" ref="L37:L46" si="7">SUM(H37:J37)</f>
         <v>5.8874445999999988E-4</v>
       </c>
       <c r="M37" s="5"/>
@@ -2278,7 +2282,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>86</v>
       </c>
@@ -2293,7 +2297,7 @@
         <v>1.7399999999999999E-5</v>
       </c>
       <c r="F38" s="11">
-        <f>SUM(C38:E38)</f>
+        <f t="shared" si="6"/>
         <v>3.3737400000000001E-2</v>
       </c>
       <c r="G38" s="14"/>
@@ -2308,7 +2312,7 @@
       </c>
       <c r="K38" s="5"/>
       <c r="L38" s="14">
-        <f>SUM(H38:J38)</f>
+        <f t="shared" si="7"/>
         <v>1.8145939999999999E-3</v>
       </c>
       <c r="M38" s="5"/>
@@ -2317,7 +2321,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>99</v>
       </c>
@@ -2332,7 +2336,7 @@
         <v>1.2200000000000001E-7</v>
       </c>
       <c r="F39" s="18">
-        <f>SUM(C39:E39)</f>
+        <f t="shared" si="6"/>
         <v>1.29682E-4</v>
       </c>
       <c r="G39" s="14"/>
@@ -2347,7 +2351,7 @@
       </c>
       <c r="K39" s="5"/>
       <c r="L39" s="5">
-        <f>SUM(H39:J39)</f>
+        <f t="shared" si="7"/>
         <v>4.2616869999999996E-4</v>
       </c>
       <c r="M39" s="5"/>
@@ -2359,7 +2363,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>100</v>
       </c>
@@ -2374,7 +2378,7 @@
         <v>1.8900000000000001E-7</v>
       </c>
       <c r="F40" s="18">
-        <f>SUM(C40:E40)</f>
+        <f t="shared" si="6"/>
         <v>2.2258900000000001E-4</v>
       </c>
       <c r="G40" s="14"/>
@@ -2389,7 +2393,7 @@
       </c>
       <c r="K40" s="5"/>
       <c r="L40" s="5">
-        <f>SUM(H40:J40)</f>
+        <f t="shared" si="7"/>
         <v>9.6601144999999995E-4</v>
       </c>
       <c r="M40" s="5"/>
@@ -2401,7 +2405,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>91</v>
       </c>
@@ -2416,7 +2420,7 @@
         <v>6.9700000000000002E-6</v>
       </c>
       <c r="F41" s="11">
-        <f>SUM(C41:E41)</f>
+        <f t="shared" si="6"/>
         <v>1.2324969999999999E-2</v>
       </c>
       <c r="G41" s="14"/>
@@ -2431,7 +2435,7 @@
       </c>
       <c r="K41" s="5"/>
       <c r="L41" s="14">
-        <f>SUM(H41:J41)</f>
+        <f t="shared" si="7"/>
         <v>8.7928850000000005E-4</v>
       </c>
       <c r="M41" s="5"/>
@@ -2440,7 +2444,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>97</v>
       </c>
@@ -2455,7 +2459,7 @@
         <v>4.8099999999999997E-5</v>
       </c>
       <c r="F42" s="11">
-        <f>SUM(C42:E42)</f>
+        <f t="shared" si="6"/>
         <v>2.5078099999999999E-2</v>
       </c>
       <c r="G42" s="14"/>
@@ -2470,7 +2474,7 @@
       </c>
       <c r="K42" s="5"/>
       <c r="L42" s="14">
-        <f>SUM(H42:J42)</f>
+        <f t="shared" si="7"/>
         <v>5.3051600000000008E-4</v>
       </c>
       <c r="M42" s="5"/>
@@ -2479,7 +2483,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>98</v>
       </c>
@@ -2494,7 +2498,7 @@
         <v>2.1100000000000001E-6</v>
       </c>
       <c r="F43" s="11">
-        <f>SUM(C43:E43)</f>
+        <f t="shared" si="6"/>
         <v>1.0214100000000002E-3</v>
       </c>
       <c r="G43" s="14"/>
@@ -2509,7 +2513,7 @@
       </c>
       <c r="K43" s="5"/>
       <c r="L43" s="14">
-        <f>SUM(H43:J43)</f>
+        <f t="shared" si="7"/>
         <v>1.1458618999999999E-4</v>
       </c>
       <c r="M43" s="5"/>
@@ -2518,7 +2522,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>90</v>
       </c>
@@ -2533,7 +2537,7 @@
         <v>2.4899999999999999E-5</v>
       </c>
       <c r="F44" s="11">
-        <f>SUM(C44:E44)</f>
+        <f t="shared" si="6"/>
         <v>2.17819E-2</v>
       </c>
       <c r="G44" s="14"/>
@@ -2548,7 +2552,7 @@
       </c>
       <c r="K44" s="5"/>
       <c r="L44" s="14">
-        <f>SUM(H44:J44)</f>
+        <f t="shared" si="7"/>
         <v>3.3639717000000001E-3</v>
       </c>
       <c r="M44" s="5"/>
@@ -2557,7 +2561,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>88</v>
       </c>
@@ -2572,7 +2576,7 @@
         <v>5.1200000000000002E-8</v>
       </c>
       <c r="F45" s="11">
-        <f>SUM(C45:E45)</f>
+        <f t="shared" si="6"/>
         <v>7.8016200000000007E-5</v>
       </c>
       <c r="G45" s="14"/>
@@ -2587,7 +2591,7 @@
       </c>
       <c r="K45" s="5"/>
       <c r="L45" s="14">
-        <f>SUM(H45:J45)</f>
+        <f t="shared" si="7"/>
         <v>6.6999509999999995E-6</v>
       </c>
       <c r="M45" s="5"/>
@@ -2596,7 +2600,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>85</v>
       </c>
@@ -2611,7 +2615,7 @@
         <v>1.13E-5</v>
       </c>
       <c r="F46" s="11">
-        <f>SUM(C46:E46)</f>
+        <f t="shared" si="6"/>
         <v>1.1072300000000002E-2</v>
       </c>
       <c r="G46" s="14"/>
@@ -2626,7 +2630,7 @@
       </c>
       <c r="K46" s="7"/>
       <c r="L46" s="14">
-        <f>SUM(H46:J46)</f>
+        <f t="shared" si="7"/>
         <v>1.0599427000000002E-3</v>
       </c>
       <c r="M46" s="5"/>
@@ -2635,12 +2639,12 @@
         <v>118</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>107</v>
       </c>
       <c r="B47" s="11">
-        <f>SUM(C47:E47)</f>
+        <f t="shared" ref="B47:B62" si="8">SUM(C47:E47)</f>
         <v>3.51464</v>
       </c>
       <c r="C47" s="5">
@@ -2654,7 +2658,7 @@
       </c>
       <c r="F47" s="5"/>
       <c r="G47" s="14">
-        <f>SUM(H47:J47)</f>
+        <f t="shared" ref="G47:G62" si="9">SUM(H47:J47)</f>
         <v>0.36993814999999997</v>
       </c>
       <c r="H47" s="5">
@@ -2674,12 +2678,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>82</v>
       </c>
       <c r="B48" s="11">
-        <f>SUM(C48:E48)</f>
+        <f t="shared" si="8"/>
         <v>0.12100999999999999</v>
       </c>
       <c r="C48" s="5">
@@ -2693,7 +2697,7 @@
       </c>
       <c r="F48" s="5"/>
       <c r="G48" s="14">
-        <f>SUM(H48:J48)</f>
+        <f t="shared" si="9"/>
         <v>9.3692799999999989E-3</v>
       </c>
       <c r="H48" s="5">
@@ -2715,12 +2719,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>105</v>
       </c>
       <c r="B49" s="11">
-        <f>SUM(C49:E49)</f>
+        <f t="shared" si="8"/>
         <v>0.51764999999999994</v>
       </c>
       <c r="C49" s="5">
@@ -2734,7 +2738,7 @@
       </c>
       <c r="F49" s="5"/>
       <c r="G49" s="14">
-        <f>SUM(H49:J49)</f>
+        <f t="shared" si="9"/>
         <v>5.4393850000000001E-2</v>
       </c>
       <c r="H49" s="5">
@@ -2750,12 +2754,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>106</v>
       </c>
       <c r="B50" s="11">
-        <f>SUM(C50:E50)</f>
+        <f t="shared" si="8"/>
         <v>5.4908799999999994E-2</v>
       </c>
       <c r="C50" s="5">
@@ -2769,7 +2773,7 @@
       </c>
       <c r="F50" s="14"/>
       <c r="G50" s="14">
-        <f>SUM(H50:J50)</f>
+        <f t="shared" si="9"/>
         <v>5.7666219999999999E-3</v>
       </c>
       <c r="H50" s="5">
@@ -2791,12 +2795,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>61</v>
       </c>
       <c r="B51" s="11">
-        <f>SUM(C51:E51)</f>
+        <f t="shared" si="8"/>
         <v>1.5100289</v>
       </c>
       <c r="C51" s="5">
@@ -2808,7 +2812,7 @@
       </c>
       <c r="F51" s="5"/>
       <c r="G51" s="14">
-        <f>SUM(H51:J51)</f>
+        <f t="shared" si="9"/>
         <v>0.115</v>
       </c>
       <c r="H51" s="5">
@@ -2817,12 +2821,12 @@
       <c r="I51" s="5"/>
       <c r="J51" s="5"/>
       <c r="K51" s="5">
-        <f>SUM(C51:J51)</f>
+        <f t="shared" ref="K51:K62" si="10">SUM(C51:J51)</f>
         <v>1.7400289</v>
       </c>
       <c r="L51" s="5"/>
       <c r="M51" s="9">
-        <f>K51/B51</f>
+        <f t="shared" ref="M51:M62" si="11">K51/B51</f>
         <v>1.1523149656274791</v>
       </c>
       <c r="N51" s="5"/>
@@ -2830,12 +2834,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>48</v>
       </c>
       <c r="B52" s="11">
-        <f>SUM(C52:E52)</f>
+        <f t="shared" si="8"/>
         <v>2.1913999999999998</v>
       </c>
       <c r="C52" s="5">
@@ -2847,7 +2851,7 @@
       <c r="E52" s="5"/>
       <c r="F52" s="5"/>
       <c r="G52" s="14">
-        <f>SUM(H52:J52)</f>
+        <f t="shared" si="9"/>
         <v>1.37E-4</v>
       </c>
       <c r="H52" s="5"/>
@@ -2856,12 +2860,12 @@
       </c>
       <c r="J52" s="5"/>
       <c r="K52" s="5">
-        <f>SUM(C52:J52)</f>
+        <f t="shared" si="10"/>
         <v>2.1916739999999999</v>
       </c>
       <c r="L52" s="5"/>
       <c r="M52" s="9">
-        <f>K52/B52</f>
+        <f t="shared" si="11"/>
         <v>1.0001250342246966</v>
       </c>
       <c r="N52" s="5"/>
@@ -2869,12 +2873,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>47</v>
       </c>
       <c r="B53" s="11">
-        <f>SUM(C53:E53)</f>
+        <f t="shared" si="8"/>
         <v>1.952</v>
       </c>
       <c r="C53" s="5">
@@ -2886,7 +2890,7 @@
       <c r="E53" s="5"/>
       <c r="F53" s="5"/>
       <c r="G53" s="14">
-        <f>SUM(H53:J53)</f>
+        <f t="shared" si="9"/>
         <v>1.0900000000000001E-4</v>
       </c>
       <c r="H53" s="5"/>
@@ -2895,12 +2899,12 @@
       </c>
       <c r="J53" s="5"/>
       <c r="K53" s="5">
-        <f>SUM(C53:J53)</f>
+        <f t="shared" si="10"/>
         <v>1.9522179999999998</v>
       </c>
       <c r="L53" s="5"/>
       <c r="M53" s="9">
-        <f>K53/B53</f>
+        <f t="shared" si="11"/>
         <v>1.0001116803278687</v>
       </c>
       <c r="N53" s="5"/>
@@ -2908,12 +2912,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>46</v>
       </c>
       <c r="B54" s="11">
-        <f>SUM(C54:E54)</f>
+        <f t="shared" si="8"/>
         <v>2.0971000000000002</v>
       </c>
       <c r="C54" s="5">
@@ -2925,7 +2929,7 @@
       <c r="E54" s="5"/>
       <c r="F54" s="5"/>
       <c r="G54" s="14">
-        <f>SUM(H54:J54)</f>
+        <f t="shared" si="9"/>
         <v>1.2400000000000001E-4</v>
       </c>
       <c r="H54" s="5"/>
@@ -2934,12 +2938,12 @@
       </c>
       <c r="J54" s="5"/>
       <c r="K54" s="5">
-        <f>SUM(C54:J54)</f>
+        <f t="shared" si="10"/>
         <v>2.0973480000000002</v>
       </c>
       <c r="L54" s="5"/>
       <c r="M54" s="9">
-        <f>K54/B54</f>
+        <f t="shared" si="11"/>
         <v>1.0001182585475181</v>
       </c>
       <c r="N54" s="5"/>
@@ -2947,12 +2951,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>50</v>
       </c>
       <c r="B55" s="11">
-        <f>SUM(C55:E55)</f>
+        <f t="shared" si="8"/>
         <v>2.05918</v>
       </c>
       <c r="C55" s="5">
@@ -2964,7 +2968,7 @@
       <c r="E55" s="5"/>
       <c r="F55" s="5"/>
       <c r="G55" s="14">
-        <f>SUM(H55:J55)</f>
+        <f t="shared" si="9"/>
         <v>0.18401619999999999</v>
       </c>
       <c r="H55" s="5">
@@ -2977,12 +2981,12 @@
         <v>2.5000000000000002E-6</v>
       </c>
       <c r="K55" s="5">
-        <f>SUM(C55:J55)</f>
+        <f t="shared" si="10"/>
         <v>2.4272123999999997</v>
       </c>
       <c r="L55" s="5"/>
       <c r="M55" s="9">
-        <f>K55/B55</f>
+        <f t="shared" si="11"/>
         <v>1.1787276488699383</v>
       </c>
       <c r="N55" s="5"/>
@@ -2990,12 +2994,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>14</v>
       </c>
       <c r="B56" s="11">
-        <f>SUM(C56:E56)</f>
+        <f t="shared" si="8"/>
         <v>4.8364000000000002E-3</v>
       </c>
       <c r="C56" s="5">
@@ -3007,7 +3011,7 @@
       <c r="E56" s="5"/>
       <c r="F56" s="5"/>
       <c r="G56" s="14">
-        <f>SUM(H56:J56)</f>
+        <f t="shared" si="9"/>
         <v>1.4165299999999999E-4</v>
       </c>
       <c r="H56" s="5">
@@ -3020,12 +3024,12 @@
         <v>5.2999999999999998E-8</v>
       </c>
       <c r="K56" s="5">
-        <f>SUM(C56:J56)</f>
+        <f t="shared" si="10"/>
         <v>5.1197060000000008E-3</v>
       </c>
       <c r="L56" s="5"/>
       <c r="M56" s="9">
-        <f>K56/B56</f>
+        <f t="shared" si="11"/>
         <v>1.0585778678355804</v>
       </c>
       <c r="N56" s="5" t="s">
@@ -3038,12 +3042,12 @@
         <v>110</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>36</v>
       </c>
       <c r="B57" s="11">
-        <f>SUM(C57:E57)</f>
+        <f t="shared" si="8"/>
         <v>5.3398300000000003E-3</v>
       </c>
       <c r="C57" s="5">
@@ -3057,7 +3061,7 @@
       </c>
       <c r="F57" s="5"/>
       <c r="G57" s="14">
-        <f>SUM(H57:J57)</f>
+        <f t="shared" si="9"/>
         <v>2.2085400000000001E-4</v>
       </c>
       <c r="H57" s="5">
@@ -3070,12 +3074,12 @@
         <v>5.4E-8</v>
       </c>
       <c r="K57" s="5">
-        <f>SUM(C57:J57)</f>
+        <f t="shared" si="10"/>
         <v>5.7815380000000001E-3</v>
       </c>
       <c r="L57" s="5"/>
       <c r="M57" s="9">
-        <f>K57/B57</f>
+        <f t="shared" si="11"/>
         <v>1.0827194873245027</v>
       </c>
       <c r="N57" s="5" t="s">
@@ -3088,12 +3092,12 @@
         <v>110</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>17</v>
       </c>
       <c r="B58" s="11">
-        <f>SUM(C58:E58)</f>
+        <f t="shared" si="8"/>
         <v>6.2811700000000012E-2</v>
       </c>
       <c r="C58" s="5">
@@ -3110,7 +3114,7 @@
       </c>
       <c r="F58" s="5"/>
       <c r="G58" s="14">
-        <f>SUM(H58:J58)</f>
+        <f t="shared" si="9"/>
         <v>3.2426277000000002E-5</v>
       </c>
       <c r="H58" s="5">
@@ -3125,12 +3129,12 @@
         <v>5.0000000000000003E-10</v>
       </c>
       <c r="K58" s="5">
-        <f>SUM(C58:J58)</f>
+        <f t="shared" si="10"/>
         <v>6.2876552554000015E-2</v>
       </c>
       <c r="L58" s="5"/>
       <c r="M58" s="9">
-        <f>K58/B58</f>
+        <f t="shared" si="11"/>
         <v>1.0010324916217839</v>
       </c>
       <c r="N58" s="5" t="s">
@@ -3143,12 +3147,12 @@
         <v>110</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>59</v>
       </c>
       <c r="B59" s="11">
-        <f>SUM(C59:E59)</f>
+        <f t="shared" si="8"/>
         <v>4.5254500000000002</v>
       </c>
       <c r="C59" s="5">
@@ -3162,7 +3166,7 @@
       </c>
       <c r="F59" s="5"/>
       <c r="G59" s="14">
-        <f>SUM(H59:J59)</f>
+        <f t="shared" si="9"/>
         <v>0.41471239999999998</v>
       </c>
       <c r="H59" s="5">
@@ -3175,12 +3179,12 @@
         <v>1.24E-5</v>
       </c>
       <c r="K59" s="5">
-        <f>SUM(C59:J59)</f>
+        <f t="shared" si="10"/>
         <v>5.3548748000000002</v>
       </c>
       <c r="L59" s="5"/>
       <c r="M59" s="9">
-        <f>K59/B59</f>
+        <f t="shared" si="11"/>
         <v>1.18328007159509</v>
       </c>
       <c r="N59" s="5" t="s">
@@ -3193,12 +3197,12 @@
         <v>110</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>67</v>
       </c>
       <c r="B60" s="11">
-        <f>SUM(C60:E60)</f>
+        <f t="shared" si="8"/>
         <v>7.0681399999999997E-5</v>
       </c>
       <c r="C60" s="7">
@@ -3212,7 +3216,7 @@
       </c>
       <c r="F60" s="7"/>
       <c r="G60" s="14">
-        <f>SUM(H60:J60)</f>
+        <f t="shared" si="9"/>
         <v>5.4510181999999996E-5</v>
       </c>
       <c r="H60" s="5">
@@ -3226,12 +3230,12 @@
         <v>1.8199999999999999E-10</v>
       </c>
       <c r="K60" s="5">
-        <f>SUM(C60:J60)</f>
+        <f t="shared" si="10"/>
         <v>1.7970176399999998E-4</v>
       </c>
       <c r="L60" s="5"/>
       <c r="M60" s="10">
-        <f>K60/B60</f>
+        <f t="shared" si="11"/>
         <v>2.5424194201020351</v>
       </c>
       <c r="N60" s="5" t="s">
@@ -3241,12 +3245,12 @@
         <v>115</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>73</v>
       </c>
       <c r="B61" s="11">
-        <f>SUM(C61:E61)</f>
+        <f t="shared" si="8"/>
         <v>8.7781100000000004E-3</v>
       </c>
       <c r="C61" s="5">
@@ -3260,7 +3264,7 @@
       </c>
       <c r="F61" s="5"/>
       <c r="G61" s="14">
-        <f>SUM(H61:J61)</f>
+        <f t="shared" si="9"/>
         <v>3.9770749700000004E-4</v>
       </c>
       <c r="H61" s="5">
@@ -3276,12 +3280,12 @@
         <v>7.7299999999999997E-8</v>
       </c>
       <c r="K61" s="5">
-        <f>SUM(C61:J61)</f>
+        <f t="shared" si="10"/>
         <v>9.573524994000002E-3</v>
       </c>
       <c r="L61" s="5"/>
       <c r="M61" s="9">
-        <f>K61/B61</f>
+        <f t="shared" si="11"/>
         <v>1.0906134685029012</v>
       </c>
       <c r="N61" s="5" t="s">
@@ -3294,12 +3298,12 @@
         <v>117</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>62</v>
       </c>
       <c r="B62" s="11">
-        <f>SUM(C62:E62)</f>
+        <f t="shared" si="8"/>
         <v>1.974315</v>
       </c>
       <c r="C62" s="5">
@@ -3313,7 +3317,7 @@
       </c>
       <c r="F62" s="5"/>
       <c r="G62" s="14">
-        <f>SUM(H62:J62)</f>
+        <f t="shared" si="9"/>
         <v>2.5557371700000001E-2</v>
       </c>
       <c r="H62" s="5">
@@ -3329,12 +3333,12 @@
         <v>3.36E-6</v>
       </c>
       <c r="K62" s="5">
-        <f>SUM(C62:J62)</f>
+        <f t="shared" si="10"/>
         <v>2.0254297434000001</v>
       </c>
       <c r="L62" s="5"/>
       <c r="M62" s="9">
-        <f>K62/B62</f>
+        <f t="shared" si="11"/>
         <v>1.0258898622560231</v>
       </c>
       <c r="N62" s="5" t="s">
@@ -3353,21 +3357,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E63"/>
   <sheetViews>
     <sheetView topLeftCell="A14" zoomScale="101" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="3" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -3384,7 +3388,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -3392,7 +3396,7 @@
       <c r="C2" s="2"/>
       <c r="D2" s="4"/>
     </row>
-    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -3402,7 +3406,7 @@
       <c r="C3" s="2"/>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -3416,7 +3420,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -3430,7 +3434,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -3444,7 +3448,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -3455,7 +3459,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -3463,7 +3467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -3471,7 +3475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -3485,7 +3489,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -3500,7 +3504,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -3515,7 +3519,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -3524,7 +3528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -3535,7 +3539,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -3546,7 +3550,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -3557,7 +3561,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -3571,7 +3575,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -3582,7 +3586,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -3593,7 +3597,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -3604,7 +3608,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -3612,7 +3616,7 @@
         <v>2.66E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>67</v>
       </c>
@@ -3624,7 +3628,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -3635,7 +3639,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -3646,7 +3650,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>44</v>
       </c>
@@ -3657,7 +3661,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>45</v>
       </c>
@@ -3665,7 +3669,7 @@
         <v>1.03</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>46</v>
       </c>
@@ -3673,7 +3677,7 @@
         <v>1.5299999999999999E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>47</v>
       </c>
@@ -3681,7 +3685,7 @@
         <v>1.03E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>48</v>
       </c>
@@ -3689,12 +3693,12 @@
         <v>1.9699999999999999E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>50</v>
       </c>
@@ -3702,7 +3706,7 @@
         <v>1.7000000000000001E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>51</v>
       </c>
@@ -3710,7 +3714,7 @@
         <v>0.58499999999999996</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>52</v>
       </c>
@@ -3718,7 +3722,7 @@
         <v>0.58599999999999997</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>53</v>
       </c>
@@ -3726,7 +3730,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>54</v>
       </c>
@@ -3734,7 +3738,7 @@
         <v>0.81399999999999995</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>61</v>
       </c>
@@ -3742,7 +3746,7 @@
         <v>2.3300000000000001E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>64</v>
       </c>
@@ -3753,7 +3757,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>63</v>
       </c>
@@ -3761,7 +3765,7 @@
         <v>4.57E-4</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>68</v>
       </c>
@@ -3770,7 +3774,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>69</v>
       </c>
@@ -3778,7 +3782,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>70</v>
       </c>
@@ -3786,7 +3790,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>78</v>
       </c>
@@ -3795,7 +3799,7 @@
         <v>4.54</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>79</v>
       </c>
@@ -3804,7 +3808,7 @@
         <v>4.54</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>80</v>
       </c>
@@ -3812,7 +3816,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>81</v>
       </c>
@@ -3820,7 +3824,7 @@
         <v>2.7799999999999999E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>82</v>
       </c>
@@ -3828,7 +3832,7 @@
         <v>4.8700000000000002E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>85</v>
       </c>
@@ -3836,7 +3840,7 @@
         <v>3.0299999999999999E-4</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>86</v>
       </c>
@@ -3844,7 +3848,7 @@
         <v>1.2199999999999999E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>108</v>
       </c>
@@ -3852,7 +3856,7 @@
         <v>2.4199999999999999E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>88</v>
       </c>
@@ -3860,7 +3864,7 @@
         <v>1.0300000000000001E-6</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>89</v>
       </c>
@@ -3868,7 +3872,7 @@
         <v>2.2499999999999999E-4</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>98</v>
       </c>
@@ -3876,7 +3880,7 @@
         <v>3.2499999999999997E-5</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>90</v>
       </c>
@@ -3884,7 +3888,7 @@
         <v>6.2E-4</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>91</v>
       </c>
@@ -3892,7 +3896,7 @@
         <v>1.7699999999999999E-4</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>92</v>
       </c>
@@ -3900,7 +3904,7 @@
         <v>4.88E-5</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>87</v>
       </c>
@@ -3908,7 +3912,7 @@
         <v>5.71E-4</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>93</v>
       </c>
@@ -3916,7 +3920,7 @@
         <v>1.7899999999999999E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>99</v>
       </c>
@@ -3924,7 +3928,7 @@
         <v>5.5799999999999999E-6</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>100</v>
       </c>
@@ -3932,7 +3936,7 @@
         <v>9.7100000000000002E-5</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="16" t="s">
         <v>102</v>
       </c>
@@ -3940,7 +3944,7 @@
         <v>1.65</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>106</v>
       </c>
@@ -3948,7 +3952,7 @@
         <v>2.5500000000000002E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>107</v>
       </c>
@@ -3956,7 +3960,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>105</v>
       </c>
@@ -3968,4 +3972,30 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated with ecoinvent 3.5
iron scrap and coal
</commit_message>
<xml_diff>
--- a/data/shared/upstream.xlsx
+++ b/data/shared/upstream.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/shared/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\BlackBlox\data\shared\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C6F6A3-C2DE-0C40-826E-362A07ED0B7D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535"/>
   </bookViews>
   <sheets>
     <sheet name="emissions" sheetId="3" r:id="rId1"/>
@@ -18,7 +17,7 @@
     <sheet name="emissions3.5" sheetId="4" r:id="rId3"/>
     <sheet name="removals3.5" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="127">
   <si>
     <t>meta-notes</t>
   </si>
@@ -409,12 +408,18 @@
   </si>
   <si>
     <t>electricity 1000g/kWh</t>
+  </si>
+  <si>
+    <t>steel scrap</t>
+  </si>
+  <si>
+    <t>"unalloyed"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
@@ -809,19 +814,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P68"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.5" customWidth="1"/>
+    <col min="1" max="1" width="44.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -871,7 +876,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -889,7 +894,7 @@
       <c r="M2" s="5"/>
       <c r="N2" s="4"/>
     </row>
-    <row r="3" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -925,7 +930,7 @@
       <c r="M3" s="5"/>
       <c r="N3" s="4"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>102</v>
       </c>
@@ -964,7 +969,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>26</v>
       </c>
@@ -990,7 +995,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -1022,7 +1027,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>53</v>
       </c>
@@ -1072,7 +1077,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>69</v>
       </c>
@@ -1104,7 +1109,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>70</v>
       </c>
@@ -1136,7 +1141,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>68</v>
       </c>
@@ -1186,7 +1191,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -1221,7 +1226,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -1268,7 +1273,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -1318,50 +1323,50 @@
         <v>114</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
       <c r="B14" s="11">
         <f t="shared" si="2"/>
-        <v>2.6330450000000001</v>
+        <v>2.8078600000000002</v>
       </c>
       <c r="C14" s="5">
         <f>C15+C34</f>
-        <v>2.5930999999999997</v>
+        <v>2.7669999999999999</v>
       </c>
       <c r="D14" s="5">
         <f>D15+D34</f>
-        <v>3.798E-2</v>
+        <v>3.8730000000000001E-2</v>
       </c>
       <c r="E14" s="5">
         <f>E15+E34</f>
-        <v>1.9650000000000002E-3</v>
+        <v>2.1299999999999999E-3</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="14">
         <f t="shared" si="3"/>
-        <v>0.7706965400000001</v>
+        <v>0.54085810000000012</v>
       </c>
       <c r="H14" s="5">
         <f>H15+H34</f>
-        <v>0.76800000000000002</v>
+        <v>0.53800000000000003</v>
       </c>
       <c r="I14" s="5">
         <f>I15+I34</f>
-        <v>2.6464399999999999E-3</v>
+        <v>2.8080000000000002E-3</v>
       </c>
       <c r="J14" s="5">
         <v>5.0099999999999998E-5</v>
       </c>
       <c r="K14" s="5">
         <f t="shared" si="1"/>
-        <v>4.1744380800000007</v>
+        <v>3.8895762000000005</v>
       </c>
       <c r="L14" s="5"/>
       <c r="M14" s="9">
         <f t="shared" si="0"/>
-        <v>1.5854032422537407</v>
+        <v>1.3852457743619697</v>
       </c>
       <c r="N14" s="5" t="s">
         <v>28</v>
@@ -1373,7 +1378,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>66</v>
       </c>
@@ -1420,7 +1425,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -1467,7 +1472,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -1495,7 +1500,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -1533,7 +1538,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -1561,7 +1566,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>81</v>
       </c>
@@ -1603,7 +1608,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>80</v>
       </c>
@@ -1645,7 +1650,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>119</v>
       </c>
@@ -1665,7 +1670,7 @@
       <c r="M22" s="5"/>
       <c r="N22" s="5"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>120</v>
       </c>
@@ -1686,7 +1691,7 @@
       <c r="M23" s="5"/>
       <c r="N23" s="5"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>122</v>
       </c>
@@ -1707,7 +1712,7 @@
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>121</v>
       </c>
@@ -1727,7 +1732,7 @@
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>123</v>
       </c>
@@ -1748,7 +1753,7 @@
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>124</v>
       </c>
@@ -1769,7 +1774,7 @@
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1814,7 +1819,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>2</v>
       </c>
@@ -1865,7 +1870,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>79</v>
       </c>
@@ -1892,7 +1897,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>78</v>
       </c>
@@ -1925,7 +1930,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>3</v>
       </c>
@@ -1976,7 +1981,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -2023,45 +2028,45 @@
         <v>111</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>32</v>
       </c>
       <c r="B34" s="11">
         <f t="shared" si="5"/>
-        <v>2.6605E-2</v>
-      </c>
-      <c r="C34" s="5">
-        <v>2.3099999999999999E-2</v>
-      </c>
-      <c r="D34" s="5">
-        <v>3.3800000000000002E-3</v>
-      </c>
-      <c r="E34" s="5">
-        <v>1.25E-4</v>
+        <v>0.20142000000000002</v>
+      </c>
+      <c r="C34">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="D34">
+        <v>4.13E-3</v>
+      </c>
+      <c r="E34">
+        <v>2.9E-4</v>
       </c>
       <c r="F34" s="5"/>
       <c r="G34" s="14">
         <f>SUM(H34:J34)</f>
-        <v>0.41700838999999995</v>
-      </c>
-      <c r="H34" s="5">
-        <v>0.41699999999999998</v>
-      </c>
-      <c r="I34" s="5">
-        <v>6.4400000000000002E-6</v>
-      </c>
-      <c r="J34" s="5">
-        <v>1.95E-6</v>
+        <v>0.18717021</v>
+      </c>
+      <c r="H34">
+        <v>0.187</v>
+      </c>
+      <c r="I34">
+        <v>1.6800000000000002E-4</v>
+      </c>
+      <c r="J34">
+        <v>2.21E-6</v>
       </c>
       <c r="K34" s="5">
         <f>SUM(C34:J34)</f>
-        <v>0.86062178</v>
+        <v>0.57576042000000005</v>
       </c>
       <c r="L34" s="5"/>
       <c r="M34" s="10">
         <f t="shared" si="4"/>
-        <v>32.348121781619994</v>
+        <v>2.8585067024128685</v>
       </c>
       <c r="N34" s="5" t="s">
         <v>28</v>
@@ -2070,7 +2075,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>5</v>
       </c>
@@ -2103,7 +2108,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>38</v>
       </c>
@@ -2143,7 +2148,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>51</v>
       </c>
@@ -2191,7 +2196,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>52</v>
       </c>
@@ -2239,7 +2244,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>89</v>
       </c>
@@ -2278,7 +2283,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>87</v>
       </c>
@@ -2317,7 +2322,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>103</v>
       </c>
@@ -2356,7 +2361,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>104</v>
       </c>
@@ -2386,7 +2391,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>92</v>
       </c>
@@ -2425,7 +2430,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>86</v>
       </c>
@@ -2464,7 +2469,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>99</v>
       </c>
@@ -2506,7 +2511,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>100</v>
       </c>
@@ -2548,7 +2553,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>91</v>
       </c>
@@ -2587,7 +2592,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>97</v>
       </c>
@@ -2626,7 +2631,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>98</v>
       </c>
@@ -2665,7 +2670,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>90</v>
       </c>
@@ -2704,7 +2709,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>88</v>
       </c>
@@ -2743,7 +2748,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>85</v>
       </c>
@@ -2782,12 +2787,12 @@
         <v>118</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>107</v>
       </c>
       <c r="B53" s="11">
-        <f t="shared" ref="B53:B68" si="8">SUM(C53:E53)</f>
+        <f t="shared" ref="B53:B69" si="8">SUM(C53:E53)</f>
         <v>3.51464</v>
       </c>
       <c r="C53" s="5">
@@ -2801,7 +2806,7 @@
       </c>
       <c r="F53" s="5"/>
       <c r="G53" s="14">
-        <f t="shared" ref="G53:G68" si="9">SUM(H53:J53)</f>
+        <f t="shared" ref="G53:G69" si="9">SUM(H53:J53)</f>
         <v>0.36993814999999997</v>
       </c>
       <c r="H53" s="5">
@@ -2821,7 +2826,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>82</v>
       </c>
@@ -2862,7 +2867,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>105</v>
       </c>
@@ -2897,12 +2902,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>106</v>
+        <v>126</v>
       </c>
       <c r="B56" s="11">
-        <f t="shared" si="8"/>
+        <f>SUM(C56:E56)</f>
         <v>5.4908799999999994E-2</v>
       </c>
       <c r="C56" s="5">
@@ -2916,7 +2921,7 @@
       </c>
       <c r="F56" s="14"/>
       <c r="G56" s="14">
-        <f t="shared" si="9"/>
+        <f>SUM(H56:J56)</f>
         <v>5.7666219999999999E-3</v>
       </c>
       <c r="H56" s="5">
@@ -2938,583 +2943,623 @@
         <v>116</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>61</v>
+        <v>106</v>
       </c>
       <c r="B57" s="11">
-        <f t="shared" si="8"/>
-        <v>1.5100289</v>
+        <f>SUM(C57:E57)</f>
+        <v>0</v>
       </c>
       <c r="C57" s="5">
-        <v>1.51</v>
-      </c>
-      <c r="D57" s="5"/>
+        <v>0</v>
+      </c>
+      <c r="D57" s="5">
+        <v>0</v>
+      </c>
       <c r="E57" s="5">
-        <v>2.8900000000000001E-5</v>
-      </c>
-      <c r="F57" s="5"/>
+        <v>0</v>
+      </c>
       <c r="G57" s="14">
-        <f t="shared" si="9"/>
-        <v>0.115</v>
+        <f>SUM(H57:J57)</f>
+        <v>0</v>
       </c>
       <c r="H57" s="5">
-        <v>0.115</v>
-      </c>
-      <c r="I57" s="5"/>
-      <c r="J57" s="5"/>
-      <c r="K57" s="5">
-        <f t="shared" ref="K57:K68" si="10">SUM(C57:J57)</f>
-        <v>1.7400289</v>
-      </c>
-      <c r="L57" s="5"/>
-      <c r="M57" s="9">
-        <f t="shared" ref="M57:M68" si="11">K57/B57</f>
-        <v>1.1523149656274791</v>
-      </c>
-      <c r="N57" s="5"/>
-      <c r="P57" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="I57" s="5">
+        <v>0</v>
+      </c>
+      <c r="J57" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>48</v>
+        <v>125</v>
       </c>
       <c r="B58" s="11">
         <f t="shared" si="8"/>
-        <v>2.1913999999999998</v>
-      </c>
-      <c r="C58" s="5">
-        <v>2.17</v>
-      </c>
-      <c r="D58" s="5">
-        <v>2.1399999999999999E-2</v>
-      </c>
-      <c r="E58" s="5"/>
+        <v>0.1167089</v>
+      </c>
+      <c r="C58">
+        <v>0.114</v>
+      </c>
+      <c r="D58">
+        <v>2.6800000000000001E-3</v>
+      </c>
+      <c r="E58">
+        <v>2.8899999999999998E-5</v>
+      </c>
       <c r="F58" s="5"/>
       <c r="G58" s="14">
         <f t="shared" si="9"/>
-        <v>1.37E-4</v>
-      </c>
-      <c r="H58" s="5"/>
-      <c r="I58" s="5">
-        <v>1.37E-4</v>
-      </c>
-      <c r="J58" s="5"/>
+        <v>7.4442399999999995E-3</v>
+      </c>
+      <c r="H58">
+        <v>7.2300000000000003E-3</v>
+      </c>
+      <c r="I58">
+        <v>2.13E-4</v>
+      </c>
+      <c r="J58">
+        <v>1.24E-6</v>
+      </c>
       <c r="K58" s="5">
-        <f t="shared" si="10"/>
-        <v>2.1916739999999999</v>
+        <f t="shared" ref="K58:K69" si="10">SUM(C58:J58)</f>
+        <v>0.13159738000000001</v>
       </c>
       <c r="L58" s="5"/>
       <c r="M58" s="9">
-        <f t="shared" si="11"/>
-        <v>1.0001250342246966</v>
-      </c>
-      <c r="N58" s="5"/>
+        <f t="shared" ref="M58:M69" si="11">K58/B58</f>
+        <v>1.1275693627478283</v>
+      </c>
+      <c r="N58" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="P58" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B59" s="11">
         <f t="shared" si="8"/>
-        <v>1.952</v>
+        <v>2.1913999999999998</v>
       </c>
       <c r="C59" s="5">
-        <v>1.94</v>
+        <v>2.17</v>
       </c>
       <c r="D59" s="5">
-        <v>1.2E-2</v>
+        <v>2.1399999999999999E-2</v>
       </c>
       <c r="E59" s="5"/>
       <c r="F59" s="5"/>
       <c r="G59" s="14">
         <f t="shared" si="9"/>
-        <v>1.0900000000000001E-4</v>
+        <v>1.37E-4</v>
       </c>
       <c r="H59" s="5"/>
       <c r="I59" s="5">
-        <v>1.0900000000000001E-4</v>
+        <v>1.37E-4</v>
       </c>
       <c r="J59" s="5"/>
       <c r="K59" s="5">
         <f t="shared" si="10"/>
-        <v>1.9522179999999998</v>
+        <v>2.1916739999999999</v>
       </c>
       <c r="L59" s="5"/>
       <c r="M59" s="9">
         <f t="shared" si="11"/>
-        <v>1.0001116803278687</v>
+        <v>1.0001250342246966</v>
       </c>
       <c r="N59" s="5"/>
       <c r="P59" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B60" s="11">
         <f t="shared" si="8"/>
-        <v>2.0971000000000002</v>
+        <v>1.952</v>
       </c>
       <c r="C60" s="5">
-        <v>2.08</v>
+        <v>1.94</v>
       </c>
       <c r="D60" s="5">
-        <v>1.7100000000000001E-2</v>
+        <v>1.2E-2</v>
       </c>
       <c r="E60" s="5"/>
       <c r="F60" s="5"/>
       <c r="G60" s="14">
         <f t="shared" si="9"/>
-        <v>1.2400000000000001E-4</v>
+        <v>1.0900000000000001E-4</v>
       </c>
       <c r="H60" s="5"/>
       <c r="I60" s="5">
-        <v>1.2400000000000001E-4</v>
+        <v>1.0900000000000001E-4</v>
       </c>
       <c r="J60" s="5"/>
       <c r="K60" s="5">
         <f t="shared" si="10"/>
-        <v>2.0973480000000002</v>
+        <v>1.9522179999999998</v>
       </c>
       <c r="L60" s="5"/>
       <c r="M60" s="9">
         <f t="shared" si="11"/>
-        <v>1.0001182585475181</v>
+        <v>1.0001116803278687</v>
       </c>
       <c r="N60" s="5"/>
       <c r="P60" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B61" s="11">
         <f t="shared" si="8"/>
-        <v>2.05918</v>
+        <v>2.0971000000000002</v>
       </c>
       <c r="C61" s="5">
-        <v>2.0499999999999998</v>
+        <v>2.08</v>
       </c>
       <c r="D61" s="5">
-        <v>9.1800000000000007E-3</v>
+        <v>1.7100000000000001E-2</v>
       </c>
       <c r="E61" s="5"/>
       <c r="F61" s="5"/>
       <c r="G61" s="14">
         <f t="shared" si="9"/>
-        <v>0.18401619999999999</v>
-      </c>
-      <c r="H61" s="5">
-        <v>0.184</v>
-      </c>
+        <v>1.2400000000000001E-4</v>
+      </c>
+      <c r="H61" s="5"/>
       <c r="I61" s="5">
-        <v>1.3699999999999999E-5</v>
-      </c>
-      <c r="J61" s="5">
-        <v>2.5000000000000002E-6</v>
-      </c>
+        <v>1.2400000000000001E-4</v>
+      </c>
+      <c r="J61" s="5"/>
       <c r="K61" s="5">
         <f t="shared" si="10"/>
-        <v>2.4272123999999997</v>
+        <v>2.0973480000000002</v>
       </c>
       <c r="L61" s="5"/>
       <c r="M61" s="9">
         <f t="shared" si="11"/>
-        <v>1.1787276488699383</v>
+        <v>1.0001182585475181</v>
       </c>
       <c r="N61" s="5"/>
       <c r="P61" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="B62" s="11">
         <f t="shared" si="8"/>
-        <v>4.8364000000000002E-3</v>
+        <v>2.05918</v>
       </c>
       <c r="C62" s="5">
-        <v>4.7499999999999999E-3</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="D62" s="5">
-        <v>8.6399999999999999E-5</v>
+        <v>9.1800000000000007E-3</v>
       </c>
       <c r="E62" s="5"/>
       <c r="F62" s="5"/>
       <c r="G62" s="14">
         <f t="shared" si="9"/>
-        <v>1.4165299999999999E-4</v>
+        <v>0.18401619999999999</v>
       </c>
       <c r="H62" s="5">
-        <v>1.3899999999999999E-4</v>
+        <v>0.184</v>
       </c>
       <c r="I62" s="5">
-        <v>2.6000000000000001E-6</v>
-      </c>
-      <c r="J62" s="7">
-        <v>5.2999999999999998E-8</v>
+        <v>1.3699999999999999E-5</v>
+      </c>
+      <c r="J62" s="5">
+        <v>2.5000000000000002E-6</v>
       </c>
       <c r="K62" s="5">
         <f t="shared" si="10"/>
-        <v>5.1197060000000008E-3</v>
+        <v>2.4272123999999997</v>
       </c>
       <c r="L62" s="5"/>
       <c r="M62" s="9">
         <f t="shared" si="11"/>
-        <v>1.0585778678355804</v>
-      </c>
-      <c r="N62" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="O62" t="s">
-        <v>34</v>
-      </c>
+        <v>1.1787276488699383</v>
+      </c>
+      <c r="N62" s="5"/>
       <c r="P62" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="B63" s="11">
         <f t="shared" si="8"/>
-        <v>5.3398300000000003E-3</v>
+        <v>4.8364000000000002E-3</v>
       </c>
       <c r="C63" s="5">
-        <v>5.2500000000000003E-3</v>
+        <v>4.7499999999999999E-3</v>
       </c>
       <c r="D63" s="5">
-        <v>8.6500000000000002E-5</v>
-      </c>
-      <c r="E63" s="5">
-        <v>3.3299999999999999E-6</v>
-      </c>
+        <v>8.6399999999999999E-5</v>
+      </c>
+      <c r="E63" s="5"/>
       <c r="F63" s="5"/>
       <c r="G63" s="14">
         <f t="shared" si="9"/>
-        <v>2.2085400000000001E-4</v>
+        <v>1.4165299999999999E-4</v>
       </c>
       <c r="H63" s="5">
-        <v>1.94E-4</v>
+        <v>1.3899999999999999E-4</v>
       </c>
       <c r="I63" s="5">
-        <v>2.6800000000000001E-5</v>
+        <v>2.6000000000000001E-6</v>
       </c>
       <c r="J63" s="7">
-        <v>5.4E-8</v>
+        <v>5.2999999999999998E-8</v>
       </c>
       <c r="K63" s="5">
         <f t="shared" si="10"/>
-        <v>5.7815380000000001E-3</v>
+        <v>5.1197060000000008E-3</v>
       </c>
       <c r="L63" s="5"/>
       <c r="M63" s="9">
         <f t="shared" si="11"/>
-        <v>1.0827194873245027</v>
+        <v>1.0585778678355804</v>
       </c>
       <c r="N63" s="5" t="s">
         <v>35</v>
       </c>
       <c r="O63" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="P63" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="B64" s="11">
         <f t="shared" si="8"/>
-        <v>6.2811700000000012E-2</v>
+        <v>5.3398300000000003E-3</v>
       </c>
       <c r="C64" s="5">
-        <f>(0.116+0.00782)/2</f>
-        <v>6.1910000000000007E-2</v>
+        <v>5.2500000000000003E-3</v>
       </c>
       <c r="D64" s="5">
-        <f>(0.000685+0.000984)/2</f>
-        <v>8.3449999999999996E-4</v>
+        <v>8.6500000000000002E-5</v>
       </c>
       <c r="E64" s="5">
-        <f>(0.0000114+0.000123)/2</f>
-        <v>6.7200000000000007E-5</v>
+        <v>3.3299999999999999E-6</v>
       </c>
       <c r="F64" s="5"/>
       <c r="G64" s="14">
         <f t="shared" si="9"/>
-        <v>3.2426277000000002E-5</v>
+        <v>2.2085400000000001E-4</v>
       </c>
       <c r="H64" s="5">
-        <f>(0.000000000244+0.00000000131)/2</f>
-        <v>7.7700000000000001E-10</v>
+        <v>1.94E-4</v>
       </c>
       <c r="I64" s="5">
-        <f>(0.00000585+0.000059)/2</f>
-        <v>3.2425000000000002E-5</v>
-      </c>
-      <c r="J64" s="5">
-        <v>5.0000000000000003E-10</v>
+        <v>2.6800000000000001E-5</v>
+      </c>
+      <c r="J64" s="7">
+        <v>5.4E-8</v>
       </c>
       <c r="K64" s="5">
         <f t="shared" si="10"/>
-        <v>6.2876552554000015E-2</v>
+        <v>5.7815380000000001E-3</v>
       </c>
       <c r="L64" s="5"/>
       <c r="M64" s="9">
         <f t="shared" si="11"/>
-        <v>1.0010324916217839</v>
+        <v>1.0827194873245027</v>
       </c>
       <c r="N64" s="5" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="O64" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="P64" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>59</v>
+        <v>17</v>
       </c>
       <c r="B65" s="11">
         <f t="shared" si="8"/>
-        <v>4.5254500000000002</v>
+        <v>6.2811700000000012E-2</v>
       </c>
       <c r="C65" s="5">
-        <v>4.4400000000000004</v>
+        <f>(0.116+0.00782)/2</f>
+        <v>6.1910000000000007E-2</v>
       </c>
       <c r="D65" s="5">
-        <v>8.1199999999999994E-2</v>
+        <f>(0.000685+0.000984)/2</f>
+        <v>8.3449999999999996E-4</v>
       </c>
       <c r="E65" s="5">
-        <v>4.2500000000000003E-3</v>
+        <f>(0.0000114+0.000123)/2</f>
+        <v>6.7200000000000007E-5</v>
       </c>
       <c r="F65" s="5"/>
       <c r="G65" s="14">
         <f t="shared" si="9"/>
-        <v>0.41471239999999998</v>
+        <v>3.2426277000000002E-5</v>
       </c>
       <c r="H65" s="5">
-        <v>0.41099999999999998</v>
+        <f>(0.000000000244+0.00000000131)/2</f>
+        <v>7.7700000000000001E-10</v>
       </c>
       <c r="I65" s="5">
-        <v>3.7000000000000002E-3</v>
+        <f>(0.00000585+0.000059)/2</f>
+        <v>3.2425000000000002E-5</v>
       </c>
       <c r="J65" s="5">
-        <v>1.24E-5</v>
+        <v>5.0000000000000003E-10</v>
       </c>
       <c r="K65" s="5">
         <f t="shared" si="10"/>
-        <v>5.3548748000000002</v>
+        <v>6.2876552554000015E-2</v>
       </c>
       <c r="L65" s="5"/>
       <c r="M65" s="9">
         <f t="shared" si="11"/>
-        <v>1.18328007159509</v>
+        <v>1.0010324916217839</v>
       </c>
       <c r="N65" s="5" t="s">
         <v>28</v>
       </c>
       <c r="O65" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="P65" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B66" s="11">
         <f t="shared" si="8"/>
-        <v>7.0681399999999997E-5</v>
-      </c>
-      <c r="C66" s="7">
-        <v>7.0599999999999995E-5</v>
+        <v>4.5254500000000002</v>
+      </c>
+      <c r="C66" s="5">
+        <v>4.4400000000000004</v>
       </c>
       <c r="D66" s="5">
-        <v>6.6100000000000003E-8</v>
-      </c>
-      <c r="E66" s="7">
-        <v>1.5300000000000001E-8</v>
-      </c>
-      <c r="F66" s="7"/>
+        <v>8.1199999999999994E-2</v>
+      </c>
+      <c r="E66" s="5">
+        <v>4.2500000000000003E-3</v>
+      </c>
+      <c r="F66" s="5"/>
       <c r="G66" s="14">
         <f t="shared" si="9"/>
+        <v>0.41471239999999998</v>
+      </c>
+      <c r="H66" s="5">
+        <v>0.41099999999999998</v>
+      </c>
+      <c r="I66" s="5">
+        <v>3.7000000000000002E-3</v>
+      </c>
+      <c r="J66" s="5">
+        <v>1.24E-5</v>
+      </c>
+      <c r="K66" s="5">
+        <f t="shared" si="10"/>
+        <v>5.3548748000000002</v>
+      </c>
+      <c r="L66" s="5"/>
+      <c r="M66" s="9">
+        <f t="shared" si="11"/>
+        <v>1.18328007159509</v>
+      </c>
+      <c r="N66" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O66" t="s">
+        <v>60</v>
+      </c>
+      <c r="P66" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>67</v>
+      </c>
+      <c r="B67" s="11">
+        <f t="shared" si="8"/>
+        <v>7.0681399999999997E-5</v>
+      </c>
+      <c r="C67" s="7">
+        <v>7.0599999999999995E-5</v>
+      </c>
+      <c r="D67" s="5">
+        <v>6.6100000000000003E-8</v>
+      </c>
+      <c r="E67" s="7">
+        <v>1.5300000000000001E-8</v>
+      </c>
+      <c r="F67" s="7"/>
+      <c r="G67" s="14">
+        <f t="shared" si="9"/>
         <v>5.4510181999999996E-5</v>
       </c>
-      <c r="H66" s="5">
+      <c r="H67" s="5">
         <v>5.4400000000000001E-5</v>
       </c>
-      <c r="I66" s="5">
+      <c r="I67" s="5">
         <f>0.00000011</f>
         <v>1.1000000000000001E-7</v>
       </c>
-      <c r="J66" s="7">
+      <c r="J67" s="7">
         <v>1.8199999999999999E-10</v>
       </c>
-      <c r="K66" s="5">
+      <c r="K67" s="5">
         <f t="shared" si="10"/>
         <v>1.7970176399999998E-4</v>
       </c>
-      <c r="L66" s="5"/>
-      <c r="M66" s="10">
+      <c r="L67" s="5"/>
+      <c r="M67" s="10">
         <f t="shared" si="11"/>
         <v>2.5424194201020351</v>
       </c>
-      <c r="N66" s="5" t="s">
+      <c r="N67" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="P66" t="s">
+      <c r="P67" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>73</v>
       </c>
-      <c r="B67" s="11">
+      <c r="B68" s="11">
         <f t="shared" si="8"/>
         <v>8.7781100000000004E-3</v>
       </c>
-      <c r="C67" s="5">
+      <c r="C68" s="5">
         <v>8.3999999999999995E-3</v>
       </c>
-      <c r="D67" s="5">
+      <c r="D68" s="5">
         <v>3.7199999999999999E-4</v>
       </c>
-      <c r="E67" s="5">
+      <c r="E68" s="5">
         <v>6.1099999999999999E-6</v>
-      </c>
-      <c r="F67" s="5"/>
-      <c r="G67" s="14">
-        <f t="shared" si="9"/>
-        <v>3.9770749700000004E-4</v>
-      </c>
-      <c r="H67" s="5">
-        <f>0.000000000197+0.000391</f>
-        <v>3.9100019700000004E-4</v>
-      </c>
-      <c r="I67" s="5">
-        <f>0.00000663</f>
-        <v>6.63E-6</v>
-      </c>
-      <c r="J67" s="5">
-        <f>0.0000000773</f>
-        <v>7.7299999999999997E-8</v>
-      </c>
-      <c r="K67" s="5">
-        <f t="shared" si="10"/>
-        <v>9.573524994000002E-3</v>
-      </c>
-      <c r="L67" s="5"/>
-      <c r="M67" s="9">
-        <f t="shared" si="11"/>
-        <v>1.0906134685029012</v>
-      </c>
-      <c r="N67" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="O67" t="s">
-        <v>65</v>
-      </c>
-      <c r="P67" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>62</v>
-      </c>
-      <c r="B68" s="11">
-        <f t="shared" si="8"/>
-        <v>1.974315</v>
-      </c>
-      <c r="C68" s="5">
-        <v>1.96</v>
-      </c>
-      <c r="D68" s="5">
-        <v>1.41E-2</v>
-      </c>
-      <c r="E68" s="5">
-        <v>2.1499999999999999E-4</v>
       </c>
       <c r="F68" s="5"/>
       <c r="G68" s="14">
         <f t="shared" si="9"/>
-        <v>2.5557371700000001E-2</v>
+        <v>3.9770749700000004E-4</v>
       </c>
       <c r="H68" s="5">
-        <f>0.0000000117+0.025</f>
-        <v>2.5000011700000001E-2</v>
+        <f>0.000000000197+0.000391</f>
+        <v>3.9100019700000004E-4</v>
       </c>
       <c r="I68" s="5">
-        <f>0.000554</f>
-        <v>5.5400000000000002E-4</v>
+        <f>0.00000663</f>
+        <v>6.63E-6</v>
       </c>
       <c r="J68" s="5">
-        <f>0.00000336</f>
-        <v>3.36E-6</v>
+        <f>0.0000000773</f>
+        <v>7.7299999999999997E-8</v>
       </c>
       <c r="K68" s="5">
         <f t="shared" si="10"/>
-        <v>2.0254297434000001</v>
+        <v>9.573524994000002E-3</v>
       </c>
       <c r="L68" s="5"/>
       <c r="M68" s="9">
         <f t="shared" si="11"/>
-        <v>1.0258898622560231</v>
+        <v>1.0906134685029012</v>
       </c>
       <c r="N68" s="5" t="s">
         <v>28</v>
       </c>
       <c r="O68" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="P68" t="s">
         <v>117</v>
       </c>
     </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>62</v>
+      </c>
+      <c r="B69" s="11">
+        <f t="shared" si="8"/>
+        <v>1.974315</v>
+      </c>
+      <c r="C69" s="5">
+        <v>1.96</v>
+      </c>
+      <c r="D69" s="5">
+        <v>1.41E-2</v>
+      </c>
+      <c r="E69" s="5">
+        <v>2.1499999999999999E-4</v>
+      </c>
+      <c r="F69" s="5"/>
+      <c r="G69" s="14">
+        <f t="shared" si="9"/>
+        <v>2.5557371700000001E-2</v>
+      </c>
+      <c r="H69" s="5">
+        <f>0.0000000117+0.025</f>
+        <v>2.5000011700000001E-2</v>
+      </c>
+      <c r="I69" s="5">
+        <f>0.000554</f>
+        <v>5.5400000000000002E-4</v>
+      </c>
+      <c r="J69" s="5">
+        <f>0.00000336</f>
+        <v>3.36E-6</v>
+      </c>
+      <c r="K69" s="5">
+        <f t="shared" si="10"/>
+        <v>2.0254297434000001</v>
+      </c>
+      <c r="L69" s="5"/>
+      <c r="M69" s="9">
+        <f t="shared" si="11"/>
+        <v>1.0258898622560231</v>
+      </c>
+      <c r="N69" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O69" t="s">
+        <v>56</v>
+      </c>
+      <c r="P69" t="s">
+        <v>117</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E63"/>
   <sheetViews>
     <sheetView zoomScale="101" workbookViewId="0">
       <selection activeCell="F71" sqref="F71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="3" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -3531,7 +3576,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -3539,7 +3584,7 @@
       <c r="C2" s="2"/>
       <c r="D2" s="4"/>
     </row>
-    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -3549,7 +3594,7 @@
       <c r="C3" s="2"/>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -3563,7 +3608,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -3577,7 +3622,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -3591,7 +3636,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -3602,7 +3647,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -3610,7 +3655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -3618,7 +3663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -3632,7 +3677,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -3647,7 +3692,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -3662,7 +3707,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -3671,7 +3716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -3682,7 +3727,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -3693,7 +3738,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -3704,7 +3749,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -3718,7 +3763,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -3729,7 +3774,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -3740,7 +3785,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -3751,7 +3796,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -3759,7 +3804,7 @@
         <v>2.66E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>67</v>
       </c>
@@ -3771,7 +3816,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -3782,7 +3827,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -3793,7 +3838,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>44</v>
       </c>
@@ -3804,7 +3849,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>45</v>
       </c>
@@ -3812,7 +3857,7 @@
         <v>1.03</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>46</v>
       </c>
@@ -3820,7 +3865,7 @@
         <v>1.5299999999999999E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>47</v>
       </c>
@@ -3828,7 +3873,7 @@
         <v>1.03E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>48</v>
       </c>
@@ -3836,12 +3881,12 @@
         <v>1.9699999999999999E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>50</v>
       </c>
@@ -3849,7 +3894,7 @@
         <v>1.7000000000000001E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>51</v>
       </c>
@@ -3857,7 +3902,7 @@
         <v>0.58499999999999996</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>52</v>
       </c>
@@ -3865,7 +3910,7 @@
         <v>0.58599999999999997</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>53</v>
       </c>
@@ -3873,7 +3918,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>54</v>
       </c>
@@ -3881,7 +3926,7 @@
         <v>0.81399999999999995</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>61</v>
       </c>
@@ -3889,7 +3934,7 @@
         <v>2.3300000000000001E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>64</v>
       </c>
@@ -3900,7 +3945,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>63</v>
       </c>
@@ -3908,7 +3953,7 @@
         <v>4.57E-4</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>68</v>
       </c>
@@ -3917,7 +3962,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>69</v>
       </c>
@@ -3925,7 +3970,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>70</v>
       </c>
@@ -3933,7 +3978,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>78</v>
       </c>
@@ -3942,7 +3987,7 @@
         <v>4.54</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>79</v>
       </c>
@@ -3951,7 +3996,7 @@
         <v>4.54</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>80</v>
       </c>
@@ -3959,7 +4004,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>81</v>
       </c>
@@ -3967,7 +4012,7 @@
         <v>2.7799999999999999E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>82</v>
       </c>
@@ -3975,7 +4020,7 @@
         <v>4.8700000000000002E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>85</v>
       </c>
@@ -3983,7 +4028,7 @@
         <v>3.0299999999999999E-4</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>86</v>
       </c>
@@ -3991,7 +4036,7 @@
         <v>1.2199999999999999E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>108</v>
       </c>
@@ -3999,7 +4044,7 @@
         <v>2.4199999999999999E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>88</v>
       </c>
@@ -4007,7 +4052,7 @@
         <v>1.0300000000000001E-6</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>89</v>
       </c>
@@ -4015,7 +4060,7 @@
         <v>2.2499999999999999E-4</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>98</v>
       </c>
@@ -4023,7 +4068,7 @@
         <v>3.2499999999999997E-5</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>90</v>
       </c>
@@ -4031,7 +4076,7 @@
         <v>6.2E-4</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>91</v>
       </c>
@@ -4039,7 +4084,7 @@
         <v>1.7699999999999999E-4</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>92</v>
       </c>
@@ -4047,7 +4092,7 @@
         <v>4.88E-5</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>87</v>
       </c>
@@ -4055,7 +4100,7 @@
         <v>5.71E-4</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>93</v>
       </c>
@@ -4063,7 +4108,7 @@
         <v>1.7899999999999999E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>99</v>
       </c>
@@ -4071,7 +4116,7 @@
         <v>5.5799999999999999E-6</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>100</v>
       </c>
@@ -4079,7 +4124,7 @@
         <v>9.7100000000000002E-5</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="16" t="s">
         <v>102</v>
       </c>
@@ -4087,7 +4132,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>106</v>
       </c>
@@ -4095,7 +4140,7 @@
         <v>2.5500000000000002E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>107</v>
       </c>
@@ -4103,7 +4148,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>105</v>
       </c>
@@ -4118,26 +4163,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
disconnected charcoal production from heat fuel. Works fine now.
</commit_message>
<xml_diff>
--- a/data/shared/upstream.xlsx
+++ b/data/shared/upstream.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\BlackBlox\data\shared\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/shared/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD4ABA31-F447-1647-8A97-769BD1B0F5F1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="emissions" sheetId="3" r:id="rId1"/>
@@ -17,7 +18,7 @@
     <sheet name="emissions3.5" sheetId="4" r:id="rId3"/>
     <sheet name="removals3.5" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="126">
   <si>
     <t>meta-notes</t>
   </si>
@@ -348,9 +349,6 @@
   </si>
   <si>
     <t>low alloy</t>
-  </si>
-  <si>
-    <t>no alloy</t>
   </si>
   <si>
     <t>chromium alloy</t>
@@ -419,7 +417,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
@@ -814,19 +812,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P69"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="44.42578125" customWidth="1"/>
+    <col min="1" max="1" width="44.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -873,10 +871,10 @@
         <v>29</v>
       </c>
       <c r="P1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -894,7 +892,7 @@
       <c r="M2" s="5"/>
       <c r="N2" s="4"/>
     </row>
-    <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -930,7 +928,7 @@
       <c r="M3" s="5"/>
       <c r="N3" s="4"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>101</v>
       </c>
@@ -966,10 +964,10 @@
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
       <c r="P4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>26</v>
       </c>
@@ -992,10 +990,10 @@
       <c r="M5" s="9"/>
       <c r="N5" s="5"/>
       <c r="P5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -1024,12 +1022,12 @@
       </c>
       <c r="N6" s="5"/>
       <c r="P6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B7" s="11">
         <f>SUM(C7:E7)</f>
@@ -1074,10 +1072,10 @@
         <v>55</v>
       </c>
       <c r="P7" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>68</v>
       </c>
@@ -1106,10 +1104,10 @@
       </c>
       <c r="N8" s="5"/>
       <c r="P8" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>69</v>
       </c>
@@ -1138,10 +1136,10 @@
       </c>
       <c r="N9" s="5"/>
       <c r="P9" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>67</v>
       </c>
@@ -1188,10 +1186,10 @@
         <v>54</v>
       </c>
       <c r="P10" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -1223,10 +1221,10 @@
       </c>
       <c r="N11" s="5"/>
       <c r="P11" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -1270,10 +1268,10 @@
         <v>28</v>
       </c>
       <c r="P12" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -1320,10 +1318,10 @@
         <v>42</v>
       </c>
       <c r="P13" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1375,10 +1373,10 @@
         <v>70</v>
       </c>
       <c r="P14" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>65</v>
       </c>
@@ -1422,10 +1420,10 @@
         <v>28</v>
       </c>
       <c r="P15" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -1469,10 +1467,10 @@
         <v>28</v>
       </c>
       <c r="P16" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -1497,10 +1495,10 @@
         <v>25</v>
       </c>
       <c r="P17" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -1535,10 +1533,10 @@
       <c r="M18" s="9"/>
       <c r="N18" s="5"/>
       <c r="P18" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -1563,10 +1561,10 @@
         <v>25</v>
       </c>
       <c r="P19" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>80</v>
       </c>
@@ -1605,10 +1603,10 @@
         <v>28</v>
       </c>
       <c r="P20" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>79</v>
       </c>
@@ -1647,12 +1645,12 @@
         <v>28</v>
       </c>
       <c r="P21" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B22" s="11">
         <v>0</v>
@@ -1670,9 +1668,9 @@
       <c r="M22" s="5"/>
       <c r="N22" s="5"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B23" s="11">
         <f>200/3.6/1000</f>
@@ -1691,9 +1689,9 @@
       <c r="M23" s="5"/>
       <c r="N23" s="5"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B24" s="11">
         <f>400/3.6/1000</f>
@@ -1712,9 +1710,9 @@
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B25" s="11">
         <f>500/3.6/1000</f>
@@ -1732,9 +1730,9 @@
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B26" s="11">
         <f>800/3.6/1000</f>
@@ -1753,9 +1751,9 @@
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B27" s="11">
         <f>1000/3.6/1000</f>
@@ -1774,7 +1772,7 @@
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1816,10 +1814,10 @@
         <v>28</v>
       </c>
       <c r="P28" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>2</v>
       </c>
@@ -1867,10 +1865,10 @@
         <v>30</v>
       </c>
       <c r="P29" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>78</v>
       </c>
@@ -1894,10 +1892,10 @@
       <c r="M30" s="5"/>
       <c r="N30" s="5"/>
       <c r="P30" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>77</v>
       </c>
@@ -1927,108 +1925,122 @@
       </c>
       <c r="N31" s="5"/>
       <c r="P31" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>3</v>
       </c>
       <c r="B32" s="11">
         <f t="shared" ref="B32:B38" si="5">SUM(C32:E32)</f>
-        <v>0.241614</v>
+        <v>0.20142000000000002</v>
       </c>
       <c r="C32" s="5">
-        <f>0.238</f>
-        <v>0.23799999999999999</v>
+        <f>C34</f>
+        <v>0.19700000000000001</v>
       </c>
       <c r="D32" s="5">
-        <v>3.3800000000000002E-3</v>
+        <f t="shared" ref="D32:E32" si="6">D34</f>
+        <v>4.13E-3</v>
       </c>
       <c r="E32" s="5">
-        <v>2.34E-4</v>
+        <f t="shared" si="6"/>
+        <v>2.9E-4</v>
       </c>
       <c r="F32" s="5"/>
       <c r="G32" s="14">
         <f>SUM(H32:J32)</f>
-        <v>0.31007200000000001</v>
+        <v>0.18717021</v>
       </c>
       <c r="H32" s="5">
-        <v>0.31</v>
+        <f t="shared" ref="H32:J32" si="7">H34</f>
+        <v>0.187</v>
       </c>
       <c r="I32" s="5">
-        <v>6.2600000000000004E-5</v>
+        <f t="shared" si="7"/>
+        <v>1.6800000000000002E-4</v>
       </c>
       <c r="J32" s="5">
-        <v>9.3999999999999998E-6</v>
+        <f t="shared" si="7"/>
+        <v>2.21E-6</v>
       </c>
       <c r="K32" s="5">
         <f>SUM(C32:J32)</f>
-        <v>0.86175800000000002</v>
+        <v>0.57576042000000005</v>
       </c>
       <c r="L32" s="5"/>
       <c r="M32" s="10">
         <f t="shared" si="4"/>
-        <v>3.5666724610328875</v>
+        <v>2.8585067024128685</v>
       </c>
       <c r="N32" s="5" t="s">
         <v>23</v>
       </c>
       <c r="O32" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="P32" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>4</v>
       </c>
       <c r="B33" s="11">
         <f t="shared" si="5"/>
-        <v>0.24137999999999998</v>
+        <v>0.20142000000000002</v>
       </c>
       <c r="C33" s="5">
-        <f>0.238</f>
-        <v>0.23799999999999999</v>
+        <f>C34</f>
+        <v>0.19700000000000001</v>
       </c>
       <c r="D33" s="5">
-        <v>3.3800000000000002E-3</v>
-      </c>
-      <c r="E33" s="5"/>
+        <f t="shared" ref="D33:E33" si="8">D34</f>
+        <v>4.13E-3</v>
+      </c>
+      <c r="E33" s="5">
+        <f t="shared" si="8"/>
+        <v>2.9E-4</v>
+      </c>
       <c r="F33" s="5"/>
       <c r="G33" s="14">
         <f>SUM(H33:J33)</f>
-        <v>0.31006260000000002</v>
+        <v>0.18717021</v>
       </c>
       <c r="H33" s="5">
-        <v>0.31</v>
+        <f t="shared" ref="H33:J33" si="9">H34</f>
+        <v>0.187</v>
       </c>
       <c r="I33" s="5">
-        <v>6.2600000000000004E-5</v>
-      </c>
-      <c r="J33" s="5"/>
+        <f t="shared" si="9"/>
+        <v>1.6800000000000002E-4</v>
+      </c>
+      <c r="J33" s="5">
+        <f t="shared" si="9"/>
+        <v>2.21E-6</v>
+      </c>
       <c r="K33" s="5">
         <f>SUM(C33:J33)</f>
-        <v>0.86150519999999997</v>
+        <v>0.57576042000000005</v>
       </c>
       <c r="L33" s="5"/>
       <c r="M33" s="10">
         <f t="shared" si="4"/>
-        <v>3.569082774049217</v>
+        <v>2.8585067024128685</v>
       </c>
       <c r="N33" s="5" t="s">
         <v>23</v>
       </c>
       <c r="O33" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="P33" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -2069,13 +2081,13 @@
         <v>2.8585067024128685</v>
       </c>
       <c r="N34" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="P34" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>5</v>
       </c>
@@ -2105,10 +2117,10 @@
         <v>28</v>
       </c>
       <c r="P35" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>38</v>
       </c>
@@ -2145,10 +2157,10 @@
         <v>83</v>
       </c>
       <c r="P36" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>51</v>
       </c>
@@ -2193,10 +2205,10 @@
         <v>56</v>
       </c>
       <c r="P37" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>52</v>
       </c>
@@ -2241,10 +2253,10 @@
         <v>56</v>
       </c>
       <c r="P38" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>88</v>
       </c>
@@ -2259,7 +2271,7 @@
         <v>1.0499999999999999E-5</v>
       </c>
       <c r="F39" s="11">
-        <f t="shared" ref="F39:F52" si="6">SUM(C39:E39)</f>
+        <f t="shared" ref="F39:F52" si="10">SUM(C39:E39)</f>
         <v>1.9099500000000002E-2</v>
       </c>
       <c r="G39" s="14"/>
@@ -2280,10 +2292,10 @@
       <c r="M39" s="5"/>
       <c r="N39" s="5"/>
       <c r="P39" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>86</v>
       </c>
@@ -2298,7 +2310,7 @@
         <v>7.5800000000000003E-6</v>
       </c>
       <c r="F40" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>1.4915580000000001E-2</v>
       </c>
       <c r="G40" s="14"/>
@@ -2319,10 +2331,10 @@
       <c r="M40" s="5"/>
       <c r="N40" s="5"/>
       <c r="P40" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>102</v>
       </c>
@@ -2337,7 +2349,7 @@
         <v>4.5800000000000002E-4</v>
       </c>
       <c r="F41" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0.53225800000000001</v>
       </c>
       <c r="G41" s="14"/>
@@ -2358,10 +2370,10 @@
       <c r="M41" s="5"/>
       <c r="N41" s="5"/>
       <c r="P41" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>103</v>
       </c>
@@ -2376,7 +2388,7 @@
         <v>2.0999999999999998E-6</v>
       </c>
       <c r="F42" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>5.0540999999999997E-3</v>
       </c>
       <c r="G42" s="17"/>
@@ -2388,10 +2400,10 @@
       <c r="M42" s="5"/>
       <c r="N42" s="5"/>
       <c r="P42" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>91</v>
       </c>
@@ -2406,7 +2418,7 @@
         <v>2.3E-6</v>
       </c>
       <c r="F43" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>5.0114000000000001E-3</v>
       </c>
       <c r="G43" s="14"/>
@@ -2421,16 +2433,16 @@
       </c>
       <c r="K43" s="5"/>
       <c r="L43" s="14">
-        <f t="shared" ref="L43:L52" si="7">SUM(H43:J43)</f>
+        <f t="shared" ref="L43:L52" si="11">SUM(H43:J43)</f>
         <v>5.8874445999999988E-4</v>
       </c>
       <c r="M43" s="5"/>
       <c r="N43" s="5"/>
       <c r="P43" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>85</v>
       </c>
@@ -2445,7 +2457,7 @@
         <v>1.7399999999999999E-5</v>
       </c>
       <c r="F44" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>3.3737400000000001E-2</v>
       </c>
       <c r="G44" s="14"/>
@@ -2460,16 +2472,16 @@
       </c>
       <c r="K44" s="5"/>
       <c r="L44" s="14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>1.8145939999999999E-3</v>
       </c>
       <c r="M44" s="5"/>
       <c r="N44" s="5"/>
       <c r="P44" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>98</v>
       </c>
@@ -2484,7 +2496,7 @@
         <v>1.2200000000000001E-7</v>
       </c>
       <c r="F45" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>1.29682E-4</v>
       </c>
       <c r="G45" s="14"/>
@@ -2499,7 +2511,7 @@
       </c>
       <c r="K45" s="5"/>
       <c r="L45" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>4.2616869999999996E-4</v>
       </c>
       <c r="M45" s="5"/>
@@ -2508,10 +2520,10 @@
         <v>100</v>
       </c>
       <c r="P45" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>99</v>
       </c>
@@ -2526,7 +2538,7 @@
         <v>1.8900000000000001E-7</v>
       </c>
       <c r="F46" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>2.2258900000000001E-4</v>
       </c>
       <c r="G46" s="14"/>
@@ -2541,7 +2553,7 @@
       </c>
       <c r="K46" s="5"/>
       <c r="L46" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>9.6601144999999995E-4</v>
       </c>
       <c r="M46" s="5"/>
@@ -2550,10 +2562,10 @@
         <v>100</v>
       </c>
       <c r="P46" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>90</v>
       </c>
@@ -2568,7 +2580,7 @@
         <v>6.9700000000000002E-6</v>
       </c>
       <c r="F47" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>1.2324969999999999E-2</v>
       </c>
       <c r="G47" s="14"/>
@@ -2583,16 +2595,16 @@
       </c>
       <c r="K47" s="5"/>
       <c r="L47" s="14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>8.7928850000000005E-4</v>
       </c>
       <c r="M47" s="5"/>
       <c r="N47" s="5"/>
       <c r="P47" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>96</v>
       </c>
@@ -2607,7 +2619,7 @@
         <v>4.8099999999999997E-5</v>
       </c>
       <c r="F48" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>2.5078099999999999E-2</v>
       </c>
       <c r="G48" s="14"/>
@@ -2622,16 +2634,16 @@
       </c>
       <c r="K48" s="5"/>
       <c r="L48" s="14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5.3051600000000008E-4</v>
       </c>
       <c r="M48" s="5"/>
       <c r="N48" s="5"/>
       <c r="P48" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>97</v>
       </c>
@@ -2646,7 +2658,7 @@
         <v>2.1100000000000001E-6</v>
       </c>
       <c r="F49" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>1.0214100000000002E-3</v>
       </c>
       <c r="G49" s="14"/>
@@ -2661,16 +2673,16 @@
       </c>
       <c r="K49" s="5"/>
       <c r="L49" s="14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>1.1458618999999999E-4</v>
       </c>
       <c r="M49" s="5"/>
       <c r="N49" s="5"/>
       <c r="P49" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>89</v>
       </c>
@@ -2685,7 +2697,7 @@
         <v>2.4899999999999999E-5</v>
       </c>
       <c r="F50" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>2.17819E-2</v>
       </c>
       <c r="G50" s="14"/>
@@ -2700,16 +2712,16 @@
       </c>
       <c r="K50" s="5"/>
       <c r="L50" s="14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>3.3639717000000001E-3</v>
       </c>
       <c r="M50" s="5"/>
       <c r="N50" s="5"/>
       <c r="P50" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>87</v>
       </c>
@@ -2724,7 +2736,7 @@
         <v>5.1200000000000002E-8</v>
       </c>
       <c r="F51" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>7.8016200000000007E-5</v>
       </c>
       <c r="G51" s="14"/>
@@ -2739,16 +2751,16 @@
       </c>
       <c r="K51" s="5"/>
       <c r="L51" s="14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>6.6999509999999995E-6</v>
       </c>
       <c r="M51" s="5"/>
       <c r="N51" s="5"/>
       <c r="P51" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>84</v>
       </c>
@@ -2763,7 +2775,7 @@
         <v>1.13E-5</v>
       </c>
       <c r="F52" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>1.1072300000000002E-2</v>
       </c>
       <c r="G52" s="14"/>
@@ -2778,21 +2790,21 @@
       </c>
       <c r="K52" s="7"/>
       <c r="L52" s="14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>1.0599427000000002E-3</v>
       </c>
       <c r="M52" s="5"/>
       <c r="N52" s="5"/>
       <c r="P52" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B53" s="11">
-        <f t="shared" ref="B53:B69" si="8">SUM(C53:E53)</f>
+        <f t="shared" ref="B53:B68" si="12">SUM(C53:E53)</f>
         <v>3.51464</v>
       </c>
       <c r="C53" s="5">
@@ -2806,7 +2818,7 @@
       </c>
       <c r="F53" s="5"/>
       <c r="G53" s="14">
-        <f t="shared" ref="G53:G69" si="9">SUM(H53:J53)</f>
+        <f t="shared" ref="G53:G68" si="13">SUM(H53:J53)</f>
         <v>0.36993814999999997</v>
       </c>
       <c r="H53" s="5">
@@ -2823,15 +2835,15 @@
       <c r="M53" s="5"/>
       <c r="N53" s="5"/>
       <c r="P53" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>81</v>
       </c>
       <c r="B54" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0.12100999999999999</v>
       </c>
       <c r="C54" s="5">
@@ -2845,7 +2857,7 @@
       </c>
       <c r="F54" s="5"/>
       <c r="G54" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>9.3692799999999989E-3</v>
       </c>
       <c r="H54" s="5">
@@ -2864,15 +2876,15 @@
         <v>28</v>
       </c>
       <c r="P54" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>104</v>
       </c>
       <c r="B55" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0.51764999999999994</v>
       </c>
       <c r="C55" s="5">
@@ -2886,7 +2898,7 @@
       </c>
       <c r="F55" s="5"/>
       <c r="G55" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>5.4393850000000001E-2</v>
       </c>
       <c r="H55" s="5">
@@ -2899,12 +2911,12 @@
         <v>1.8500000000000001E-6</v>
       </c>
       <c r="P55" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B56" s="11">
         <f>SUM(C56:E56)</f>
@@ -2940,602 +2952,571 @@
       <c r="M56" s="5"/>
       <c r="N56" s="5"/>
       <c r="P56" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="B57" s="11">
-        <f>SUM(C57:E57)</f>
-        <v>0</v>
-      </c>
-      <c r="C57" s="5">
-        <v>0</v>
-      </c>
-      <c r="D57" s="5">
-        <v>0</v>
-      </c>
-      <c r="E57" s="5">
-        <v>0</v>
-      </c>
+        <f t="shared" si="12"/>
+        <v>0.1167089</v>
+      </c>
+      <c r="C57">
+        <v>0.114</v>
+      </c>
+      <c r="D57">
+        <v>2.6800000000000001E-3</v>
+      </c>
+      <c r="E57">
+        <v>2.8899999999999998E-5</v>
+      </c>
+      <c r="F57" s="5"/>
       <c r="G57" s="14">
-        <f>SUM(H57:J57)</f>
-        <v>0</v>
-      </c>
-      <c r="H57" s="5">
-        <v>0</v>
-      </c>
-      <c r="I57" s="5">
-        <v>0</v>
-      </c>
-      <c r="J57" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="13"/>
+        <v>7.4442399999999995E-3</v>
+      </c>
+      <c r="H57">
+        <v>7.2300000000000003E-3</v>
+      </c>
+      <c r="I57">
+        <v>2.13E-4</v>
+      </c>
+      <c r="J57">
+        <v>1.24E-6</v>
+      </c>
+      <c r="K57" s="5">
+        <f t="shared" ref="K57:K68" si="14">SUM(C57:J57)</f>
+        <v>0.13159738000000001</v>
+      </c>
+      <c r="L57" s="5"/>
+      <c r="M57" s="9">
+        <f t="shared" ref="M57:M68" si="15">K57/B57</f>
+        <v>1.1275693627478283</v>
+      </c>
+      <c r="N57" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="P57" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>124</v>
+        <v>48</v>
       </c>
       <c r="B58" s="11">
-        <f t="shared" si="8"/>
-        <v>0.1167089</v>
-      </c>
-      <c r="C58">
-        <v>0.114</v>
-      </c>
-      <c r="D58">
-        <v>2.6800000000000001E-3</v>
-      </c>
-      <c r="E58">
-        <v>2.8899999999999998E-5</v>
-      </c>
+        <f t="shared" si="12"/>
+        <v>2.1913999999999998</v>
+      </c>
+      <c r="C58" s="5">
+        <v>2.17</v>
+      </c>
+      <c r="D58" s="5">
+        <v>2.1399999999999999E-2</v>
+      </c>
+      <c r="E58" s="5"/>
       <c r="F58" s="5"/>
       <c r="G58" s="14">
-        <f t="shared" si="9"/>
-        <v>7.4442399999999995E-3</v>
-      </c>
-      <c r="H58">
-        <v>7.2300000000000003E-3</v>
-      </c>
-      <c r="I58">
-        <v>2.13E-4</v>
-      </c>
-      <c r="J58">
-        <v>1.24E-6</v>
-      </c>
+        <f t="shared" si="13"/>
+        <v>1.37E-4</v>
+      </c>
+      <c r="H58" s="5"/>
+      <c r="I58" s="5">
+        <v>1.37E-4</v>
+      </c>
+      <c r="J58" s="5"/>
       <c r="K58" s="5">
-        <f t="shared" ref="K58:K69" si="10">SUM(C58:J58)</f>
-        <v>0.13159738000000001</v>
+        <f t="shared" si="14"/>
+        <v>2.1916739999999999</v>
       </c>
       <c r="L58" s="5"/>
       <c r="M58" s="9">
-        <f t="shared" ref="M58:M69" si="11">K58/B58</f>
-        <v>1.1275693627478283</v>
-      </c>
-      <c r="N58" s="5" t="s">
-        <v>23</v>
-      </c>
+        <f t="shared" si="15"/>
+        <v>1.0001250342246966</v>
+      </c>
+      <c r="N58" s="5"/>
       <c r="P58" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B59" s="11">
-        <f t="shared" si="8"/>
-        <v>2.1913999999999998</v>
+        <f t="shared" si="12"/>
+        <v>1.952</v>
       </c>
       <c r="C59" s="5">
-        <v>2.17</v>
+        <v>1.94</v>
       </c>
       <c r="D59" s="5">
-        <v>2.1399999999999999E-2</v>
+        <v>1.2E-2</v>
       </c>
       <c r="E59" s="5"/>
       <c r="F59" s="5"/>
       <c r="G59" s="14">
-        <f t="shared" si="9"/>
-        <v>1.37E-4</v>
+        <f t="shared" si="13"/>
+        <v>1.0900000000000001E-4</v>
       </c>
       <c r="H59" s="5"/>
       <c r="I59" s="5">
-        <v>1.37E-4</v>
+        <v>1.0900000000000001E-4</v>
       </c>
       <c r="J59" s="5"/>
       <c r="K59" s="5">
-        <f t="shared" si="10"/>
-        <v>2.1916739999999999</v>
+        <f t="shared" si="14"/>
+        <v>1.9522179999999998</v>
       </c>
       <c r="L59" s="5"/>
       <c r="M59" s="9">
-        <f t="shared" si="11"/>
-        <v>1.0001250342246966</v>
+        <f t="shared" si="15"/>
+        <v>1.0001116803278687</v>
       </c>
       <c r="N59" s="5"/>
       <c r="P59" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B60" s="11">
-        <f t="shared" si="8"/>
-        <v>1.952</v>
+        <f t="shared" si="12"/>
+        <v>2.0971000000000002</v>
       </c>
       <c r="C60" s="5">
-        <v>1.94</v>
+        <v>2.08</v>
       </c>
       <c r="D60" s="5">
-        <v>1.2E-2</v>
+        <v>1.7100000000000001E-2</v>
       </c>
       <c r="E60" s="5"/>
       <c r="F60" s="5"/>
       <c r="G60" s="14">
-        <f t="shared" si="9"/>
-        <v>1.0900000000000001E-4</v>
+        <f t="shared" si="13"/>
+        <v>1.2400000000000001E-4</v>
       </c>
       <c r="H60" s="5"/>
       <c r="I60" s="5">
-        <v>1.0900000000000001E-4</v>
+        <v>1.2400000000000001E-4</v>
       </c>
       <c r="J60" s="5"/>
       <c r="K60" s="5">
-        <f t="shared" si="10"/>
-        <v>1.9522179999999998</v>
+        <f t="shared" si="14"/>
+        <v>2.0973480000000002</v>
       </c>
       <c r="L60" s="5"/>
       <c r="M60" s="9">
-        <f t="shared" si="11"/>
-        <v>1.0001116803278687</v>
+        <f t="shared" si="15"/>
+        <v>1.0001182585475181</v>
       </c>
       <c r="N60" s="5"/>
       <c r="P60" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B61" s="11">
-        <f t="shared" si="8"/>
-        <v>2.0971000000000002</v>
+        <f t="shared" si="12"/>
+        <v>2.05918</v>
       </c>
       <c r="C61" s="5">
-        <v>2.08</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="D61" s="5">
-        <v>1.7100000000000001E-2</v>
+        <v>9.1800000000000007E-3</v>
       </c>
       <c r="E61" s="5"/>
       <c r="F61" s="5"/>
       <c r="G61" s="14">
-        <f t="shared" si="9"/>
-        <v>1.2400000000000001E-4</v>
-      </c>
-      <c r="H61" s="5"/>
+        <f t="shared" si="13"/>
+        <v>0.18401619999999999</v>
+      </c>
+      <c r="H61" s="5">
+        <v>0.184</v>
+      </c>
       <c r="I61" s="5">
-        <v>1.2400000000000001E-4</v>
-      </c>
-      <c r="J61" s="5"/>
+        <v>1.3699999999999999E-5</v>
+      </c>
+      <c r="J61" s="5">
+        <v>2.5000000000000002E-6</v>
+      </c>
       <c r="K61" s="5">
-        <f t="shared" si="10"/>
-        <v>2.0973480000000002</v>
+        <f t="shared" si="14"/>
+        <v>2.4272123999999997</v>
       </c>
       <c r="L61" s="5"/>
       <c r="M61" s="9">
-        <f t="shared" si="11"/>
-        <v>1.0001182585475181</v>
+        <f t="shared" si="15"/>
+        <v>1.1787276488699383</v>
       </c>
       <c r="N61" s="5"/>
       <c r="P61" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="B62" s="11">
-        <f t="shared" si="8"/>
-        <v>2.05918</v>
+        <f t="shared" si="12"/>
+        <v>4.8364000000000002E-3</v>
       </c>
       <c r="C62" s="5">
-        <v>2.0499999999999998</v>
+        <v>4.7499999999999999E-3</v>
       </c>
       <c r="D62" s="5">
-        <v>9.1800000000000007E-3</v>
+        <v>8.6399999999999999E-5</v>
       </c>
       <c r="E62" s="5"/>
       <c r="F62" s="5"/>
       <c r="G62" s="14">
-        <f t="shared" si="9"/>
-        <v>0.18401619999999999</v>
+        <f t="shared" si="13"/>
+        <v>1.4165299999999999E-4</v>
       </c>
       <c r="H62" s="5">
-        <v>0.184</v>
+        <v>1.3899999999999999E-4</v>
       </c>
       <c r="I62" s="5">
-        <v>1.3699999999999999E-5</v>
-      </c>
-      <c r="J62" s="5">
-        <v>2.5000000000000002E-6</v>
+        <v>2.6000000000000001E-6</v>
+      </c>
+      <c r="J62" s="7">
+        <v>5.2999999999999998E-8</v>
       </c>
       <c r="K62" s="5">
-        <f t="shared" si="10"/>
-        <v>2.4272123999999997</v>
+        <f t="shared" si="14"/>
+        <v>5.1197060000000008E-3</v>
       </c>
       <c r="L62" s="5"/>
       <c r="M62" s="9">
-        <f t="shared" si="11"/>
-        <v>1.1787276488699383</v>
-      </c>
-      <c r="N62" s="5"/>
+        <f t="shared" si="15"/>
+        <v>1.0585778678355804</v>
+      </c>
+      <c r="N62" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O62" t="s">
+        <v>34</v>
+      </c>
       <c r="P62" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="B63" s="11">
-        <f t="shared" si="8"/>
-        <v>4.8364000000000002E-3</v>
+        <f t="shared" si="12"/>
+        <v>5.3398300000000003E-3</v>
       </c>
       <c r="C63" s="5">
-        <v>4.7499999999999999E-3</v>
+        <v>5.2500000000000003E-3</v>
       </c>
       <c r="D63" s="5">
-        <v>8.6399999999999999E-5</v>
-      </c>
-      <c r="E63" s="5"/>
+        <v>8.6500000000000002E-5</v>
+      </c>
+      <c r="E63" s="5">
+        <v>3.3299999999999999E-6</v>
+      </c>
       <c r="F63" s="5"/>
       <c r="G63" s="14">
-        <f t="shared" si="9"/>
-        <v>1.4165299999999999E-4</v>
+        <f t="shared" si="13"/>
+        <v>2.2085400000000001E-4</v>
       </c>
       <c r="H63" s="5">
-        <v>1.3899999999999999E-4</v>
+        <v>1.94E-4</v>
       </c>
       <c r="I63" s="5">
-        <v>2.6000000000000001E-6</v>
+        <v>2.6800000000000001E-5</v>
       </c>
       <c r="J63" s="7">
-        <v>5.2999999999999998E-8</v>
+        <v>5.4E-8</v>
       </c>
       <c r="K63" s="5">
-        <f t="shared" si="10"/>
-        <v>5.1197060000000008E-3</v>
+        <f t="shared" si="14"/>
+        <v>5.7815380000000001E-3</v>
       </c>
       <c r="L63" s="5"/>
       <c r="M63" s="9">
-        <f t="shared" si="11"/>
-        <v>1.0585778678355804</v>
+        <f t="shared" si="15"/>
+        <v>1.0827194873245027</v>
       </c>
       <c r="N63" s="5" t="s">
         <v>35</v>
       </c>
       <c r="O63" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="P63" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="B64" s="11">
-        <f t="shared" si="8"/>
-        <v>5.3398300000000003E-3</v>
+        <f t="shared" si="12"/>
+        <v>6.2811700000000012E-2</v>
       </c>
       <c r="C64" s="5">
-        <v>5.2500000000000003E-3</v>
+        <f>(0.116+0.00782)/2</f>
+        <v>6.1910000000000007E-2</v>
       </c>
       <c r="D64" s="5">
-        <v>8.6500000000000002E-5</v>
+        <f>(0.000685+0.000984)/2</f>
+        <v>8.3449999999999996E-4</v>
       </c>
       <c r="E64" s="5">
-        <v>3.3299999999999999E-6</v>
+        <f>(0.0000114+0.000123)/2</f>
+        <v>6.7200000000000007E-5</v>
       </c>
       <c r="F64" s="5"/>
       <c r="G64" s="14">
-        <f t="shared" si="9"/>
-        <v>2.2085400000000001E-4</v>
+        <f t="shared" si="13"/>
+        <v>3.2426277000000002E-5</v>
       </c>
       <c r="H64" s="5">
-        <v>1.94E-4</v>
+        <f>(0.000000000244+0.00000000131)/2</f>
+        <v>7.7700000000000001E-10</v>
       </c>
       <c r="I64" s="5">
-        <v>2.6800000000000001E-5</v>
-      </c>
-      <c r="J64" s="7">
-        <v>5.4E-8</v>
+        <f>(0.00000585+0.000059)/2</f>
+        <v>3.2425000000000002E-5</v>
+      </c>
+      <c r="J64" s="5">
+        <v>5.0000000000000003E-10</v>
       </c>
       <c r="K64" s="5">
-        <f t="shared" si="10"/>
-        <v>5.7815380000000001E-3</v>
+        <f t="shared" si="14"/>
+        <v>6.2876552554000015E-2</v>
       </c>
       <c r="L64" s="5"/>
       <c r="M64" s="9">
-        <f t="shared" si="11"/>
-        <v>1.0827194873245027</v>
+        <f t="shared" si="15"/>
+        <v>1.0010324916217839</v>
       </c>
       <c r="N64" s="5" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="O64" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="P64" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="B65" s="11">
-        <f t="shared" si="8"/>
-        <v>6.2811700000000012E-2</v>
+        <f t="shared" si="12"/>
+        <v>4.5254500000000002</v>
       </c>
       <c r="C65" s="5">
-        <f>(0.116+0.00782)/2</f>
-        <v>6.1910000000000007E-2</v>
+        <v>4.4400000000000004</v>
       </c>
       <c r="D65" s="5">
-        <f>(0.000685+0.000984)/2</f>
-        <v>8.3449999999999996E-4</v>
+        <v>8.1199999999999994E-2</v>
       </c>
       <c r="E65" s="5">
-        <f>(0.0000114+0.000123)/2</f>
-        <v>6.7200000000000007E-5</v>
+        <v>4.2500000000000003E-3</v>
       </c>
       <c r="F65" s="5"/>
       <c r="G65" s="14">
-        <f t="shared" si="9"/>
-        <v>3.2426277000000002E-5</v>
+        <f t="shared" si="13"/>
+        <v>0.41471239999999998</v>
       </c>
       <c r="H65" s="5">
-        <f>(0.000000000244+0.00000000131)/2</f>
-        <v>7.7700000000000001E-10</v>
+        <v>0.41099999999999998</v>
       </c>
       <c r="I65" s="5">
-        <f>(0.00000585+0.000059)/2</f>
-        <v>3.2425000000000002E-5</v>
+        <v>3.7000000000000002E-3</v>
       </c>
       <c r="J65" s="5">
-        <v>5.0000000000000003E-10</v>
+        <v>1.24E-5</v>
       </c>
       <c r="K65" s="5">
-        <f t="shared" si="10"/>
-        <v>6.2876552554000015E-2</v>
+        <f t="shared" si="14"/>
+        <v>5.3548748000000002</v>
       </c>
       <c r="L65" s="5"/>
       <c r="M65" s="9">
-        <f t="shared" si="11"/>
-        <v>1.0010324916217839</v>
+        <f t="shared" si="15"/>
+        <v>1.18328007159509</v>
       </c>
       <c r="N65" s="5" t="s">
         <v>28</v>
       </c>
       <c r="O65" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="P65" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="B66" s="11">
-        <f t="shared" si="8"/>
-        <v>4.5254500000000002</v>
-      </c>
-      <c r="C66" s="5">
-        <v>4.4400000000000004</v>
+        <f t="shared" si="12"/>
+        <v>7.0681399999999997E-5</v>
+      </c>
+      <c r="C66" s="7">
+        <v>7.0599999999999995E-5</v>
       </c>
       <c r="D66" s="5">
-        <v>8.1199999999999994E-2</v>
-      </c>
-      <c r="E66" s="5">
-        <v>4.2500000000000003E-3</v>
-      </c>
-      <c r="F66" s="5"/>
+        <v>6.6100000000000003E-8</v>
+      </c>
+      <c r="E66" s="7">
+        <v>1.5300000000000001E-8</v>
+      </c>
+      <c r="F66" s="7"/>
       <c r="G66" s="14">
-        <f t="shared" si="9"/>
-        <v>0.41471239999999998</v>
+        <f t="shared" si="13"/>
+        <v>5.4510181999999996E-5</v>
       </c>
       <c r="H66" s="5">
-        <v>0.41099999999999998</v>
+        <v>5.4400000000000001E-5</v>
       </c>
       <c r="I66" s="5">
-        <v>3.7000000000000002E-3</v>
-      </c>
-      <c r="J66" s="5">
-        <v>1.24E-5</v>
+        <f>0.00000011</f>
+        <v>1.1000000000000001E-7</v>
+      </c>
+      <c r="J66" s="7">
+        <v>1.8199999999999999E-10</v>
       </c>
       <c r="K66" s="5">
-        <f t="shared" si="10"/>
-        <v>5.3548748000000002</v>
+        <f t="shared" si="14"/>
+        <v>1.7970176399999998E-4</v>
       </c>
       <c r="L66" s="5"/>
-      <c r="M66" s="9">
-        <f t="shared" si="11"/>
-        <v>1.18328007159509</v>
+      <c r="M66" s="10">
+        <f t="shared" si="15"/>
+        <v>2.5424194201020351</v>
       </c>
       <c r="N66" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="O66" t="s">
-        <v>59</v>
-      </c>
       <c r="P66" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B67" s="11">
-        <f t="shared" si="8"/>
-        <v>7.0681399999999997E-5</v>
-      </c>
-      <c r="C67" s="7">
-        <v>7.0599999999999995E-5</v>
+        <f t="shared" si="12"/>
+        <v>8.7781100000000004E-3</v>
+      </c>
+      <c r="C67" s="5">
+        <v>8.3999999999999995E-3</v>
       </c>
       <c r="D67" s="5">
-        <v>6.6100000000000003E-8</v>
-      </c>
-      <c r="E67" s="7">
-        <v>1.5300000000000001E-8</v>
-      </c>
-      <c r="F67" s="7"/>
+        <v>3.7199999999999999E-4</v>
+      </c>
+      <c r="E67" s="5">
+        <v>6.1099999999999999E-6</v>
+      </c>
+      <c r="F67" s="5"/>
       <c r="G67" s="14">
-        <f t="shared" si="9"/>
-        <v>5.4510181999999996E-5</v>
+        <f t="shared" si="13"/>
+        <v>3.9770749700000004E-4</v>
       </c>
       <c r="H67" s="5">
-        <v>5.4400000000000001E-5</v>
+        <f>0.000000000197+0.000391</f>
+        <v>3.9100019700000004E-4</v>
       </c>
       <c r="I67" s="5">
-        <f>0.00000011</f>
-        <v>1.1000000000000001E-7</v>
-      </c>
-      <c r="J67" s="7">
-        <v>1.8199999999999999E-10</v>
+        <f>0.00000663</f>
+        <v>6.63E-6</v>
+      </c>
+      <c r="J67" s="5">
+        <f>0.0000000773</f>
+        <v>7.7299999999999997E-8</v>
       </c>
       <c r="K67" s="5">
-        <f t="shared" si="10"/>
-        <v>1.7970176399999998E-4</v>
+        <f t="shared" si="14"/>
+        <v>9.573524994000002E-3</v>
       </c>
       <c r="L67" s="5"/>
-      <c r="M67" s="10">
-        <f t="shared" si="11"/>
-        <v>2.5424194201020351</v>
+      <c r="M67" s="9">
+        <f t="shared" si="15"/>
+        <v>1.0906134685029012</v>
       </c>
       <c r="N67" s="5" t="s">
         <v>28</v>
       </c>
+      <c r="O67" t="s">
+        <v>64</v>
+      </c>
       <c r="P67" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="B68" s="11">
-        <f t="shared" si="8"/>
-        <v>8.7781100000000004E-3</v>
+        <f t="shared" si="12"/>
+        <v>1.974315</v>
       </c>
       <c r="C68" s="5">
-        <v>8.3999999999999995E-3</v>
+        <v>1.96</v>
       </c>
       <c r="D68" s="5">
-        <v>3.7199999999999999E-4</v>
+        <v>1.41E-2</v>
       </c>
       <c r="E68" s="5">
-        <v>6.1099999999999999E-6</v>
+        <v>2.1499999999999999E-4</v>
       </c>
       <c r="F68" s="5"/>
       <c r="G68" s="14">
-        <f t="shared" si="9"/>
-        <v>3.9770749700000004E-4</v>
+        <f t="shared" si="13"/>
+        <v>2.5557371700000001E-2</v>
       </c>
       <c r="H68" s="5">
-        <f>0.000000000197+0.000391</f>
-        <v>3.9100019700000004E-4</v>
+        <f>0.0000000117+0.025</f>
+        <v>2.5000011700000001E-2</v>
       </c>
       <c r="I68" s="5">
-        <f>0.00000663</f>
-        <v>6.63E-6</v>
+        <f>0.000554</f>
+        <v>5.5400000000000002E-4</v>
       </c>
       <c r="J68" s="5">
-        <f>0.0000000773</f>
-        <v>7.7299999999999997E-8</v>
+        <f>0.00000336</f>
+        <v>3.36E-6</v>
       </c>
       <c r="K68" s="5">
-        <f t="shared" si="10"/>
-        <v>9.573524994000002E-3</v>
+        <f t="shared" si="14"/>
+        <v>2.0254297434000001</v>
       </c>
       <c r="L68" s="5"/>
       <c r="M68" s="9">
-        <f t="shared" si="11"/>
-        <v>1.0906134685029012</v>
+        <f t="shared" si="15"/>
+        <v>1.0258898622560231</v>
       </c>
       <c r="N68" s="5" t="s">
         <v>28</v>
       </c>
       <c r="O68" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="P68" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>61</v>
-      </c>
-      <c r="B69" s="11">
-        <f t="shared" si="8"/>
-        <v>1.974315</v>
-      </c>
-      <c r="C69" s="5">
-        <v>1.96</v>
-      </c>
-      <c r="D69" s="5">
-        <v>1.41E-2</v>
-      </c>
-      <c r="E69" s="5">
-        <v>2.1499999999999999E-4</v>
-      </c>
-      <c r="F69" s="5"/>
-      <c r="G69" s="14">
-        <f t="shared" si="9"/>
-        <v>2.5557371700000001E-2</v>
-      </c>
-      <c r="H69" s="5">
-        <f>0.0000000117+0.025</f>
-        <v>2.5000011700000001E-2</v>
-      </c>
-      <c r="I69" s="5">
-        <f>0.000554</f>
-        <v>5.5400000000000002E-4</v>
-      </c>
-      <c r="J69" s="5">
-        <f>0.00000336</f>
-        <v>3.36E-6</v>
-      </c>
-      <c r="K69" s="5">
-        <f t="shared" si="10"/>
-        <v>2.0254297434000001</v>
-      </c>
-      <c r="L69" s="5"/>
-      <c r="M69" s="9">
-        <f t="shared" si="11"/>
-        <v>1.0258898622560231</v>
-      </c>
-      <c r="N69" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="O69" t="s">
-        <v>55</v>
-      </c>
-      <c r="P69" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -3545,21 +3526,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="101" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView topLeftCell="A10" zoomScale="101" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="3" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -3576,7 +3557,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -3584,7 +3565,7 @@
       <c r="C2" s="2"/>
       <c r="D2" s="4"/>
     </row>
-    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -3594,7 +3575,7 @@
       <c r="C3" s="2"/>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -3608,7 +3589,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -3622,7 +3603,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -3636,7 +3617,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -3647,7 +3628,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -3655,7 +3636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -3663,7 +3644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -3677,7 +3658,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -3692,7 +3673,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -3707,7 +3688,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -3716,7 +3697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -3727,7 +3708,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -3738,7 +3719,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -3749,7 +3730,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -3763,7 +3744,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -3774,7 +3755,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -3785,7 +3766,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -3796,7 +3777,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -3804,7 +3785,7 @@
         <v>2.66E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>66</v>
       </c>
@@ -3816,7 +3797,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -3827,7 +3808,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -3838,7 +3819,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>44</v>
       </c>
@@ -3849,7 +3830,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>45</v>
       </c>
@@ -3857,7 +3838,7 @@
         <v>1.03</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>46</v>
       </c>
@@ -3865,7 +3846,7 @@
         <v>1.5299999999999999E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>47</v>
       </c>
@@ -3873,7 +3854,7 @@
         <v>1.03E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>48</v>
       </c>
@@ -3881,12 +3862,12 @@
         <v>1.9699999999999999E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>50</v>
       </c>
@@ -3894,7 +3875,7 @@
         <v>1.7000000000000001E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>51</v>
       </c>
@@ -3902,7 +3883,7 @@
         <v>0.58499999999999996</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>52</v>
       </c>
@@ -3910,15 +3891,15 @@
         <v>0.58599999999999997</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B34">
         <v>1.81</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>53</v>
       </c>
@@ -3926,7 +3907,7 @@
         <v>0.81399999999999995</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>60</v>
       </c>
@@ -3934,7 +3915,7 @@
         <v>2.3300000000000001E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>63</v>
       </c>
@@ -3945,7 +3926,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>62</v>
       </c>
@@ -3953,7 +3934,7 @@
         <v>4.57E-4</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>67</v>
       </c>
@@ -3962,7 +3943,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>68</v>
       </c>
@@ -3970,7 +3951,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>69</v>
       </c>
@@ -3978,7 +3959,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>77</v>
       </c>
@@ -3987,7 +3968,7 @@
         <v>4.54</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>78</v>
       </c>
@@ -3996,7 +3977,7 @@
         <v>4.54</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>79</v>
       </c>
@@ -4004,7 +3985,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>80</v>
       </c>
@@ -4012,7 +3993,7 @@
         <v>2.7799999999999999E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>81</v>
       </c>
@@ -4020,7 +4001,7 @@
         <v>4.8700000000000002E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>84</v>
       </c>
@@ -4028,7 +4009,7 @@
         <v>3.0299999999999999E-4</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>85</v>
       </c>
@@ -4036,15 +4017,15 @@
         <v>1.2199999999999999E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C49">
         <v>2.4199999999999999E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>87</v>
       </c>
@@ -4052,7 +4033,7 @@
         <v>1.0300000000000001E-6</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>88</v>
       </c>
@@ -4060,7 +4041,7 @@
         <v>2.2499999999999999E-4</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>97</v>
       </c>
@@ -4068,7 +4049,7 @@
         <v>3.2499999999999997E-5</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>89</v>
       </c>
@@ -4076,7 +4057,7 @@
         <v>6.2E-4</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>90</v>
       </c>
@@ -4084,7 +4065,7 @@
         <v>1.7699999999999999E-4</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>91</v>
       </c>
@@ -4092,7 +4073,7 @@
         <v>4.88E-5</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>86</v>
       </c>
@@ -4100,7 +4081,7 @@
         <v>5.71E-4</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>92</v>
       </c>
@@ -4108,7 +4089,7 @@
         <v>1.7899999999999999E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>98</v>
       </c>
@@ -4116,7 +4097,7 @@
         <v>5.5799999999999999E-6</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>99</v>
       </c>
@@ -4124,7 +4105,7 @@
         <v>9.7100000000000002E-5</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="16" t="s">
         <v>101</v>
       </c>
@@ -4132,23 +4113,23 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>105</v>
+        <v>124</v>
       </c>
       <c r="B61">
         <v>2.5500000000000002E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B62">
         <v>0.16</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>104</v>
       </c>
@@ -4163,26 +4144,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>